<commit_message>
fix bug in `MCDA`, finish adding figures for #21
</commit_message>
<xml_diff>
--- a/dmsan/comparison/results/uncertainty_winners.xlsx
+++ b/dmsan/comparison/results/uncertainty_winners.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10500" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10500" uniqueCount="106">
   <si>
     <t>0.8784777661468466:0.006370503431624358:0.04859964178467366:0.028206730676399738:0.03834535796045566</t>
   </si>
@@ -332,1207 +332,7 @@
     <t>reB</t>
   </si>
   <si>
-    <t>0.8784777661468466:0.006370503431624358:0.04859964178467366:0.028206730676399738:0.03834535796045566:'0.8784777661468466:0.006370503431624358:0.04859964178467366:0.028206730676399738:0.03834535796045566'</t>
-  </si>
-  <si>
-    <t>0.5788884213912752:0.1148213613226778:0.07098608081635895:0.2342593506406826:0.0010447858290055308:'0.5788884213912752:0.1148213613226778:0.07098608081635895:0.2342593506406826:0.0010447858290055308'</t>
-  </si>
-  <si>
-    <t>0.1045832742016494:0.2739786511896807:0.04193551102332393:0.4496555852728088:0.1298469783125372:'0.1045832742016494:0.2739786511896807:0.04193551102332393:0.4496555852728088:0.1298469783125372'</t>
-  </si>
-  <si>
-    <t>0.46969157849230714:0.03744275801747336:0.16899734942148248:0.09394011306381288:0.22992820100492414:'0.46969157849230714:0.03744275801747336:0.16899734942148248:0.09394011306381288:0.22992820100492414'</t>
-  </si>
-  <si>
-    <t>0.3957114651979722:0.12655103364603323:0.21722155723607658:0.06003495743759002:0.20048098648232784:'0.3957114651979722:0.12655103364603323:0.21722155723607658:0.06003495743759002:0.20048098648232784'</t>
-  </si>
-  <si>
-    <t>0.6379849661155549:0.12237712616089151:0.07293784141940536:0.039180538245610075:0.12751952805853817:'0.6379849661155549:0.12237712616089151:0.07293784141940536:0.039180538245610075:0.12751952805853817'</t>
-  </si>
-  <si>
-    <t>0.6919501954151895:0.15649884726812238:0.08597952671094426:0.007373107703755164:0.05819832290198865:'0.6919501954151895:0.15649884726812238:0.08597952671094426:0.007373107703755164:0.05819832290198865'</t>
-  </si>
-  <si>
-    <t>0.341735955717008:0.26218025344058743:0.2391269771185358:0.11980515008466874:0.0371516636392:'0.341735955717008:0.26218025344058743:0.2391269771185358:0.11980515008466874:0.0371516636392'</t>
-  </si>
-  <si>
-    <t>0.5478035918166799:0.17297868951796821:0.0038734044236464053:0.15141123544969604:0.1239330787920094:'0.5478035918166799:0.17297868951796821:0.0038734044236464053:0.15141123544969604:0.1239330787920094'</t>
-  </si>
-  <si>
-    <t>0.24233858495952668:0.3071458935191035:0.13511293658740064:0.06436706646403009:0.25103551846993916:'0.24233858495952668:0.3071458935191035:0.13511293658740064:0.06436706646403009:0.25103551846993916'</t>
-  </si>
-  <si>
-    <t>0.9964069679491023:0.0008499840013651758:0.0010790274898496441:0.001230791211281703:0.00043322934840114803:'0.9964069679491023:0.0008499840013651758:0.0010790274898496441:0.001230791211281703:0.00043322934840114803'</t>
-  </si>
-  <si>
-    <t>0.2580814265398616:0.074537560053405:0.23377596013418603:0.21868577765632807:0.21491927561621915:'0.2580814265398616:0.074537560053405:0.23377596013418603:0.21868577765632807:0.21491927561621915'</t>
-  </si>
-  <si>
-    <t>0.17438907388885735:0.0038831449836855747:0.2570750647234156:0.34538605480971696:0.21926666159432445:'0.17438907388885735:0.0038831449836855747:0.2570750647234156:0.34538605480971696:0.21926666159432445'</t>
-  </si>
-  <si>
-    <t>0.7656895374345389:0.10000252830735035:0.05411212378682602:0.040184273334564105:0.040011537136720614:'0.7656895374345389:0.10000252830735035:0.05411212378682602:0.040184273334564105:0.040011537136720614'</t>
-  </si>
-  <si>
-    <t>0.7462431889969952:0.05009674706362561:0.08270077476439788:0.0405067293390163:0.08045255983596511:'0.7462431889969952:0.05009674706362561:0.08270077476439788:0.0405067293390163:0.08045255983596511'</t>
-  </si>
-  <si>
-    <t>0.8165026538916844:0.043478271812166396:0.04165595053028977:0.06006448699021291:0.038298636775646516:'0.8165026538916844:0.043478271812166396:0.04165595053028977:0.06006448699021291:0.038298636775646516'</t>
-  </si>
-  <si>
-    <t>0.048691367112449924:0.14037800101418405:0.3252409319849474:0.19884286680342372:0.2868468330849948:'0.048691367112449924:0.14037800101418405:0.3252409319849474:0.19884286680342372:0.2868468330849948'</t>
-  </si>
-  <si>
-    <t>0.41688949152990207:0.267275179454366:0.04723230298522335:0.24410864883377942:0.024494377196729145:'0.41688949152990207:0.267275179454366:0.04723230298522335:0.24410864883377942:0.024494377196729145'</t>
-  </si>
-  <si>
-    <t>0.9496819961510143:0.012580916913995415:0.013647930365035737:0.012313135409237473:0.011776021160717033:'0.9496819961510143:0.012580916913995415:0.013647930365035737:0.012313135409237473:0.011776021160717033'</t>
-  </si>
-  <si>
-    <t>0.07145714857544264:0.1797578576761459:0.08087059903348022:0.09418509128847868:0.5737293034264526:'0.07145714857544264:0.1797578576761459:0.08087059903348022:0.09418509128847868:0.5737293034264526'</t>
-  </si>
-  <si>
-    <t>0.03834535796045566:0.8784777661468466:0.006370503431624358:0.04859964178467366:0.028206730676399738:'0.03834535796045566:0.8784777661468466:0.006370503431624358:0.04859964178467366:0.028206730676399738'</t>
-  </si>
-  <si>
-    <t>0.0010447858290055308:0.5788884213912752:0.1148213613226778:0.07098608081635895:0.2342593506406826:'0.0010447858290055308:0.5788884213912752:0.1148213613226778:0.07098608081635895:0.2342593506406826'</t>
-  </si>
-  <si>
-    <t>0.1298469783125372:0.1045832742016494:0.2739786511896807:0.04193551102332393:0.4496555852728088:'0.1298469783125372:0.1045832742016494:0.2739786511896807:0.04193551102332393:0.4496555852728088'</t>
-  </si>
-  <si>
-    <t>0.22992820100492414:0.46969157849230714:0.03744275801747336:0.16899734942148248:0.09394011306381288:'0.22992820100492414:0.46969157849230714:0.03744275801747336:0.16899734942148248:0.09394011306381288'</t>
-  </si>
-  <si>
-    <t>0.20048098648232784:0.3957114651979722:0.12655103364603323:0.21722155723607658:0.06003495743759002:'0.20048098648232784:0.3957114651979722:0.12655103364603323:0.21722155723607658:0.06003495743759002'</t>
-  </si>
-  <si>
-    <t>0.12751952805853817:0.6379849661155549:0.12237712616089151:0.07293784141940536:0.039180538245610075:'0.12751952805853817:0.6379849661155549:0.12237712616089151:0.07293784141940536:0.039180538245610075'</t>
-  </si>
-  <si>
-    <t>0.05819832290198865:0.6919501954151895:0.15649884726812238:0.08597952671094426:0.007373107703755164:'0.05819832290198865:0.6919501954151895:0.15649884726812238:0.08597952671094426:0.007373107703755164'</t>
-  </si>
-  <si>
-    <t>0.0371516636392:0.341735955717008:0.26218025344058743:0.2391269771185358:0.11980515008466874:'0.0371516636392:0.341735955717008:0.26218025344058743:0.2391269771185358:0.11980515008466874'</t>
-  </si>
-  <si>
-    <t>0.1239330787920094:0.5478035918166799:0.17297868951796821:0.0038734044236464053:0.15141123544969604:'0.1239330787920094:0.5478035918166799:0.17297868951796821:0.0038734044236464053:0.15141123544969604'</t>
-  </si>
-  <si>
-    <t>0.25103551846993916:0.24233858495952668:0.3071458935191035:0.13511293658740064:0.06436706646403009:'0.25103551846993916:0.24233858495952668:0.3071458935191035:0.13511293658740064:0.06436706646403009'</t>
-  </si>
-  <si>
-    <t>0.00043322934840114803:0.9964069679491023:0.0008499840013651758:0.0010790274898496441:0.001230791211281703:'0.00043322934840114803:0.9964069679491023:0.0008499840013651758:0.0010790274898496441:0.001230791211281703'</t>
-  </si>
-  <si>
-    <t>0.21491927561621915:0.2580814265398616:0.074537560053405:0.23377596013418603:0.21868577765632807:'0.21491927561621915:0.2580814265398616:0.074537560053405:0.23377596013418603:0.21868577765632807'</t>
-  </si>
-  <si>
-    <t>0.21926666159432445:0.17438907388885735:0.0038831449836855747:0.2570750647234156:0.34538605480971696:'0.21926666159432445:0.17438907388885735:0.0038831449836855747:0.2570750647234156:0.34538605480971696'</t>
-  </si>
-  <si>
-    <t>0.040011537136720614:0.7656895374345389:0.10000252830735035:0.05411212378682602:0.040184273334564105:'0.040011537136720614:0.7656895374345389:0.10000252830735035:0.05411212378682602:0.040184273334564105'</t>
-  </si>
-  <si>
-    <t>0.08045255983596511:0.7462431889969952:0.05009674706362561:0.08270077476439788:0.0405067293390163:'0.08045255983596511:0.7462431889969952:0.05009674706362561:0.08270077476439788:0.0405067293390163'</t>
-  </si>
-  <si>
-    <t>0.038298636775646516:0.8165026538916844:0.043478271812166396:0.04165595053028977:0.06006448699021291:'0.038298636775646516:0.8165026538916844:0.043478271812166396:0.04165595053028977:0.06006448699021291'</t>
-  </si>
-  <si>
-    <t>0.2868468330849948:0.048691367112449924:0.14037800101418405:0.3252409319849474:0.19884286680342372:'0.2868468330849948:0.048691367112449924:0.14037800101418405:0.3252409319849474:0.19884286680342372'</t>
-  </si>
-  <si>
-    <t>0.024494377196729145:0.41688949152990207:0.267275179454366:0.04723230298522335:0.24410864883377942:'0.024494377196729145:0.41688949152990207:0.267275179454366:0.04723230298522335:0.24410864883377942'</t>
-  </si>
-  <si>
-    <t>0.011776021160717033:0.9496819961510143:0.012580916913995415:0.013647930365035737:0.012313135409237473:'0.011776021160717033:0.9496819961510143:0.012580916913995415:0.013647930365035737:0.012313135409237473'</t>
-  </si>
-  <si>
-    <t>0.5737293034264526:0.07145714857544264:0.1797578576761459:0.08087059903348022:0.09418509128847868:'0.5737293034264526:0.07145714857544264:0.1797578576761459:0.08087059903348022:0.09418509128847868'</t>
-  </si>
-  <si>
-    <t>0.028206730676399738:0.03834535796045566:0.8784777661468466:0.006370503431624358:0.04859964178467366:'0.028206730676399738:0.03834535796045566:0.8784777661468466:0.006370503431624358:0.04859964178467366'</t>
-  </si>
-  <si>
-    <t>0.2342593506406826:0.0010447858290055308:0.5788884213912752:0.1148213613226778:0.07098608081635895:'0.2342593506406826:0.0010447858290055308:0.5788884213912752:0.1148213613226778:0.07098608081635895'</t>
-  </si>
-  <si>
-    <t>0.4496555852728088:0.1298469783125372:0.1045832742016494:0.2739786511896807:0.04193551102332393:'0.4496555852728088:0.1298469783125372:0.1045832742016494:0.2739786511896807:0.04193551102332393'</t>
-  </si>
-  <si>
-    <t>0.09394011306381288:0.22992820100492414:0.46969157849230714:0.03744275801747336:0.16899734942148248:'0.09394011306381288:0.22992820100492414:0.46969157849230714:0.03744275801747336:0.16899734942148248'</t>
-  </si>
-  <si>
-    <t>0.06003495743759002:0.20048098648232784:0.3957114651979722:0.12655103364603323:0.21722155723607658:'0.06003495743759002:0.20048098648232784:0.3957114651979722:0.12655103364603323:0.21722155723607658'</t>
-  </si>
-  <si>
-    <t>0.039180538245610075:0.12751952805853817:0.6379849661155549:0.12237712616089151:0.07293784141940536:'0.039180538245610075:0.12751952805853817:0.6379849661155549:0.12237712616089151:0.07293784141940536'</t>
-  </si>
-  <si>
-    <t>0.007373107703755164:0.05819832290198865:0.6919501954151895:0.15649884726812238:0.08597952671094426:'0.007373107703755164:0.05819832290198865:0.6919501954151895:0.15649884726812238:0.08597952671094426'</t>
-  </si>
-  <si>
-    <t>0.11980515008466874:0.0371516636392:0.341735955717008:0.26218025344058743:0.2391269771185358:'0.11980515008466874:0.0371516636392:0.341735955717008:0.26218025344058743:0.2391269771185358'</t>
-  </si>
-  <si>
-    <t>0.15141123544969604:0.1239330787920094:0.5478035918166799:0.17297868951796821:0.0038734044236464053:'0.15141123544969604:0.1239330787920094:0.5478035918166799:0.17297868951796821:0.0038734044236464053'</t>
-  </si>
-  <si>
-    <t>0.06436706646403009:0.25103551846993916:0.24233858495952668:0.3071458935191035:0.13511293658740064:'0.06436706646403009:0.25103551846993916:0.24233858495952668:0.3071458935191035:0.13511293658740064'</t>
-  </si>
-  <si>
-    <t>0.001230791211281703:0.00043322934840114803:0.9964069679491023:0.0008499840013651758:0.0010790274898496441:'0.001230791211281703:0.00043322934840114803:0.9964069679491023:0.0008499840013651758:0.0010790274898496441'</t>
-  </si>
-  <si>
-    <t>0.21868577765632807:0.21491927561621915:0.2580814265398616:0.074537560053405:0.23377596013418603:'0.21868577765632807:0.21491927561621915:0.2580814265398616:0.074537560053405:0.23377596013418603'</t>
-  </si>
-  <si>
-    <t>0.34538605480971696:0.21926666159432445:0.17438907388885735:0.0038831449836855747:0.2570750647234156:'0.34538605480971696:0.21926666159432445:0.17438907388885735:0.0038831449836855747:0.2570750647234156'</t>
-  </si>
-  <si>
-    <t>0.040184273334564105:0.040011537136720614:0.7656895374345389:0.10000252830735035:0.05411212378682602:'0.040184273334564105:0.040011537136720614:0.7656895374345389:0.10000252830735035:0.05411212378682602'</t>
-  </si>
-  <si>
-    <t>0.0405067293390163:0.08045255983596511:0.7462431889969952:0.05009674706362561:0.08270077476439788:'0.0405067293390163:0.08045255983596511:0.7462431889969952:0.05009674706362561:0.08270077476439788'</t>
-  </si>
-  <si>
-    <t>0.06006448699021291:0.038298636775646516:0.8165026538916844:0.043478271812166396:0.04165595053028977:'0.06006448699021291:0.038298636775646516:0.8165026538916844:0.043478271812166396:0.04165595053028977'</t>
-  </si>
-  <si>
-    <t>0.19884286680342372:0.2868468330849948:0.048691367112449924:0.14037800101418405:0.3252409319849474:'0.19884286680342372:0.2868468330849948:0.048691367112449924:0.14037800101418405:0.3252409319849474'</t>
-  </si>
-  <si>
-    <t>0.24410864883377942:0.024494377196729145:0.41688949152990207:0.267275179454366:0.04723230298522335:'0.24410864883377942:0.024494377196729145:0.41688949152990207:0.267275179454366:0.04723230298522335'</t>
-  </si>
-  <si>
-    <t>0.012313135409237473:0.011776021160717033:0.9496819961510143:0.012580916913995415:0.013647930365035737:'0.012313135409237473:0.011776021160717033:0.9496819961510143:0.012580916913995415:0.013647930365035737'</t>
-  </si>
-  <si>
-    <t>0.09418509128847868:0.5737293034264526:0.07145714857544264:0.1797578576761459:0.08087059903348022:'0.09418509128847868:0.5737293034264526:0.07145714857544264:0.1797578576761459:0.08087059903348022'</t>
-  </si>
-  <si>
-    <t>0.04859964178467366:0.028206730676399738:0.03834535796045566:0.8784777661468466:0.006370503431624358:'0.04859964178467366:0.028206730676399738:0.03834535796045566:0.8784777661468466:0.006370503431624358'</t>
-  </si>
-  <si>
-    <t>0.07098608081635895:0.2342593506406826:0.0010447858290055308:0.5788884213912752:0.1148213613226778:'0.07098608081635895:0.2342593506406826:0.0010447858290055308:0.5788884213912752:0.1148213613226778'</t>
-  </si>
-  <si>
-    <t>0.04193551102332393:0.4496555852728088:0.1298469783125372:0.1045832742016494:0.2739786511896807:'0.04193551102332393:0.4496555852728088:0.1298469783125372:0.1045832742016494:0.2739786511896807'</t>
-  </si>
-  <si>
-    <t>0.16899734942148248:0.09394011306381288:0.22992820100492414:0.46969157849230714:0.03744275801747336:'0.16899734942148248:0.09394011306381288:0.22992820100492414:0.46969157849230714:0.03744275801747336'</t>
-  </si>
-  <si>
-    <t>0.21722155723607658:0.06003495743759002:0.20048098648232784:0.3957114651979722:0.12655103364603323:'0.21722155723607658:0.06003495743759002:0.20048098648232784:0.3957114651979722:0.12655103364603323'</t>
-  </si>
-  <si>
-    <t>0.07293784141940536:0.039180538245610075:0.12751952805853817:0.6379849661155549:0.12237712616089151:'0.07293784141940536:0.039180538245610075:0.12751952805853817:0.6379849661155549:0.12237712616089151'</t>
-  </si>
-  <si>
-    <t>0.08597952671094426:0.007373107703755164:0.05819832290198865:0.6919501954151895:0.15649884726812238:'0.08597952671094426:0.007373107703755164:0.05819832290198865:0.6919501954151895:0.15649884726812238'</t>
-  </si>
-  <si>
-    <t>0.2391269771185358:0.11980515008466874:0.0371516636392:0.341735955717008:0.26218025344058743:'0.2391269771185358:0.11980515008466874:0.0371516636392:0.341735955717008:0.26218025344058743'</t>
-  </si>
-  <si>
-    <t>0.0038734044236464053:0.15141123544969604:0.1239330787920094:0.5478035918166799:0.17297868951796821:'0.0038734044236464053:0.15141123544969604:0.1239330787920094:0.5478035918166799:0.17297868951796821'</t>
-  </si>
-  <si>
-    <t>0.13511293658740064:0.06436706646403009:0.25103551846993916:0.24233858495952668:0.3071458935191035:'0.13511293658740064:0.06436706646403009:0.25103551846993916:0.24233858495952668:0.3071458935191035'</t>
-  </si>
-  <si>
-    <t>0.0010790274898496441:0.001230791211281703:0.00043322934840114803:0.9964069679491023:0.0008499840013651758:'0.0010790274898496441:0.001230791211281703:0.00043322934840114803:0.9964069679491023:0.0008499840013651758'</t>
-  </si>
-  <si>
-    <t>0.23377596013418603:0.21868577765632807:0.21491927561621915:0.2580814265398616:0.074537560053405:'0.23377596013418603:0.21868577765632807:0.21491927561621915:0.2580814265398616:0.074537560053405'</t>
-  </si>
-  <si>
-    <t>0.2570750647234156:0.34538605480971696:0.21926666159432445:0.17438907388885735:0.0038831449836855747:'0.2570750647234156:0.34538605480971696:0.21926666159432445:0.17438907388885735:0.0038831449836855747'</t>
-  </si>
-  <si>
-    <t>0.05411212378682602:0.040184273334564105:0.040011537136720614:0.7656895374345389:0.10000252830735035:'0.05411212378682602:0.040184273334564105:0.040011537136720614:0.7656895374345389:0.10000252830735035'</t>
-  </si>
-  <si>
-    <t>0.08270077476439788:0.0405067293390163:0.08045255983596511:0.7462431889969952:0.05009674706362561:'0.08270077476439788:0.0405067293390163:0.08045255983596511:0.7462431889969952:0.05009674706362561'</t>
-  </si>
-  <si>
-    <t>0.04165595053028977:0.06006448699021291:0.038298636775646516:0.8165026538916844:0.043478271812166396:'0.04165595053028977:0.06006448699021291:0.038298636775646516:0.8165026538916844:0.043478271812166396'</t>
-  </si>
-  <si>
-    <t>0.3252409319849474:0.19884286680342372:0.2868468330849948:0.048691367112449924:0.14037800101418405:'0.3252409319849474:0.19884286680342372:0.2868468330849948:0.048691367112449924:0.14037800101418405'</t>
-  </si>
-  <si>
-    <t>0.04723230298522335:0.24410864883377942:0.024494377196729145:0.41688949152990207:0.267275179454366:'0.04723230298522335:0.24410864883377942:0.024494377196729145:0.41688949152990207:0.267275179454366'</t>
-  </si>
-  <si>
-    <t>0.013647930365035737:0.012313135409237473:0.011776021160717033:0.9496819961510143:0.012580916913995415:'0.013647930365035737:0.012313135409237473:0.011776021160717033:0.9496819961510143:0.012580916913995415'</t>
-  </si>
-  <si>
-    <t>0.08087059903348022:0.09418509128847868:0.5737293034264526:0.07145714857544264:0.1797578576761459:'0.08087059903348022:0.09418509128847868:0.5737293034264526:0.07145714857544264:0.1797578576761459'</t>
-  </si>
-  <si>
-    <t>0.006370503431624358:0.04859964178467366:0.028206730676399738:0.03834535796045566:0.8784777661468466:'0.006370503431624358:0.04859964178467366:0.028206730676399738:0.03834535796045566:0.8784777661468466'</t>
-  </si>
-  <si>
-    <t>0.1148213613226778:0.07098608081635895:0.2342593506406826:0.0010447858290055308:0.5788884213912752:'0.1148213613226778:0.07098608081635895:0.2342593506406826:0.0010447858290055308:0.5788884213912752'</t>
-  </si>
-  <si>
-    <t>0.2739786511896807:0.04193551102332393:0.4496555852728088:0.1298469783125372:0.1045832742016494:'0.2739786511896807:0.04193551102332393:0.4496555852728088:0.1298469783125372:0.1045832742016494'</t>
-  </si>
-  <si>
-    <t>0.03744275801747336:0.16899734942148248:0.09394011306381288:0.22992820100492414:0.46969157849230714:'0.03744275801747336:0.16899734942148248:0.09394011306381288:0.22992820100492414:0.46969157849230714'</t>
-  </si>
-  <si>
-    <t>0.12655103364603323:0.21722155723607658:0.06003495743759002:0.20048098648232784:0.3957114651979722:'0.12655103364603323:0.21722155723607658:0.06003495743759002:0.20048098648232784:0.3957114651979722'</t>
-  </si>
-  <si>
-    <t>0.12237712616089151:0.07293784141940536:0.039180538245610075:0.12751952805853817:0.6379849661155549:'0.12237712616089151:0.07293784141940536:0.039180538245610075:0.12751952805853817:0.6379849661155549'</t>
-  </si>
-  <si>
-    <t>0.15649884726812238:0.08597952671094426:0.007373107703755164:0.05819832290198865:0.6919501954151895:'0.15649884726812238:0.08597952671094426:0.007373107703755164:0.05819832290198865:0.6919501954151895'</t>
-  </si>
-  <si>
-    <t>0.26218025344058743:0.2391269771185358:0.11980515008466874:0.0371516636392:0.341735955717008:'0.26218025344058743:0.2391269771185358:0.11980515008466874:0.0371516636392:0.341735955717008'</t>
-  </si>
-  <si>
-    <t>0.17297868951796821:0.0038734044236464053:0.15141123544969604:0.1239330787920094:0.5478035918166799:'0.17297868951796821:0.0038734044236464053:0.15141123544969604:0.1239330787920094:0.5478035918166799'</t>
-  </si>
-  <si>
-    <t>0.3071458935191035:0.13511293658740064:0.06436706646403009:0.25103551846993916:0.24233858495952668:'0.3071458935191035:0.13511293658740064:0.06436706646403009:0.25103551846993916:0.24233858495952668'</t>
-  </si>
-  <si>
-    <t>0.0008499840013651758:0.0010790274898496441:0.001230791211281703:0.00043322934840114803:0.9964069679491023:'0.0008499840013651758:0.0010790274898496441:0.001230791211281703:0.00043322934840114803:0.9964069679491023'</t>
-  </si>
-  <si>
-    <t>0.074537560053405:0.23377596013418603:0.21868577765632807:0.21491927561621915:0.2580814265398616:'0.074537560053405:0.23377596013418603:0.21868577765632807:0.21491927561621915:0.2580814265398616'</t>
-  </si>
-  <si>
-    <t>0.0038831449836855747:0.2570750647234156:0.34538605480971696:0.21926666159432445:0.17438907388885735:'0.0038831449836855747:0.2570750647234156:0.34538605480971696:0.21926666159432445:0.17438907388885735'</t>
-  </si>
-  <si>
-    <t>0.10000252830735035:0.05411212378682602:0.040184273334564105:0.040011537136720614:0.7656895374345389:'0.10000252830735035:0.05411212378682602:0.040184273334564105:0.040011537136720614:0.7656895374345389'</t>
-  </si>
-  <si>
-    <t>0.05009674706362561:0.08270077476439788:0.0405067293390163:0.08045255983596511:0.7462431889969952:'0.05009674706362561:0.08270077476439788:0.0405067293390163:0.08045255983596511:0.7462431889969952'</t>
-  </si>
-  <si>
-    <t>0.043478271812166396:0.04165595053028977:0.06006448699021291:0.038298636775646516:0.8165026538916844:'0.043478271812166396:0.04165595053028977:0.06006448699021291:0.038298636775646516:0.8165026538916844'</t>
-  </si>
-  <si>
-    <t>0.14037800101418405:0.3252409319849474:0.19884286680342372:0.2868468330849948:0.048691367112449924:'0.14037800101418405:0.3252409319849474:0.19884286680342372:0.2868468330849948:0.048691367112449924'</t>
-  </si>
-  <si>
-    <t>0.267275179454366:0.04723230298522335:0.24410864883377942:0.024494377196729145:0.41688949152990207:'0.267275179454366:0.04723230298522335:0.24410864883377942:0.024494377196729145:0.41688949152990207'</t>
-  </si>
-  <si>
-    <t>0.012580916913995415:0.013647930365035737:0.012313135409237473:0.011776021160717033:0.9496819961510143:'0.012580916913995415:0.013647930365035737:0.012313135409237473:0.011776021160717033:0.9496819961510143'</t>
-  </si>
-  <si>
-    <t>0.1797578576761459:0.08087059903348022:0.09418509128847868:0.5737293034264526:0.07145714857544264:'0.1797578576761459:0.08087059903348022:0.09418509128847868:0.5737293034264526:0.07145714857544264'</t>
-  </si>
-  <si>
     <t>ngA</t>
-  </si>
-  <si>
-    <t>0.8784777661468466:0.006370503431624358:0.04859964178467366:0.028206730676399738:0.03834535796045566:"0.8784777661468466:0.006370503431624358:0.04859964178467366:0.028206730676399738:0.03834535796045566:'0.8784777661468466:0.006370503431624358:0.04859964178467366:0.028206730676399738:0.03834535796045566'"</t>
-  </si>
-  <si>
-    <t>0.5788884213912752:0.1148213613226778:0.07098608081635895:0.2342593506406826:0.0010447858290055308:"0.5788884213912752:0.1148213613226778:0.07098608081635895:0.2342593506406826:0.0010447858290055308:'0.5788884213912752:0.1148213613226778:0.07098608081635895:0.2342593506406826:0.0010447858290055308'"</t>
-  </si>
-  <si>
-    <t>0.1045832742016494:0.2739786511896807:0.04193551102332393:0.4496555852728088:0.1298469783125372:"0.1045832742016494:0.2739786511896807:0.04193551102332393:0.4496555852728088:0.1298469783125372:'0.1045832742016494:0.2739786511896807:0.04193551102332393:0.4496555852728088:0.1298469783125372'"</t>
-  </si>
-  <si>
-    <t>0.46969157849230714:0.03744275801747336:0.16899734942148248:0.09394011306381288:0.22992820100492414:"0.46969157849230714:0.03744275801747336:0.16899734942148248:0.09394011306381288:0.22992820100492414:'0.46969157849230714:0.03744275801747336:0.16899734942148248:0.09394011306381288:0.22992820100492414'"</t>
-  </si>
-  <si>
-    <t>0.3957114651979722:0.12655103364603323:0.21722155723607658:0.06003495743759002:0.20048098648232784:"0.3957114651979722:0.12655103364603323:0.21722155723607658:0.06003495743759002:0.20048098648232784:'0.3957114651979722:0.12655103364603323:0.21722155723607658:0.06003495743759002:0.20048098648232784'"</t>
-  </si>
-  <si>
-    <t>0.6379849661155549:0.12237712616089151:0.07293784141940536:0.039180538245610075:0.12751952805853817:"0.6379849661155549:0.12237712616089151:0.07293784141940536:0.039180538245610075:0.12751952805853817:'0.6379849661155549:0.12237712616089151:0.07293784141940536:0.039180538245610075:0.12751952805853817'"</t>
-  </si>
-  <si>
-    <t>0.6919501954151895:0.15649884726812238:0.08597952671094426:0.007373107703755164:0.05819832290198865:"0.6919501954151895:0.15649884726812238:0.08597952671094426:0.007373107703755164:0.05819832290198865:'0.6919501954151895:0.15649884726812238:0.08597952671094426:0.007373107703755164:0.05819832290198865'"</t>
-  </si>
-  <si>
-    <t>0.341735955717008:0.26218025344058743:0.2391269771185358:0.11980515008466874:0.0371516636392:"0.341735955717008:0.26218025344058743:0.2391269771185358:0.11980515008466874:0.0371516636392:'0.341735955717008:0.26218025344058743:0.2391269771185358:0.11980515008466874:0.0371516636392'"</t>
-  </si>
-  <si>
-    <t>0.5478035918166799:0.17297868951796821:0.0038734044236464053:0.15141123544969604:0.1239330787920094:"0.5478035918166799:0.17297868951796821:0.0038734044236464053:0.15141123544969604:0.1239330787920094:'0.5478035918166799:0.17297868951796821:0.0038734044236464053:0.15141123544969604:0.1239330787920094'"</t>
-  </si>
-  <si>
-    <t>0.24233858495952668:0.3071458935191035:0.13511293658740064:0.06436706646403009:0.25103551846993916:"0.24233858495952668:0.3071458935191035:0.13511293658740064:0.06436706646403009:0.25103551846993916:'0.24233858495952668:0.3071458935191035:0.13511293658740064:0.06436706646403009:0.25103551846993916'"</t>
-  </si>
-  <si>
-    <t>0.9964069679491023:0.0008499840013651758:0.0010790274898496441:0.001230791211281703:0.00043322934840114803:"0.9964069679491023:0.0008499840013651758:0.0010790274898496441:0.001230791211281703:0.00043322934840114803:'0.9964069679491023:0.0008499840013651758:0.0010790274898496441:0.001230791211281703:0.00043322934840114803'"</t>
-  </si>
-  <si>
-    <t>0.2580814265398616:0.074537560053405:0.23377596013418603:0.21868577765632807:0.21491927561621915:"0.2580814265398616:0.074537560053405:0.23377596013418603:0.21868577765632807:0.21491927561621915:'0.2580814265398616:0.074537560053405:0.23377596013418603:0.21868577765632807:0.21491927561621915'"</t>
-  </si>
-  <si>
-    <t>0.17438907388885735:0.0038831449836855747:0.2570750647234156:0.34538605480971696:0.21926666159432445:"0.17438907388885735:0.0038831449836855747:0.2570750647234156:0.34538605480971696:0.21926666159432445:'0.17438907388885735:0.0038831449836855747:0.2570750647234156:0.34538605480971696:0.21926666159432445'"</t>
-  </si>
-  <si>
-    <t>0.7656895374345389:0.10000252830735035:0.05411212378682602:0.040184273334564105:0.040011537136720614:"0.7656895374345389:0.10000252830735035:0.05411212378682602:0.040184273334564105:0.040011537136720614:'0.7656895374345389:0.10000252830735035:0.05411212378682602:0.040184273334564105:0.040011537136720614'"</t>
-  </si>
-  <si>
-    <t>0.7462431889969952:0.05009674706362561:0.08270077476439788:0.0405067293390163:0.08045255983596511:"0.7462431889969952:0.05009674706362561:0.08270077476439788:0.0405067293390163:0.08045255983596511:'0.7462431889969952:0.05009674706362561:0.08270077476439788:0.0405067293390163:0.08045255983596511'"</t>
-  </si>
-  <si>
-    <t>0.8165026538916844:0.043478271812166396:0.04165595053028977:0.06006448699021291:0.038298636775646516:"0.8165026538916844:0.043478271812166396:0.04165595053028977:0.06006448699021291:0.038298636775646516:'0.8165026538916844:0.043478271812166396:0.04165595053028977:0.06006448699021291:0.038298636775646516'"</t>
-  </si>
-  <si>
-    <t>0.048691367112449924:0.14037800101418405:0.3252409319849474:0.19884286680342372:0.2868468330849948:"0.048691367112449924:0.14037800101418405:0.3252409319849474:0.19884286680342372:0.2868468330849948:'0.048691367112449924:0.14037800101418405:0.3252409319849474:0.19884286680342372:0.2868468330849948'"</t>
-  </si>
-  <si>
-    <t>0.41688949152990207:0.267275179454366:0.04723230298522335:0.24410864883377942:0.024494377196729145:"0.41688949152990207:0.267275179454366:0.04723230298522335:0.24410864883377942:0.024494377196729145:'0.41688949152990207:0.267275179454366:0.04723230298522335:0.24410864883377942:0.024494377196729145'"</t>
-  </si>
-  <si>
-    <t>0.9496819961510143:0.012580916913995415:0.013647930365035737:0.012313135409237473:0.011776021160717033:"0.9496819961510143:0.012580916913995415:0.013647930365035737:0.012313135409237473:0.011776021160717033:'0.9496819961510143:0.012580916913995415:0.013647930365035737:0.012313135409237473:0.011776021160717033'"</t>
-  </si>
-  <si>
-    <t>0.07145714857544264:0.1797578576761459:0.08087059903348022:0.09418509128847868:0.5737293034264526:"0.07145714857544264:0.1797578576761459:0.08087059903348022:0.09418509128847868:0.5737293034264526:'0.07145714857544264:0.1797578576761459:0.08087059903348022:0.09418509128847868:0.5737293034264526'"</t>
-  </si>
-  <si>
-    <t>0.03834535796045566:0.8784777661468466:0.006370503431624358:0.04859964178467366:0.028206730676399738:"0.03834535796045566:0.8784777661468466:0.006370503431624358:0.04859964178467366:0.028206730676399738:'0.03834535796045566:0.8784777661468466:0.006370503431624358:0.04859964178467366:0.028206730676399738'"</t>
-  </si>
-  <si>
-    <t>0.0010447858290055308:0.5788884213912752:0.1148213613226778:0.07098608081635895:0.2342593506406826:"0.0010447858290055308:0.5788884213912752:0.1148213613226778:0.07098608081635895:0.2342593506406826:'0.0010447858290055308:0.5788884213912752:0.1148213613226778:0.07098608081635895:0.2342593506406826'"</t>
-  </si>
-  <si>
-    <t>0.1298469783125372:0.1045832742016494:0.2739786511896807:0.04193551102332393:0.4496555852728088:"0.1298469783125372:0.1045832742016494:0.2739786511896807:0.04193551102332393:0.4496555852728088:'0.1298469783125372:0.1045832742016494:0.2739786511896807:0.04193551102332393:0.4496555852728088'"</t>
-  </si>
-  <si>
-    <t>0.22992820100492414:0.46969157849230714:0.03744275801747336:0.16899734942148248:0.09394011306381288:"0.22992820100492414:0.46969157849230714:0.03744275801747336:0.16899734942148248:0.09394011306381288:'0.22992820100492414:0.46969157849230714:0.03744275801747336:0.16899734942148248:0.09394011306381288'"</t>
-  </si>
-  <si>
-    <t>0.20048098648232784:0.3957114651979722:0.12655103364603323:0.21722155723607658:0.06003495743759002:"0.20048098648232784:0.3957114651979722:0.12655103364603323:0.21722155723607658:0.06003495743759002:'0.20048098648232784:0.3957114651979722:0.12655103364603323:0.21722155723607658:0.06003495743759002'"</t>
-  </si>
-  <si>
-    <t>0.12751952805853817:0.6379849661155549:0.12237712616089151:0.07293784141940536:0.039180538245610075:"0.12751952805853817:0.6379849661155549:0.12237712616089151:0.07293784141940536:0.039180538245610075:'0.12751952805853817:0.6379849661155549:0.12237712616089151:0.07293784141940536:0.039180538245610075'"</t>
-  </si>
-  <si>
-    <t>0.05819832290198865:0.6919501954151895:0.15649884726812238:0.08597952671094426:0.007373107703755164:"0.05819832290198865:0.6919501954151895:0.15649884726812238:0.08597952671094426:0.007373107703755164:'0.05819832290198865:0.6919501954151895:0.15649884726812238:0.08597952671094426:0.007373107703755164'"</t>
-  </si>
-  <si>
-    <t>0.0371516636392:0.341735955717008:0.26218025344058743:0.2391269771185358:0.11980515008466874:"0.0371516636392:0.341735955717008:0.26218025344058743:0.2391269771185358:0.11980515008466874:'0.0371516636392:0.341735955717008:0.26218025344058743:0.2391269771185358:0.11980515008466874'"</t>
-  </si>
-  <si>
-    <t>0.1239330787920094:0.5478035918166799:0.17297868951796821:0.0038734044236464053:0.15141123544969604:"0.1239330787920094:0.5478035918166799:0.17297868951796821:0.0038734044236464053:0.15141123544969604:'0.1239330787920094:0.5478035918166799:0.17297868951796821:0.0038734044236464053:0.15141123544969604'"</t>
-  </si>
-  <si>
-    <t>0.25103551846993916:0.24233858495952668:0.3071458935191035:0.13511293658740064:0.06436706646403009:"0.25103551846993916:0.24233858495952668:0.3071458935191035:0.13511293658740064:0.06436706646403009:'0.25103551846993916:0.24233858495952668:0.3071458935191035:0.13511293658740064:0.06436706646403009'"</t>
-  </si>
-  <si>
-    <t>0.00043322934840114803:0.9964069679491023:0.0008499840013651758:0.0010790274898496441:0.001230791211281703:"0.00043322934840114803:0.9964069679491023:0.0008499840013651758:0.0010790274898496441:0.001230791211281703:'0.00043322934840114803:0.9964069679491023:0.0008499840013651758:0.0010790274898496441:0.001230791211281703'"</t>
-  </si>
-  <si>
-    <t>0.21491927561621915:0.2580814265398616:0.074537560053405:0.23377596013418603:0.21868577765632807:"0.21491927561621915:0.2580814265398616:0.074537560053405:0.23377596013418603:0.21868577765632807:'0.21491927561621915:0.2580814265398616:0.074537560053405:0.23377596013418603:0.21868577765632807'"</t>
-  </si>
-  <si>
-    <t>0.21926666159432445:0.17438907388885735:0.0038831449836855747:0.2570750647234156:0.34538605480971696:"0.21926666159432445:0.17438907388885735:0.0038831449836855747:0.2570750647234156:0.34538605480971696:'0.21926666159432445:0.17438907388885735:0.0038831449836855747:0.2570750647234156:0.34538605480971696'"</t>
-  </si>
-  <si>
-    <t>0.040011537136720614:0.7656895374345389:0.10000252830735035:0.05411212378682602:0.040184273334564105:"0.040011537136720614:0.7656895374345389:0.10000252830735035:0.05411212378682602:0.040184273334564105:'0.040011537136720614:0.7656895374345389:0.10000252830735035:0.05411212378682602:0.040184273334564105'"</t>
-  </si>
-  <si>
-    <t>0.08045255983596511:0.7462431889969952:0.05009674706362561:0.08270077476439788:0.0405067293390163:"0.08045255983596511:0.7462431889969952:0.05009674706362561:0.08270077476439788:0.0405067293390163:'0.08045255983596511:0.7462431889969952:0.05009674706362561:0.08270077476439788:0.0405067293390163'"</t>
-  </si>
-  <si>
-    <t>0.038298636775646516:0.8165026538916844:0.043478271812166396:0.04165595053028977:0.06006448699021291:"0.038298636775646516:0.8165026538916844:0.043478271812166396:0.04165595053028977:0.06006448699021291:'0.038298636775646516:0.8165026538916844:0.043478271812166396:0.04165595053028977:0.06006448699021291'"</t>
-  </si>
-  <si>
-    <t>0.2868468330849948:0.048691367112449924:0.14037800101418405:0.3252409319849474:0.19884286680342372:"0.2868468330849948:0.048691367112449924:0.14037800101418405:0.3252409319849474:0.19884286680342372:'0.2868468330849948:0.048691367112449924:0.14037800101418405:0.3252409319849474:0.19884286680342372'"</t>
-  </si>
-  <si>
-    <t>0.024494377196729145:0.41688949152990207:0.267275179454366:0.04723230298522335:0.24410864883377942:"0.024494377196729145:0.41688949152990207:0.267275179454366:0.04723230298522335:0.24410864883377942:'0.024494377196729145:0.41688949152990207:0.267275179454366:0.04723230298522335:0.24410864883377942'"</t>
-  </si>
-  <si>
-    <t>0.011776021160717033:0.9496819961510143:0.012580916913995415:0.013647930365035737:0.012313135409237473:"0.011776021160717033:0.9496819961510143:0.012580916913995415:0.013647930365035737:0.012313135409237473:'0.011776021160717033:0.9496819961510143:0.012580916913995415:0.013647930365035737:0.012313135409237473'"</t>
-  </si>
-  <si>
-    <t>0.5737293034264526:0.07145714857544264:0.1797578576761459:0.08087059903348022:0.09418509128847868:"0.5737293034264526:0.07145714857544264:0.1797578576761459:0.08087059903348022:0.09418509128847868:'0.5737293034264526:0.07145714857544264:0.1797578576761459:0.08087059903348022:0.09418509128847868'"</t>
-  </si>
-  <si>
-    <t>0.028206730676399738:0.03834535796045566:0.8784777661468466:0.006370503431624358:0.04859964178467366:"0.028206730676399738:0.03834535796045566:0.8784777661468466:0.006370503431624358:0.04859964178467366:'0.028206730676399738:0.03834535796045566:0.8784777661468466:0.006370503431624358:0.04859964178467366'"</t>
-  </si>
-  <si>
-    <t>0.2342593506406826:0.0010447858290055308:0.5788884213912752:0.1148213613226778:0.07098608081635895:"0.2342593506406826:0.0010447858290055308:0.5788884213912752:0.1148213613226778:0.07098608081635895:'0.2342593506406826:0.0010447858290055308:0.5788884213912752:0.1148213613226778:0.07098608081635895'"</t>
-  </si>
-  <si>
-    <t>0.4496555852728088:0.1298469783125372:0.1045832742016494:0.2739786511896807:0.04193551102332393:"0.4496555852728088:0.1298469783125372:0.1045832742016494:0.2739786511896807:0.04193551102332393:'0.4496555852728088:0.1298469783125372:0.1045832742016494:0.2739786511896807:0.04193551102332393'"</t>
-  </si>
-  <si>
-    <t>0.09394011306381288:0.22992820100492414:0.46969157849230714:0.03744275801747336:0.16899734942148248:"0.09394011306381288:0.22992820100492414:0.46969157849230714:0.03744275801747336:0.16899734942148248:'0.09394011306381288:0.22992820100492414:0.46969157849230714:0.03744275801747336:0.16899734942148248'"</t>
-  </si>
-  <si>
-    <t>0.06003495743759002:0.20048098648232784:0.3957114651979722:0.12655103364603323:0.21722155723607658:"0.06003495743759002:0.20048098648232784:0.3957114651979722:0.12655103364603323:0.21722155723607658:'0.06003495743759002:0.20048098648232784:0.3957114651979722:0.12655103364603323:0.21722155723607658'"</t>
-  </si>
-  <si>
-    <t>0.039180538245610075:0.12751952805853817:0.6379849661155549:0.12237712616089151:0.07293784141940536:"0.039180538245610075:0.12751952805853817:0.6379849661155549:0.12237712616089151:0.07293784141940536:'0.039180538245610075:0.12751952805853817:0.6379849661155549:0.12237712616089151:0.07293784141940536'"</t>
-  </si>
-  <si>
-    <t>0.007373107703755164:0.05819832290198865:0.6919501954151895:0.15649884726812238:0.08597952671094426:"0.007373107703755164:0.05819832290198865:0.6919501954151895:0.15649884726812238:0.08597952671094426:'0.007373107703755164:0.05819832290198865:0.6919501954151895:0.15649884726812238:0.08597952671094426'"</t>
-  </si>
-  <si>
-    <t>0.11980515008466874:0.0371516636392:0.341735955717008:0.26218025344058743:0.2391269771185358:"0.11980515008466874:0.0371516636392:0.341735955717008:0.26218025344058743:0.2391269771185358:'0.11980515008466874:0.0371516636392:0.341735955717008:0.26218025344058743:0.2391269771185358'"</t>
-  </si>
-  <si>
-    <t>0.15141123544969604:0.1239330787920094:0.5478035918166799:0.17297868951796821:0.0038734044236464053:"0.15141123544969604:0.1239330787920094:0.5478035918166799:0.17297868951796821:0.0038734044236464053:'0.15141123544969604:0.1239330787920094:0.5478035918166799:0.17297868951796821:0.0038734044236464053'"</t>
-  </si>
-  <si>
-    <t>0.06436706646403009:0.25103551846993916:0.24233858495952668:0.3071458935191035:0.13511293658740064:"0.06436706646403009:0.25103551846993916:0.24233858495952668:0.3071458935191035:0.13511293658740064:'0.06436706646403009:0.25103551846993916:0.24233858495952668:0.3071458935191035:0.13511293658740064'"</t>
-  </si>
-  <si>
-    <t>0.001230791211281703:0.00043322934840114803:0.9964069679491023:0.0008499840013651758:0.0010790274898496441:"0.001230791211281703:0.00043322934840114803:0.9964069679491023:0.0008499840013651758:0.0010790274898496441:'0.001230791211281703:0.00043322934840114803:0.9964069679491023:0.0008499840013651758:0.0010790274898496441'"</t>
-  </si>
-  <si>
-    <t>0.21868577765632807:0.21491927561621915:0.2580814265398616:0.074537560053405:0.23377596013418603:"0.21868577765632807:0.21491927561621915:0.2580814265398616:0.074537560053405:0.23377596013418603:'0.21868577765632807:0.21491927561621915:0.2580814265398616:0.074537560053405:0.23377596013418603'"</t>
-  </si>
-  <si>
-    <t>0.34538605480971696:0.21926666159432445:0.17438907388885735:0.0038831449836855747:0.2570750647234156:"0.34538605480971696:0.21926666159432445:0.17438907388885735:0.0038831449836855747:0.2570750647234156:'0.34538605480971696:0.21926666159432445:0.17438907388885735:0.0038831449836855747:0.2570750647234156'"</t>
-  </si>
-  <si>
-    <t>0.040184273334564105:0.040011537136720614:0.7656895374345389:0.10000252830735035:0.05411212378682602:"0.040184273334564105:0.040011537136720614:0.7656895374345389:0.10000252830735035:0.05411212378682602:'0.040184273334564105:0.040011537136720614:0.7656895374345389:0.10000252830735035:0.05411212378682602'"</t>
-  </si>
-  <si>
-    <t>0.0405067293390163:0.08045255983596511:0.7462431889969952:0.05009674706362561:0.08270077476439788:"0.0405067293390163:0.08045255983596511:0.7462431889969952:0.05009674706362561:0.08270077476439788:'0.0405067293390163:0.08045255983596511:0.7462431889969952:0.05009674706362561:0.08270077476439788'"</t>
-  </si>
-  <si>
-    <t>0.06006448699021291:0.038298636775646516:0.8165026538916844:0.043478271812166396:0.04165595053028977:"0.06006448699021291:0.038298636775646516:0.8165026538916844:0.043478271812166396:0.04165595053028977:'0.06006448699021291:0.038298636775646516:0.8165026538916844:0.043478271812166396:0.04165595053028977'"</t>
-  </si>
-  <si>
-    <t>0.19884286680342372:0.2868468330849948:0.048691367112449924:0.14037800101418405:0.3252409319849474:"0.19884286680342372:0.2868468330849948:0.048691367112449924:0.14037800101418405:0.3252409319849474:'0.19884286680342372:0.2868468330849948:0.048691367112449924:0.14037800101418405:0.3252409319849474'"</t>
-  </si>
-  <si>
-    <t>0.24410864883377942:0.024494377196729145:0.41688949152990207:0.267275179454366:0.04723230298522335:"0.24410864883377942:0.024494377196729145:0.41688949152990207:0.267275179454366:0.04723230298522335:'0.24410864883377942:0.024494377196729145:0.41688949152990207:0.267275179454366:0.04723230298522335'"</t>
-  </si>
-  <si>
-    <t>0.012313135409237473:0.011776021160717033:0.9496819961510143:0.012580916913995415:0.013647930365035737:"0.012313135409237473:0.011776021160717033:0.9496819961510143:0.012580916913995415:0.013647930365035737:'0.012313135409237473:0.011776021160717033:0.9496819961510143:0.012580916913995415:0.013647930365035737'"</t>
-  </si>
-  <si>
-    <t>0.09418509128847868:0.5737293034264526:0.07145714857544264:0.1797578576761459:0.08087059903348022:"0.09418509128847868:0.5737293034264526:0.07145714857544264:0.1797578576761459:0.08087059903348022:'0.09418509128847868:0.5737293034264526:0.07145714857544264:0.1797578576761459:0.08087059903348022'"</t>
-  </si>
-  <si>
-    <t>0.04859964178467366:0.028206730676399738:0.03834535796045566:0.8784777661468466:0.006370503431624358:"0.04859964178467366:0.028206730676399738:0.03834535796045566:0.8784777661468466:0.006370503431624358:'0.04859964178467366:0.028206730676399738:0.03834535796045566:0.8784777661468466:0.006370503431624358'"</t>
-  </si>
-  <si>
-    <t>0.07098608081635895:0.2342593506406826:0.0010447858290055308:0.5788884213912752:0.1148213613226778:"0.07098608081635895:0.2342593506406826:0.0010447858290055308:0.5788884213912752:0.1148213613226778:'0.07098608081635895:0.2342593506406826:0.0010447858290055308:0.5788884213912752:0.1148213613226778'"</t>
-  </si>
-  <si>
-    <t>0.04193551102332393:0.4496555852728088:0.1298469783125372:0.1045832742016494:0.2739786511896807:"0.04193551102332393:0.4496555852728088:0.1298469783125372:0.1045832742016494:0.2739786511896807:'0.04193551102332393:0.4496555852728088:0.1298469783125372:0.1045832742016494:0.2739786511896807'"</t>
-  </si>
-  <si>
-    <t>0.16899734942148248:0.09394011306381288:0.22992820100492414:0.46969157849230714:0.03744275801747336:"0.16899734942148248:0.09394011306381288:0.22992820100492414:0.46969157849230714:0.03744275801747336:'0.16899734942148248:0.09394011306381288:0.22992820100492414:0.46969157849230714:0.03744275801747336'"</t>
-  </si>
-  <si>
-    <t>0.21722155723607658:0.06003495743759002:0.20048098648232784:0.3957114651979722:0.12655103364603323:"0.21722155723607658:0.06003495743759002:0.20048098648232784:0.3957114651979722:0.12655103364603323:'0.21722155723607658:0.06003495743759002:0.20048098648232784:0.3957114651979722:0.12655103364603323'"</t>
-  </si>
-  <si>
-    <t>0.07293784141940536:0.039180538245610075:0.12751952805853817:0.6379849661155549:0.12237712616089151:"0.07293784141940536:0.039180538245610075:0.12751952805853817:0.6379849661155549:0.12237712616089151:'0.07293784141940536:0.039180538245610075:0.12751952805853817:0.6379849661155549:0.12237712616089151'"</t>
-  </si>
-  <si>
-    <t>0.08597952671094426:0.007373107703755164:0.05819832290198865:0.6919501954151895:0.15649884726812238:"0.08597952671094426:0.007373107703755164:0.05819832290198865:0.6919501954151895:0.15649884726812238:'0.08597952671094426:0.007373107703755164:0.05819832290198865:0.6919501954151895:0.15649884726812238'"</t>
-  </si>
-  <si>
-    <t>0.2391269771185358:0.11980515008466874:0.0371516636392:0.341735955717008:0.26218025344058743:"0.2391269771185358:0.11980515008466874:0.0371516636392:0.341735955717008:0.26218025344058743:'0.2391269771185358:0.11980515008466874:0.0371516636392:0.341735955717008:0.26218025344058743'"</t>
-  </si>
-  <si>
-    <t>0.0038734044236464053:0.15141123544969604:0.1239330787920094:0.5478035918166799:0.17297868951796821:"0.0038734044236464053:0.15141123544969604:0.1239330787920094:0.5478035918166799:0.17297868951796821:'0.0038734044236464053:0.15141123544969604:0.1239330787920094:0.5478035918166799:0.17297868951796821'"</t>
-  </si>
-  <si>
-    <t>0.13511293658740064:0.06436706646403009:0.25103551846993916:0.24233858495952668:0.3071458935191035:"0.13511293658740064:0.06436706646403009:0.25103551846993916:0.24233858495952668:0.3071458935191035:'0.13511293658740064:0.06436706646403009:0.25103551846993916:0.24233858495952668:0.3071458935191035'"</t>
-  </si>
-  <si>
-    <t>0.0010790274898496441:0.001230791211281703:0.00043322934840114803:0.9964069679491023:0.0008499840013651758:"0.0010790274898496441:0.001230791211281703:0.00043322934840114803:0.9964069679491023:0.0008499840013651758:'0.0010790274898496441:0.001230791211281703:0.00043322934840114803:0.9964069679491023:0.0008499840013651758'"</t>
-  </si>
-  <si>
-    <t>0.23377596013418603:0.21868577765632807:0.21491927561621915:0.2580814265398616:0.074537560053405:"0.23377596013418603:0.21868577765632807:0.21491927561621915:0.2580814265398616:0.074537560053405:'0.23377596013418603:0.21868577765632807:0.21491927561621915:0.2580814265398616:0.074537560053405'"</t>
-  </si>
-  <si>
-    <t>0.2570750647234156:0.34538605480971696:0.21926666159432445:0.17438907388885735:0.0038831449836855747:"0.2570750647234156:0.34538605480971696:0.21926666159432445:0.17438907388885735:0.0038831449836855747:'0.2570750647234156:0.34538605480971696:0.21926666159432445:0.17438907388885735:0.0038831449836855747'"</t>
-  </si>
-  <si>
-    <t>0.05411212378682602:0.040184273334564105:0.040011537136720614:0.7656895374345389:0.10000252830735035:"0.05411212378682602:0.040184273334564105:0.040011537136720614:0.7656895374345389:0.10000252830735035:'0.05411212378682602:0.040184273334564105:0.040011537136720614:0.7656895374345389:0.10000252830735035'"</t>
-  </si>
-  <si>
-    <t>0.08270077476439788:0.0405067293390163:0.08045255983596511:0.7462431889969952:0.05009674706362561:"0.08270077476439788:0.0405067293390163:0.08045255983596511:0.7462431889969952:0.05009674706362561:'0.08270077476439788:0.0405067293390163:0.08045255983596511:0.7462431889969952:0.05009674706362561'"</t>
-  </si>
-  <si>
-    <t>0.04165595053028977:0.06006448699021291:0.038298636775646516:0.8165026538916844:0.043478271812166396:"0.04165595053028977:0.06006448699021291:0.038298636775646516:0.8165026538916844:0.043478271812166396:'0.04165595053028977:0.06006448699021291:0.038298636775646516:0.8165026538916844:0.043478271812166396'"</t>
-  </si>
-  <si>
-    <t>0.3252409319849474:0.19884286680342372:0.2868468330849948:0.048691367112449924:0.14037800101418405:"0.3252409319849474:0.19884286680342372:0.2868468330849948:0.048691367112449924:0.14037800101418405:'0.3252409319849474:0.19884286680342372:0.2868468330849948:0.048691367112449924:0.14037800101418405'"</t>
-  </si>
-  <si>
-    <t>0.04723230298522335:0.24410864883377942:0.024494377196729145:0.41688949152990207:0.267275179454366:"0.04723230298522335:0.24410864883377942:0.024494377196729145:0.41688949152990207:0.267275179454366:'0.04723230298522335:0.24410864883377942:0.024494377196729145:0.41688949152990207:0.267275179454366'"</t>
-  </si>
-  <si>
-    <t>0.013647930365035737:0.012313135409237473:0.011776021160717033:0.9496819961510143:0.012580916913995415:"0.013647930365035737:0.012313135409237473:0.011776021160717033:0.9496819961510143:0.012580916913995415:'0.013647930365035737:0.012313135409237473:0.011776021160717033:0.9496819961510143:0.012580916913995415'"</t>
-  </si>
-  <si>
-    <t>0.08087059903348022:0.09418509128847868:0.5737293034264526:0.07145714857544264:0.1797578576761459:"0.08087059903348022:0.09418509128847868:0.5737293034264526:0.07145714857544264:0.1797578576761459:'0.08087059903348022:0.09418509128847868:0.5737293034264526:0.07145714857544264:0.1797578576761459'"</t>
-  </si>
-  <si>
-    <t>0.006370503431624358:0.04859964178467366:0.028206730676399738:0.03834535796045566:0.8784777661468466:"0.006370503431624358:0.04859964178467366:0.028206730676399738:0.03834535796045566:0.8784777661468466:'0.006370503431624358:0.04859964178467366:0.028206730676399738:0.03834535796045566:0.8784777661468466'"</t>
-  </si>
-  <si>
-    <t>0.1148213613226778:0.07098608081635895:0.2342593506406826:0.0010447858290055308:0.5788884213912752:"0.1148213613226778:0.07098608081635895:0.2342593506406826:0.0010447858290055308:0.5788884213912752:'0.1148213613226778:0.07098608081635895:0.2342593506406826:0.0010447858290055308:0.5788884213912752'"</t>
-  </si>
-  <si>
-    <t>0.2739786511896807:0.04193551102332393:0.4496555852728088:0.1298469783125372:0.1045832742016494:"0.2739786511896807:0.04193551102332393:0.4496555852728088:0.1298469783125372:0.1045832742016494:'0.2739786511896807:0.04193551102332393:0.4496555852728088:0.1298469783125372:0.1045832742016494'"</t>
-  </si>
-  <si>
-    <t>0.03744275801747336:0.16899734942148248:0.09394011306381288:0.22992820100492414:0.46969157849230714:"0.03744275801747336:0.16899734942148248:0.09394011306381288:0.22992820100492414:0.46969157849230714:'0.03744275801747336:0.16899734942148248:0.09394011306381288:0.22992820100492414:0.46969157849230714'"</t>
-  </si>
-  <si>
-    <t>0.12655103364603323:0.21722155723607658:0.06003495743759002:0.20048098648232784:0.3957114651979722:"0.12655103364603323:0.21722155723607658:0.06003495743759002:0.20048098648232784:0.3957114651979722:'0.12655103364603323:0.21722155723607658:0.06003495743759002:0.20048098648232784:0.3957114651979722'"</t>
-  </si>
-  <si>
-    <t>0.12237712616089151:0.07293784141940536:0.039180538245610075:0.12751952805853817:0.6379849661155549:"0.12237712616089151:0.07293784141940536:0.039180538245610075:0.12751952805853817:0.6379849661155549:'0.12237712616089151:0.07293784141940536:0.039180538245610075:0.12751952805853817:0.6379849661155549'"</t>
-  </si>
-  <si>
-    <t>0.15649884726812238:0.08597952671094426:0.007373107703755164:0.05819832290198865:0.6919501954151895:"0.15649884726812238:0.08597952671094426:0.007373107703755164:0.05819832290198865:0.6919501954151895:'0.15649884726812238:0.08597952671094426:0.007373107703755164:0.05819832290198865:0.6919501954151895'"</t>
-  </si>
-  <si>
-    <t>0.26218025344058743:0.2391269771185358:0.11980515008466874:0.0371516636392:0.341735955717008:"0.26218025344058743:0.2391269771185358:0.11980515008466874:0.0371516636392:0.341735955717008:'0.26218025344058743:0.2391269771185358:0.11980515008466874:0.0371516636392:0.341735955717008'"</t>
-  </si>
-  <si>
-    <t>0.17297868951796821:0.0038734044236464053:0.15141123544969604:0.1239330787920094:0.5478035918166799:"0.17297868951796821:0.0038734044236464053:0.15141123544969604:0.1239330787920094:0.5478035918166799:'0.17297868951796821:0.0038734044236464053:0.15141123544969604:0.1239330787920094:0.5478035918166799'"</t>
-  </si>
-  <si>
-    <t>0.3071458935191035:0.13511293658740064:0.06436706646403009:0.25103551846993916:0.24233858495952668:"0.3071458935191035:0.13511293658740064:0.06436706646403009:0.25103551846993916:0.24233858495952668:'0.3071458935191035:0.13511293658740064:0.06436706646403009:0.25103551846993916:0.24233858495952668'"</t>
-  </si>
-  <si>
-    <t>0.0008499840013651758:0.0010790274898496441:0.001230791211281703:0.00043322934840114803:0.9964069679491023:"0.0008499840013651758:0.0010790274898496441:0.001230791211281703:0.00043322934840114803:0.9964069679491023:'0.0008499840013651758:0.0010790274898496441:0.001230791211281703:0.00043322934840114803:0.9964069679491023'"</t>
-  </si>
-  <si>
-    <t>0.074537560053405:0.23377596013418603:0.21868577765632807:0.21491927561621915:0.2580814265398616:"0.074537560053405:0.23377596013418603:0.21868577765632807:0.21491927561621915:0.2580814265398616:'0.074537560053405:0.23377596013418603:0.21868577765632807:0.21491927561621915:0.2580814265398616'"</t>
-  </si>
-  <si>
-    <t>0.0038831449836855747:0.2570750647234156:0.34538605480971696:0.21926666159432445:0.17438907388885735:"0.0038831449836855747:0.2570750647234156:0.34538605480971696:0.21926666159432445:0.17438907388885735:'0.0038831449836855747:0.2570750647234156:0.34538605480971696:0.21926666159432445:0.17438907388885735'"</t>
-  </si>
-  <si>
-    <t>0.10000252830735035:0.05411212378682602:0.040184273334564105:0.040011537136720614:0.7656895374345389:"0.10000252830735035:0.05411212378682602:0.040184273334564105:0.040011537136720614:0.7656895374345389:'0.10000252830735035:0.05411212378682602:0.040184273334564105:0.040011537136720614:0.7656895374345389'"</t>
-  </si>
-  <si>
-    <t>0.05009674706362561:0.08270077476439788:0.0405067293390163:0.08045255983596511:0.7462431889969952:"0.05009674706362561:0.08270077476439788:0.0405067293390163:0.08045255983596511:0.7462431889969952:'0.05009674706362561:0.08270077476439788:0.0405067293390163:0.08045255983596511:0.7462431889969952'"</t>
-  </si>
-  <si>
-    <t>0.043478271812166396:0.04165595053028977:0.06006448699021291:0.038298636775646516:0.8165026538916844:"0.043478271812166396:0.04165595053028977:0.06006448699021291:0.038298636775646516:0.8165026538916844:'0.043478271812166396:0.04165595053028977:0.06006448699021291:0.038298636775646516:0.8165026538916844'"</t>
-  </si>
-  <si>
-    <t>0.14037800101418405:0.3252409319849474:0.19884286680342372:0.2868468330849948:0.048691367112449924:"0.14037800101418405:0.3252409319849474:0.19884286680342372:0.2868468330849948:0.048691367112449924:'0.14037800101418405:0.3252409319849474:0.19884286680342372:0.2868468330849948:0.048691367112449924'"</t>
-  </si>
-  <si>
-    <t>0.267275179454366:0.04723230298522335:0.24410864883377942:0.024494377196729145:0.41688949152990207:"0.267275179454366:0.04723230298522335:0.24410864883377942:0.024494377196729145:0.41688949152990207:'0.267275179454366:0.04723230298522335:0.24410864883377942:0.024494377196729145:0.41688949152990207'"</t>
-  </si>
-  <si>
-    <t>0.012580916913995415:0.013647930365035737:0.012313135409237473:0.011776021160717033:0.9496819961510143:"0.012580916913995415:0.013647930365035737:0.012313135409237473:0.011776021160717033:0.9496819961510143:'0.012580916913995415:0.013647930365035737:0.012313135409237473:0.011776021160717033:0.9496819961510143'"</t>
-  </si>
-  <si>
-    <t>0.1797578576761459:0.08087059903348022:0.09418509128847868:0.5737293034264526:0.07145714857544264:"0.1797578576761459:0.08087059903348022:0.09418509128847868:0.5737293034264526:0.07145714857544264:'0.1797578576761459:0.08087059903348022:0.09418509128847868:0.5737293034264526:0.07145714857544264'"</t>
-  </si>
-  <si>
-    <t>0.8784777661468466:0.006370503431624358:0.04859964178467366:0.028206730676399738:0.03834535796045566:'0.8784777661468466:0.006370503431624358:0.04859964178467366:0.028206730676399738:0.03834535796045566:"0.8784777661468466:0.006370503431624358:0.04859964178467366:0.028206730676399738:0.03834535796045566:\'0.8784777661468466:0.006370503431624358:0.04859964178467366:0.028206730676399738:0.03834535796045566\'"'</t>
-  </si>
-  <si>
-    <t>0.5788884213912752:0.1148213613226778:0.07098608081635895:0.2342593506406826:0.0010447858290055308:'0.5788884213912752:0.1148213613226778:0.07098608081635895:0.2342593506406826:0.0010447858290055308:"0.5788884213912752:0.1148213613226778:0.07098608081635895:0.2342593506406826:0.0010447858290055308:\'0.5788884213912752:0.1148213613226778:0.07098608081635895:0.2342593506406826:0.0010447858290055308\'"'</t>
-  </si>
-  <si>
-    <t>0.1045832742016494:0.2739786511896807:0.04193551102332393:0.4496555852728088:0.1298469783125372:'0.1045832742016494:0.2739786511896807:0.04193551102332393:0.4496555852728088:0.1298469783125372:"0.1045832742016494:0.2739786511896807:0.04193551102332393:0.4496555852728088:0.1298469783125372:\'0.1045832742016494:0.2739786511896807:0.04193551102332393:0.4496555852728088:0.1298469783125372\'"'</t>
-  </si>
-  <si>
-    <t>0.46969157849230714:0.03744275801747336:0.16899734942148248:0.09394011306381288:0.22992820100492414:'0.46969157849230714:0.03744275801747336:0.16899734942148248:0.09394011306381288:0.22992820100492414:"0.46969157849230714:0.03744275801747336:0.16899734942148248:0.09394011306381288:0.22992820100492414:\'0.46969157849230714:0.03744275801747336:0.16899734942148248:0.09394011306381288:0.22992820100492414\'"'</t>
-  </si>
-  <si>
-    <t>0.3957114651979722:0.12655103364603323:0.21722155723607658:0.06003495743759002:0.20048098648232784:'0.3957114651979722:0.12655103364603323:0.21722155723607658:0.06003495743759002:0.20048098648232784:"0.3957114651979722:0.12655103364603323:0.21722155723607658:0.06003495743759002:0.20048098648232784:\'0.3957114651979722:0.12655103364603323:0.21722155723607658:0.06003495743759002:0.20048098648232784\'"'</t>
-  </si>
-  <si>
-    <t>0.6379849661155549:0.12237712616089151:0.07293784141940536:0.039180538245610075:0.12751952805853817:'0.6379849661155549:0.12237712616089151:0.07293784141940536:0.039180538245610075:0.12751952805853817:"0.6379849661155549:0.12237712616089151:0.07293784141940536:0.039180538245610075:0.12751952805853817:\'0.6379849661155549:0.12237712616089151:0.07293784141940536:0.039180538245610075:0.12751952805853817\'"'</t>
-  </si>
-  <si>
-    <t>0.6919501954151895:0.15649884726812238:0.08597952671094426:0.007373107703755164:0.05819832290198865:'0.6919501954151895:0.15649884726812238:0.08597952671094426:0.007373107703755164:0.05819832290198865:"0.6919501954151895:0.15649884726812238:0.08597952671094426:0.007373107703755164:0.05819832290198865:\'0.6919501954151895:0.15649884726812238:0.08597952671094426:0.007373107703755164:0.05819832290198865\'"'</t>
-  </si>
-  <si>
-    <t>0.341735955717008:0.26218025344058743:0.2391269771185358:0.11980515008466874:0.0371516636392:'0.341735955717008:0.26218025344058743:0.2391269771185358:0.11980515008466874:0.0371516636392:"0.341735955717008:0.26218025344058743:0.2391269771185358:0.11980515008466874:0.0371516636392:\'0.341735955717008:0.26218025344058743:0.2391269771185358:0.11980515008466874:0.0371516636392\'"'</t>
-  </si>
-  <si>
-    <t>0.5478035918166799:0.17297868951796821:0.0038734044236464053:0.15141123544969604:0.1239330787920094:'0.5478035918166799:0.17297868951796821:0.0038734044236464053:0.15141123544969604:0.1239330787920094:"0.5478035918166799:0.17297868951796821:0.0038734044236464053:0.15141123544969604:0.1239330787920094:\'0.5478035918166799:0.17297868951796821:0.0038734044236464053:0.15141123544969604:0.1239330787920094\'"'</t>
-  </si>
-  <si>
-    <t>0.24233858495952668:0.3071458935191035:0.13511293658740064:0.06436706646403009:0.25103551846993916:'0.24233858495952668:0.3071458935191035:0.13511293658740064:0.06436706646403009:0.25103551846993916:"0.24233858495952668:0.3071458935191035:0.13511293658740064:0.06436706646403009:0.25103551846993916:\'0.24233858495952668:0.3071458935191035:0.13511293658740064:0.06436706646403009:0.25103551846993916\'"'</t>
-  </si>
-  <si>
-    <t>0.9964069679491023:0.0008499840013651758:0.0010790274898496441:0.001230791211281703:0.00043322934840114803:'0.9964069679491023:0.0008499840013651758:0.0010790274898496441:0.001230791211281703:0.00043322934840114803:"0.9964069679491023:0.0008499840013651758:0.0010790274898496441:0.001230791211281703:0.00043322934840114803:\'0.9964069679491023:0.0008499840013651758:0.0010790274898496441:0.001230791211281703:0.00043322934840114803\'"'</t>
-  </si>
-  <si>
-    <t>0.2580814265398616:0.074537560053405:0.23377596013418603:0.21868577765632807:0.21491927561621915:'0.2580814265398616:0.074537560053405:0.23377596013418603:0.21868577765632807:0.21491927561621915:"0.2580814265398616:0.074537560053405:0.23377596013418603:0.21868577765632807:0.21491927561621915:\'0.2580814265398616:0.074537560053405:0.23377596013418603:0.21868577765632807:0.21491927561621915\'"'</t>
-  </si>
-  <si>
-    <t>0.17438907388885735:0.0038831449836855747:0.2570750647234156:0.34538605480971696:0.21926666159432445:'0.17438907388885735:0.0038831449836855747:0.2570750647234156:0.34538605480971696:0.21926666159432445:"0.17438907388885735:0.0038831449836855747:0.2570750647234156:0.34538605480971696:0.21926666159432445:\'0.17438907388885735:0.0038831449836855747:0.2570750647234156:0.34538605480971696:0.21926666159432445\'"'</t>
-  </si>
-  <si>
-    <t>0.7656895374345389:0.10000252830735035:0.05411212378682602:0.040184273334564105:0.040011537136720614:'0.7656895374345389:0.10000252830735035:0.05411212378682602:0.040184273334564105:0.040011537136720614:"0.7656895374345389:0.10000252830735035:0.05411212378682602:0.040184273334564105:0.040011537136720614:\'0.7656895374345389:0.10000252830735035:0.05411212378682602:0.040184273334564105:0.040011537136720614\'"'</t>
-  </si>
-  <si>
-    <t>0.7462431889969952:0.05009674706362561:0.08270077476439788:0.0405067293390163:0.08045255983596511:'0.7462431889969952:0.05009674706362561:0.08270077476439788:0.0405067293390163:0.08045255983596511:"0.7462431889969952:0.05009674706362561:0.08270077476439788:0.0405067293390163:0.08045255983596511:\'0.7462431889969952:0.05009674706362561:0.08270077476439788:0.0405067293390163:0.08045255983596511\'"'</t>
-  </si>
-  <si>
-    <t>0.8165026538916844:0.043478271812166396:0.04165595053028977:0.06006448699021291:0.038298636775646516:'0.8165026538916844:0.043478271812166396:0.04165595053028977:0.06006448699021291:0.038298636775646516:"0.8165026538916844:0.043478271812166396:0.04165595053028977:0.06006448699021291:0.038298636775646516:\'0.8165026538916844:0.043478271812166396:0.04165595053028977:0.06006448699021291:0.038298636775646516\'"'</t>
-  </si>
-  <si>
-    <t>0.048691367112449924:0.14037800101418405:0.3252409319849474:0.19884286680342372:0.2868468330849948:'0.048691367112449924:0.14037800101418405:0.3252409319849474:0.19884286680342372:0.2868468330849948:"0.048691367112449924:0.14037800101418405:0.3252409319849474:0.19884286680342372:0.2868468330849948:\'0.048691367112449924:0.14037800101418405:0.3252409319849474:0.19884286680342372:0.2868468330849948\'"'</t>
-  </si>
-  <si>
-    <t>0.41688949152990207:0.267275179454366:0.04723230298522335:0.24410864883377942:0.024494377196729145:'0.41688949152990207:0.267275179454366:0.04723230298522335:0.24410864883377942:0.024494377196729145:"0.41688949152990207:0.267275179454366:0.04723230298522335:0.24410864883377942:0.024494377196729145:\'0.41688949152990207:0.267275179454366:0.04723230298522335:0.24410864883377942:0.024494377196729145\'"'</t>
-  </si>
-  <si>
-    <t>0.9496819961510143:0.012580916913995415:0.013647930365035737:0.012313135409237473:0.011776021160717033:'0.9496819961510143:0.012580916913995415:0.013647930365035737:0.012313135409237473:0.011776021160717033:"0.9496819961510143:0.012580916913995415:0.013647930365035737:0.012313135409237473:0.011776021160717033:\'0.9496819961510143:0.012580916913995415:0.013647930365035737:0.012313135409237473:0.011776021160717033\'"'</t>
-  </si>
-  <si>
-    <t>0.07145714857544264:0.1797578576761459:0.08087059903348022:0.09418509128847868:0.5737293034264526:'0.07145714857544264:0.1797578576761459:0.08087059903348022:0.09418509128847868:0.5737293034264526:"0.07145714857544264:0.1797578576761459:0.08087059903348022:0.09418509128847868:0.5737293034264526:\'0.07145714857544264:0.1797578576761459:0.08087059903348022:0.09418509128847868:0.5737293034264526\'"'</t>
-  </si>
-  <si>
-    <t>0.03834535796045566:0.8784777661468466:0.006370503431624358:0.04859964178467366:0.028206730676399738:'0.03834535796045566:0.8784777661468466:0.006370503431624358:0.04859964178467366:0.028206730676399738:"0.03834535796045566:0.8784777661468466:0.006370503431624358:0.04859964178467366:0.028206730676399738:\'0.03834535796045566:0.8784777661468466:0.006370503431624358:0.04859964178467366:0.028206730676399738\'"'</t>
-  </si>
-  <si>
-    <t>0.0010447858290055308:0.5788884213912752:0.1148213613226778:0.07098608081635895:0.2342593506406826:'0.0010447858290055308:0.5788884213912752:0.1148213613226778:0.07098608081635895:0.2342593506406826:"0.0010447858290055308:0.5788884213912752:0.1148213613226778:0.07098608081635895:0.2342593506406826:\'0.0010447858290055308:0.5788884213912752:0.1148213613226778:0.07098608081635895:0.2342593506406826\'"'</t>
-  </si>
-  <si>
-    <t>0.1298469783125372:0.1045832742016494:0.2739786511896807:0.04193551102332393:0.4496555852728088:'0.1298469783125372:0.1045832742016494:0.2739786511896807:0.04193551102332393:0.4496555852728088:"0.1298469783125372:0.1045832742016494:0.2739786511896807:0.04193551102332393:0.4496555852728088:\'0.1298469783125372:0.1045832742016494:0.2739786511896807:0.04193551102332393:0.4496555852728088\'"'</t>
-  </si>
-  <si>
-    <t>0.22992820100492414:0.46969157849230714:0.03744275801747336:0.16899734942148248:0.09394011306381288:'0.22992820100492414:0.46969157849230714:0.03744275801747336:0.16899734942148248:0.09394011306381288:"0.22992820100492414:0.46969157849230714:0.03744275801747336:0.16899734942148248:0.09394011306381288:\'0.22992820100492414:0.46969157849230714:0.03744275801747336:0.16899734942148248:0.09394011306381288\'"'</t>
-  </si>
-  <si>
-    <t>0.20048098648232784:0.3957114651979722:0.12655103364603323:0.21722155723607658:0.06003495743759002:'0.20048098648232784:0.3957114651979722:0.12655103364603323:0.21722155723607658:0.06003495743759002:"0.20048098648232784:0.3957114651979722:0.12655103364603323:0.21722155723607658:0.06003495743759002:\'0.20048098648232784:0.3957114651979722:0.12655103364603323:0.21722155723607658:0.06003495743759002\'"'</t>
-  </si>
-  <si>
-    <t>0.12751952805853817:0.6379849661155549:0.12237712616089151:0.07293784141940536:0.039180538245610075:'0.12751952805853817:0.6379849661155549:0.12237712616089151:0.07293784141940536:0.039180538245610075:"0.12751952805853817:0.6379849661155549:0.12237712616089151:0.07293784141940536:0.039180538245610075:\'0.12751952805853817:0.6379849661155549:0.12237712616089151:0.07293784141940536:0.039180538245610075\'"'</t>
-  </si>
-  <si>
-    <t>0.05819832290198865:0.6919501954151895:0.15649884726812238:0.08597952671094426:0.007373107703755164:'0.05819832290198865:0.6919501954151895:0.15649884726812238:0.08597952671094426:0.007373107703755164:"0.05819832290198865:0.6919501954151895:0.15649884726812238:0.08597952671094426:0.007373107703755164:\'0.05819832290198865:0.6919501954151895:0.15649884726812238:0.08597952671094426:0.007373107703755164\'"'</t>
-  </si>
-  <si>
-    <t>0.0371516636392:0.341735955717008:0.26218025344058743:0.2391269771185358:0.11980515008466874:'0.0371516636392:0.341735955717008:0.26218025344058743:0.2391269771185358:0.11980515008466874:"0.0371516636392:0.341735955717008:0.26218025344058743:0.2391269771185358:0.11980515008466874:\'0.0371516636392:0.341735955717008:0.26218025344058743:0.2391269771185358:0.11980515008466874\'"'</t>
-  </si>
-  <si>
-    <t>0.1239330787920094:0.5478035918166799:0.17297868951796821:0.0038734044236464053:0.15141123544969604:'0.1239330787920094:0.5478035918166799:0.17297868951796821:0.0038734044236464053:0.15141123544969604:"0.1239330787920094:0.5478035918166799:0.17297868951796821:0.0038734044236464053:0.15141123544969604:\'0.1239330787920094:0.5478035918166799:0.17297868951796821:0.0038734044236464053:0.15141123544969604\'"'</t>
-  </si>
-  <si>
-    <t>0.25103551846993916:0.24233858495952668:0.3071458935191035:0.13511293658740064:0.06436706646403009:'0.25103551846993916:0.24233858495952668:0.3071458935191035:0.13511293658740064:0.06436706646403009:"0.25103551846993916:0.24233858495952668:0.3071458935191035:0.13511293658740064:0.06436706646403009:\'0.25103551846993916:0.24233858495952668:0.3071458935191035:0.13511293658740064:0.06436706646403009\'"'</t>
-  </si>
-  <si>
-    <t>0.00043322934840114803:0.9964069679491023:0.0008499840013651758:0.0010790274898496441:0.001230791211281703:'0.00043322934840114803:0.9964069679491023:0.0008499840013651758:0.0010790274898496441:0.001230791211281703:"0.00043322934840114803:0.9964069679491023:0.0008499840013651758:0.0010790274898496441:0.001230791211281703:\'0.00043322934840114803:0.9964069679491023:0.0008499840013651758:0.0010790274898496441:0.001230791211281703\'"'</t>
-  </si>
-  <si>
-    <t>0.21491927561621915:0.2580814265398616:0.074537560053405:0.23377596013418603:0.21868577765632807:'0.21491927561621915:0.2580814265398616:0.074537560053405:0.23377596013418603:0.21868577765632807:"0.21491927561621915:0.2580814265398616:0.074537560053405:0.23377596013418603:0.21868577765632807:\'0.21491927561621915:0.2580814265398616:0.074537560053405:0.23377596013418603:0.21868577765632807\'"'</t>
-  </si>
-  <si>
-    <t>0.21926666159432445:0.17438907388885735:0.0038831449836855747:0.2570750647234156:0.34538605480971696:'0.21926666159432445:0.17438907388885735:0.0038831449836855747:0.2570750647234156:0.34538605480971696:"0.21926666159432445:0.17438907388885735:0.0038831449836855747:0.2570750647234156:0.34538605480971696:\'0.21926666159432445:0.17438907388885735:0.0038831449836855747:0.2570750647234156:0.34538605480971696\'"'</t>
-  </si>
-  <si>
-    <t>0.040011537136720614:0.7656895374345389:0.10000252830735035:0.05411212378682602:0.040184273334564105:'0.040011537136720614:0.7656895374345389:0.10000252830735035:0.05411212378682602:0.040184273334564105:"0.040011537136720614:0.7656895374345389:0.10000252830735035:0.05411212378682602:0.040184273334564105:\'0.040011537136720614:0.7656895374345389:0.10000252830735035:0.05411212378682602:0.040184273334564105\'"'</t>
-  </si>
-  <si>
-    <t>0.08045255983596511:0.7462431889969952:0.05009674706362561:0.08270077476439788:0.0405067293390163:'0.08045255983596511:0.7462431889969952:0.05009674706362561:0.08270077476439788:0.0405067293390163:"0.08045255983596511:0.7462431889969952:0.05009674706362561:0.08270077476439788:0.0405067293390163:\'0.08045255983596511:0.7462431889969952:0.05009674706362561:0.08270077476439788:0.0405067293390163\'"'</t>
-  </si>
-  <si>
-    <t>0.038298636775646516:0.8165026538916844:0.043478271812166396:0.04165595053028977:0.06006448699021291:'0.038298636775646516:0.8165026538916844:0.043478271812166396:0.04165595053028977:0.06006448699021291:"0.038298636775646516:0.8165026538916844:0.043478271812166396:0.04165595053028977:0.06006448699021291:\'0.038298636775646516:0.8165026538916844:0.043478271812166396:0.04165595053028977:0.06006448699021291\'"'</t>
-  </si>
-  <si>
-    <t>0.2868468330849948:0.048691367112449924:0.14037800101418405:0.3252409319849474:0.19884286680342372:'0.2868468330849948:0.048691367112449924:0.14037800101418405:0.3252409319849474:0.19884286680342372:"0.2868468330849948:0.048691367112449924:0.14037800101418405:0.3252409319849474:0.19884286680342372:\'0.2868468330849948:0.048691367112449924:0.14037800101418405:0.3252409319849474:0.19884286680342372\'"'</t>
-  </si>
-  <si>
-    <t>0.024494377196729145:0.41688949152990207:0.267275179454366:0.04723230298522335:0.24410864883377942:'0.024494377196729145:0.41688949152990207:0.267275179454366:0.04723230298522335:0.24410864883377942:"0.024494377196729145:0.41688949152990207:0.267275179454366:0.04723230298522335:0.24410864883377942:\'0.024494377196729145:0.41688949152990207:0.267275179454366:0.04723230298522335:0.24410864883377942\'"'</t>
-  </si>
-  <si>
-    <t>0.011776021160717033:0.9496819961510143:0.012580916913995415:0.013647930365035737:0.012313135409237473:'0.011776021160717033:0.9496819961510143:0.012580916913995415:0.013647930365035737:0.012313135409237473:"0.011776021160717033:0.9496819961510143:0.012580916913995415:0.013647930365035737:0.012313135409237473:\'0.011776021160717033:0.9496819961510143:0.012580916913995415:0.013647930365035737:0.012313135409237473\'"'</t>
-  </si>
-  <si>
-    <t>0.5737293034264526:0.07145714857544264:0.1797578576761459:0.08087059903348022:0.09418509128847868:'0.5737293034264526:0.07145714857544264:0.1797578576761459:0.08087059903348022:0.09418509128847868:"0.5737293034264526:0.07145714857544264:0.1797578576761459:0.08087059903348022:0.09418509128847868:\'0.5737293034264526:0.07145714857544264:0.1797578576761459:0.08087059903348022:0.09418509128847868\'"'</t>
-  </si>
-  <si>
-    <t>0.028206730676399738:0.03834535796045566:0.8784777661468466:0.006370503431624358:0.04859964178467366:'0.028206730676399738:0.03834535796045566:0.8784777661468466:0.006370503431624358:0.04859964178467366:"0.028206730676399738:0.03834535796045566:0.8784777661468466:0.006370503431624358:0.04859964178467366:\'0.028206730676399738:0.03834535796045566:0.8784777661468466:0.006370503431624358:0.04859964178467366\'"'</t>
-  </si>
-  <si>
-    <t>0.2342593506406826:0.0010447858290055308:0.5788884213912752:0.1148213613226778:0.07098608081635895:'0.2342593506406826:0.0010447858290055308:0.5788884213912752:0.1148213613226778:0.07098608081635895:"0.2342593506406826:0.0010447858290055308:0.5788884213912752:0.1148213613226778:0.07098608081635895:\'0.2342593506406826:0.0010447858290055308:0.5788884213912752:0.1148213613226778:0.07098608081635895\'"'</t>
-  </si>
-  <si>
-    <t>0.4496555852728088:0.1298469783125372:0.1045832742016494:0.2739786511896807:0.04193551102332393:'0.4496555852728088:0.1298469783125372:0.1045832742016494:0.2739786511896807:0.04193551102332393:"0.4496555852728088:0.1298469783125372:0.1045832742016494:0.2739786511896807:0.04193551102332393:\'0.4496555852728088:0.1298469783125372:0.1045832742016494:0.2739786511896807:0.04193551102332393\'"'</t>
-  </si>
-  <si>
-    <t>0.09394011306381288:0.22992820100492414:0.46969157849230714:0.03744275801747336:0.16899734942148248:'0.09394011306381288:0.22992820100492414:0.46969157849230714:0.03744275801747336:0.16899734942148248:"0.09394011306381288:0.22992820100492414:0.46969157849230714:0.03744275801747336:0.16899734942148248:\'0.09394011306381288:0.22992820100492414:0.46969157849230714:0.03744275801747336:0.16899734942148248\'"'</t>
-  </si>
-  <si>
-    <t>0.06003495743759002:0.20048098648232784:0.3957114651979722:0.12655103364603323:0.21722155723607658:'0.06003495743759002:0.20048098648232784:0.3957114651979722:0.12655103364603323:0.21722155723607658:"0.06003495743759002:0.20048098648232784:0.3957114651979722:0.12655103364603323:0.21722155723607658:\'0.06003495743759002:0.20048098648232784:0.3957114651979722:0.12655103364603323:0.21722155723607658\'"'</t>
-  </si>
-  <si>
-    <t>0.039180538245610075:0.12751952805853817:0.6379849661155549:0.12237712616089151:0.07293784141940536:'0.039180538245610075:0.12751952805853817:0.6379849661155549:0.12237712616089151:0.07293784141940536:"0.039180538245610075:0.12751952805853817:0.6379849661155549:0.12237712616089151:0.07293784141940536:\'0.039180538245610075:0.12751952805853817:0.6379849661155549:0.12237712616089151:0.07293784141940536\'"'</t>
-  </si>
-  <si>
-    <t>0.007373107703755164:0.05819832290198865:0.6919501954151895:0.15649884726812238:0.08597952671094426:'0.007373107703755164:0.05819832290198865:0.6919501954151895:0.15649884726812238:0.08597952671094426:"0.007373107703755164:0.05819832290198865:0.6919501954151895:0.15649884726812238:0.08597952671094426:\'0.007373107703755164:0.05819832290198865:0.6919501954151895:0.15649884726812238:0.08597952671094426\'"'</t>
-  </si>
-  <si>
-    <t>0.11980515008466874:0.0371516636392:0.341735955717008:0.26218025344058743:0.2391269771185358:'0.11980515008466874:0.0371516636392:0.341735955717008:0.26218025344058743:0.2391269771185358:"0.11980515008466874:0.0371516636392:0.341735955717008:0.26218025344058743:0.2391269771185358:\'0.11980515008466874:0.0371516636392:0.341735955717008:0.26218025344058743:0.2391269771185358\'"'</t>
-  </si>
-  <si>
-    <t>0.15141123544969604:0.1239330787920094:0.5478035918166799:0.17297868951796821:0.0038734044236464053:'0.15141123544969604:0.1239330787920094:0.5478035918166799:0.17297868951796821:0.0038734044236464053:"0.15141123544969604:0.1239330787920094:0.5478035918166799:0.17297868951796821:0.0038734044236464053:\'0.15141123544969604:0.1239330787920094:0.5478035918166799:0.17297868951796821:0.0038734044236464053\'"'</t>
-  </si>
-  <si>
-    <t>0.06436706646403009:0.25103551846993916:0.24233858495952668:0.3071458935191035:0.13511293658740064:'0.06436706646403009:0.25103551846993916:0.24233858495952668:0.3071458935191035:0.13511293658740064:"0.06436706646403009:0.25103551846993916:0.24233858495952668:0.3071458935191035:0.13511293658740064:\'0.06436706646403009:0.25103551846993916:0.24233858495952668:0.3071458935191035:0.13511293658740064\'"'</t>
-  </si>
-  <si>
-    <t>0.001230791211281703:0.00043322934840114803:0.9964069679491023:0.0008499840013651758:0.0010790274898496441:'0.001230791211281703:0.00043322934840114803:0.9964069679491023:0.0008499840013651758:0.0010790274898496441:"0.001230791211281703:0.00043322934840114803:0.9964069679491023:0.0008499840013651758:0.0010790274898496441:\'0.001230791211281703:0.00043322934840114803:0.9964069679491023:0.0008499840013651758:0.0010790274898496441\'"'</t>
-  </si>
-  <si>
-    <t>0.21868577765632807:0.21491927561621915:0.2580814265398616:0.074537560053405:0.23377596013418603:'0.21868577765632807:0.21491927561621915:0.2580814265398616:0.074537560053405:0.23377596013418603:"0.21868577765632807:0.21491927561621915:0.2580814265398616:0.074537560053405:0.23377596013418603:\'0.21868577765632807:0.21491927561621915:0.2580814265398616:0.074537560053405:0.23377596013418603\'"'</t>
-  </si>
-  <si>
-    <t>0.34538605480971696:0.21926666159432445:0.17438907388885735:0.0038831449836855747:0.2570750647234156:'0.34538605480971696:0.21926666159432445:0.17438907388885735:0.0038831449836855747:0.2570750647234156:"0.34538605480971696:0.21926666159432445:0.17438907388885735:0.0038831449836855747:0.2570750647234156:\'0.34538605480971696:0.21926666159432445:0.17438907388885735:0.0038831449836855747:0.2570750647234156\'"'</t>
-  </si>
-  <si>
-    <t>0.040184273334564105:0.040011537136720614:0.7656895374345389:0.10000252830735035:0.05411212378682602:'0.040184273334564105:0.040011537136720614:0.7656895374345389:0.10000252830735035:0.05411212378682602:"0.040184273334564105:0.040011537136720614:0.7656895374345389:0.10000252830735035:0.05411212378682602:\'0.040184273334564105:0.040011537136720614:0.7656895374345389:0.10000252830735035:0.05411212378682602\'"'</t>
-  </si>
-  <si>
-    <t>0.0405067293390163:0.08045255983596511:0.7462431889969952:0.05009674706362561:0.08270077476439788:'0.0405067293390163:0.08045255983596511:0.7462431889969952:0.05009674706362561:0.08270077476439788:"0.0405067293390163:0.08045255983596511:0.7462431889969952:0.05009674706362561:0.08270077476439788:\'0.0405067293390163:0.08045255983596511:0.7462431889969952:0.05009674706362561:0.08270077476439788\'"'</t>
-  </si>
-  <si>
-    <t>0.06006448699021291:0.038298636775646516:0.8165026538916844:0.043478271812166396:0.04165595053028977:'0.06006448699021291:0.038298636775646516:0.8165026538916844:0.043478271812166396:0.04165595053028977:"0.06006448699021291:0.038298636775646516:0.8165026538916844:0.043478271812166396:0.04165595053028977:\'0.06006448699021291:0.038298636775646516:0.8165026538916844:0.043478271812166396:0.04165595053028977\'"'</t>
-  </si>
-  <si>
-    <t>0.19884286680342372:0.2868468330849948:0.048691367112449924:0.14037800101418405:0.3252409319849474:'0.19884286680342372:0.2868468330849948:0.048691367112449924:0.14037800101418405:0.3252409319849474:"0.19884286680342372:0.2868468330849948:0.048691367112449924:0.14037800101418405:0.3252409319849474:\'0.19884286680342372:0.2868468330849948:0.048691367112449924:0.14037800101418405:0.3252409319849474\'"'</t>
-  </si>
-  <si>
-    <t>0.24410864883377942:0.024494377196729145:0.41688949152990207:0.267275179454366:0.04723230298522335:'0.24410864883377942:0.024494377196729145:0.41688949152990207:0.267275179454366:0.04723230298522335:"0.24410864883377942:0.024494377196729145:0.41688949152990207:0.267275179454366:0.04723230298522335:\'0.24410864883377942:0.024494377196729145:0.41688949152990207:0.267275179454366:0.04723230298522335\'"'</t>
-  </si>
-  <si>
-    <t>0.012313135409237473:0.011776021160717033:0.9496819961510143:0.012580916913995415:0.013647930365035737:'0.012313135409237473:0.011776021160717033:0.9496819961510143:0.012580916913995415:0.013647930365035737:"0.012313135409237473:0.011776021160717033:0.9496819961510143:0.012580916913995415:0.013647930365035737:\'0.012313135409237473:0.011776021160717033:0.9496819961510143:0.012580916913995415:0.013647930365035737\'"'</t>
-  </si>
-  <si>
-    <t>0.09418509128847868:0.5737293034264526:0.07145714857544264:0.1797578576761459:0.08087059903348022:'0.09418509128847868:0.5737293034264526:0.07145714857544264:0.1797578576761459:0.08087059903348022:"0.09418509128847868:0.5737293034264526:0.07145714857544264:0.1797578576761459:0.08087059903348022:\'0.09418509128847868:0.5737293034264526:0.07145714857544264:0.1797578576761459:0.08087059903348022\'"'</t>
-  </si>
-  <si>
-    <t>0.04859964178467366:0.028206730676399738:0.03834535796045566:0.8784777661468466:0.006370503431624358:'0.04859964178467366:0.028206730676399738:0.03834535796045566:0.8784777661468466:0.006370503431624358:"0.04859964178467366:0.028206730676399738:0.03834535796045566:0.8784777661468466:0.006370503431624358:\'0.04859964178467366:0.028206730676399738:0.03834535796045566:0.8784777661468466:0.006370503431624358\'"'</t>
-  </si>
-  <si>
-    <t>0.07098608081635895:0.2342593506406826:0.0010447858290055308:0.5788884213912752:0.1148213613226778:'0.07098608081635895:0.2342593506406826:0.0010447858290055308:0.5788884213912752:0.1148213613226778:"0.07098608081635895:0.2342593506406826:0.0010447858290055308:0.5788884213912752:0.1148213613226778:\'0.07098608081635895:0.2342593506406826:0.0010447858290055308:0.5788884213912752:0.1148213613226778\'"'</t>
-  </si>
-  <si>
-    <t>0.04193551102332393:0.4496555852728088:0.1298469783125372:0.1045832742016494:0.2739786511896807:'0.04193551102332393:0.4496555852728088:0.1298469783125372:0.1045832742016494:0.2739786511896807:"0.04193551102332393:0.4496555852728088:0.1298469783125372:0.1045832742016494:0.2739786511896807:\'0.04193551102332393:0.4496555852728088:0.1298469783125372:0.1045832742016494:0.2739786511896807\'"'</t>
-  </si>
-  <si>
-    <t>0.16899734942148248:0.09394011306381288:0.22992820100492414:0.46969157849230714:0.03744275801747336:'0.16899734942148248:0.09394011306381288:0.22992820100492414:0.46969157849230714:0.03744275801747336:"0.16899734942148248:0.09394011306381288:0.22992820100492414:0.46969157849230714:0.03744275801747336:\'0.16899734942148248:0.09394011306381288:0.22992820100492414:0.46969157849230714:0.03744275801747336\'"'</t>
-  </si>
-  <si>
-    <t>0.21722155723607658:0.06003495743759002:0.20048098648232784:0.3957114651979722:0.12655103364603323:'0.21722155723607658:0.06003495743759002:0.20048098648232784:0.3957114651979722:0.12655103364603323:"0.21722155723607658:0.06003495743759002:0.20048098648232784:0.3957114651979722:0.12655103364603323:\'0.21722155723607658:0.06003495743759002:0.20048098648232784:0.3957114651979722:0.12655103364603323\'"'</t>
-  </si>
-  <si>
-    <t>0.07293784141940536:0.039180538245610075:0.12751952805853817:0.6379849661155549:0.12237712616089151:'0.07293784141940536:0.039180538245610075:0.12751952805853817:0.6379849661155549:0.12237712616089151:"0.07293784141940536:0.039180538245610075:0.12751952805853817:0.6379849661155549:0.12237712616089151:\'0.07293784141940536:0.039180538245610075:0.12751952805853817:0.6379849661155549:0.12237712616089151\'"'</t>
-  </si>
-  <si>
-    <t>0.08597952671094426:0.007373107703755164:0.05819832290198865:0.6919501954151895:0.15649884726812238:'0.08597952671094426:0.007373107703755164:0.05819832290198865:0.6919501954151895:0.15649884726812238:"0.08597952671094426:0.007373107703755164:0.05819832290198865:0.6919501954151895:0.15649884726812238:\'0.08597952671094426:0.007373107703755164:0.05819832290198865:0.6919501954151895:0.15649884726812238\'"'</t>
-  </si>
-  <si>
-    <t>0.2391269771185358:0.11980515008466874:0.0371516636392:0.341735955717008:0.26218025344058743:'0.2391269771185358:0.11980515008466874:0.0371516636392:0.341735955717008:0.26218025344058743:"0.2391269771185358:0.11980515008466874:0.0371516636392:0.341735955717008:0.26218025344058743:\'0.2391269771185358:0.11980515008466874:0.0371516636392:0.341735955717008:0.26218025344058743\'"'</t>
-  </si>
-  <si>
-    <t>0.0038734044236464053:0.15141123544969604:0.1239330787920094:0.5478035918166799:0.17297868951796821:'0.0038734044236464053:0.15141123544969604:0.1239330787920094:0.5478035918166799:0.17297868951796821:"0.0038734044236464053:0.15141123544969604:0.1239330787920094:0.5478035918166799:0.17297868951796821:\'0.0038734044236464053:0.15141123544969604:0.1239330787920094:0.5478035918166799:0.17297868951796821\'"'</t>
-  </si>
-  <si>
-    <t>0.13511293658740064:0.06436706646403009:0.25103551846993916:0.24233858495952668:0.3071458935191035:'0.13511293658740064:0.06436706646403009:0.25103551846993916:0.24233858495952668:0.3071458935191035:"0.13511293658740064:0.06436706646403009:0.25103551846993916:0.24233858495952668:0.3071458935191035:\'0.13511293658740064:0.06436706646403009:0.25103551846993916:0.24233858495952668:0.3071458935191035\'"'</t>
-  </si>
-  <si>
-    <t>0.0010790274898496441:0.001230791211281703:0.00043322934840114803:0.9964069679491023:0.0008499840013651758:'0.0010790274898496441:0.001230791211281703:0.00043322934840114803:0.9964069679491023:0.0008499840013651758:"0.0010790274898496441:0.001230791211281703:0.00043322934840114803:0.9964069679491023:0.0008499840013651758:\'0.0010790274898496441:0.001230791211281703:0.00043322934840114803:0.9964069679491023:0.0008499840013651758\'"'</t>
-  </si>
-  <si>
-    <t>0.23377596013418603:0.21868577765632807:0.21491927561621915:0.2580814265398616:0.074537560053405:'0.23377596013418603:0.21868577765632807:0.21491927561621915:0.2580814265398616:0.074537560053405:"0.23377596013418603:0.21868577765632807:0.21491927561621915:0.2580814265398616:0.074537560053405:\'0.23377596013418603:0.21868577765632807:0.21491927561621915:0.2580814265398616:0.074537560053405\'"'</t>
-  </si>
-  <si>
-    <t>0.2570750647234156:0.34538605480971696:0.21926666159432445:0.17438907388885735:0.0038831449836855747:'0.2570750647234156:0.34538605480971696:0.21926666159432445:0.17438907388885735:0.0038831449836855747:"0.2570750647234156:0.34538605480971696:0.21926666159432445:0.17438907388885735:0.0038831449836855747:\'0.2570750647234156:0.34538605480971696:0.21926666159432445:0.17438907388885735:0.0038831449836855747\'"'</t>
-  </si>
-  <si>
-    <t>0.05411212378682602:0.040184273334564105:0.040011537136720614:0.7656895374345389:0.10000252830735035:'0.05411212378682602:0.040184273334564105:0.040011537136720614:0.7656895374345389:0.10000252830735035:"0.05411212378682602:0.040184273334564105:0.040011537136720614:0.7656895374345389:0.10000252830735035:\'0.05411212378682602:0.040184273334564105:0.040011537136720614:0.7656895374345389:0.10000252830735035\'"'</t>
-  </si>
-  <si>
-    <t>0.08270077476439788:0.0405067293390163:0.08045255983596511:0.7462431889969952:0.05009674706362561:'0.08270077476439788:0.0405067293390163:0.08045255983596511:0.7462431889969952:0.05009674706362561:"0.08270077476439788:0.0405067293390163:0.08045255983596511:0.7462431889969952:0.05009674706362561:\'0.08270077476439788:0.0405067293390163:0.08045255983596511:0.7462431889969952:0.05009674706362561\'"'</t>
-  </si>
-  <si>
-    <t>0.04165595053028977:0.06006448699021291:0.038298636775646516:0.8165026538916844:0.043478271812166396:'0.04165595053028977:0.06006448699021291:0.038298636775646516:0.8165026538916844:0.043478271812166396:"0.04165595053028977:0.06006448699021291:0.038298636775646516:0.8165026538916844:0.043478271812166396:\'0.04165595053028977:0.06006448699021291:0.038298636775646516:0.8165026538916844:0.043478271812166396\'"'</t>
-  </si>
-  <si>
-    <t>0.3252409319849474:0.19884286680342372:0.2868468330849948:0.048691367112449924:0.14037800101418405:'0.3252409319849474:0.19884286680342372:0.2868468330849948:0.048691367112449924:0.14037800101418405:"0.3252409319849474:0.19884286680342372:0.2868468330849948:0.048691367112449924:0.14037800101418405:\'0.3252409319849474:0.19884286680342372:0.2868468330849948:0.048691367112449924:0.14037800101418405\'"'</t>
-  </si>
-  <si>
-    <t>0.04723230298522335:0.24410864883377942:0.024494377196729145:0.41688949152990207:0.267275179454366:'0.04723230298522335:0.24410864883377942:0.024494377196729145:0.41688949152990207:0.267275179454366:"0.04723230298522335:0.24410864883377942:0.024494377196729145:0.41688949152990207:0.267275179454366:\'0.04723230298522335:0.24410864883377942:0.024494377196729145:0.41688949152990207:0.267275179454366\'"'</t>
-  </si>
-  <si>
-    <t>0.013647930365035737:0.012313135409237473:0.011776021160717033:0.9496819961510143:0.012580916913995415:'0.013647930365035737:0.012313135409237473:0.011776021160717033:0.9496819961510143:0.012580916913995415:"0.013647930365035737:0.012313135409237473:0.011776021160717033:0.9496819961510143:0.012580916913995415:\'0.013647930365035737:0.012313135409237473:0.011776021160717033:0.9496819961510143:0.012580916913995415\'"'</t>
-  </si>
-  <si>
-    <t>0.08087059903348022:0.09418509128847868:0.5737293034264526:0.07145714857544264:0.1797578576761459:'0.08087059903348022:0.09418509128847868:0.5737293034264526:0.07145714857544264:0.1797578576761459:"0.08087059903348022:0.09418509128847868:0.5737293034264526:0.07145714857544264:0.1797578576761459:\'0.08087059903348022:0.09418509128847868:0.5737293034264526:0.07145714857544264:0.1797578576761459\'"'</t>
-  </si>
-  <si>
-    <t>0.006370503431624358:0.04859964178467366:0.028206730676399738:0.03834535796045566:0.8784777661468466:'0.006370503431624358:0.04859964178467366:0.028206730676399738:0.03834535796045566:0.8784777661468466:"0.006370503431624358:0.04859964178467366:0.028206730676399738:0.03834535796045566:0.8784777661468466:\'0.006370503431624358:0.04859964178467366:0.028206730676399738:0.03834535796045566:0.8784777661468466\'"'</t>
-  </si>
-  <si>
-    <t>0.1148213613226778:0.07098608081635895:0.2342593506406826:0.0010447858290055308:0.5788884213912752:'0.1148213613226778:0.07098608081635895:0.2342593506406826:0.0010447858290055308:0.5788884213912752:"0.1148213613226778:0.07098608081635895:0.2342593506406826:0.0010447858290055308:0.5788884213912752:\'0.1148213613226778:0.07098608081635895:0.2342593506406826:0.0010447858290055308:0.5788884213912752\'"'</t>
-  </si>
-  <si>
-    <t>0.2739786511896807:0.04193551102332393:0.4496555852728088:0.1298469783125372:0.1045832742016494:'0.2739786511896807:0.04193551102332393:0.4496555852728088:0.1298469783125372:0.1045832742016494:"0.2739786511896807:0.04193551102332393:0.4496555852728088:0.1298469783125372:0.1045832742016494:\'0.2739786511896807:0.04193551102332393:0.4496555852728088:0.1298469783125372:0.1045832742016494\'"'</t>
-  </si>
-  <si>
-    <t>0.03744275801747336:0.16899734942148248:0.09394011306381288:0.22992820100492414:0.46969157849230714:'0.03744275801747336:0.16899734942148248:0.09394011306381288:0.22992820100492414:0.46969157849230714:"0.03744275801747336:0.16899734942148248:0.09394011306381288:0.22992820100492414:0.46969157849230714:\'0.03744275801747336:0.16899734942148248:0.09394011306381288:0.22992820100492414:0.46969157849230714\'"'</t>
-  </si>
-  <si>
-    <t>0.12655103364603323:0.21722155723607658:0.06003495743759002:0.20048098648232784:0.3957114651979722:'0.12655103364603323:0.21722155723607658:0.06003495743759002:0.20048098648232784:0.3957114651979722:"0.12655103364603323:0.21722155723607658:0.06003495743759002:0.20048098648232784:0.3957114651979722:\'0.12655103364603323:0.21722155723607658:0.06003495743759002:0.20048098648232784:0.3957114651979722\'"'</t>
-  </si>
-  <si>
-    <t>0.12237712616089151:0.07293784141940536:0.039180538245610075:0.12751952805853817:0.6379849661155549:'0.12237712616089151:0.07293784141940536:0.039180538245610075:0.12751952805853817:0.6379849661155549:"0.12237712616089151:0.07293784141940536:0.039180538245610075:0.12751952805853817:0.6379849661155549:\'0.12237712616089151:0.07293784141940536:0.039180538245610075:0.12751952805853817:0.6379849661155549\'"'</t>
-  </si>
-  <si>
-    <t>0.15649884726812238:0.08597952671094426:0.007373107703755164:0.05819832290198865:0.6919501954151895:'0.15649884726812238:0.08597952671094426:0.007373107703755164:0.05819832290198865:0.6919501954151895:"0.15649884726812238:0.08597952671094426:0.007373107703755164:0.05819832290198865:0.6919501954151895:\'0.15649884726812238:0.08597952671094426:0.007373107703755164:0.05819832290198865:0.6919501954151895\'"'</t>
-  </si>
-  <si>
-    <t>0.26218025344058743:0.2391269771185358:0.11980515008466874:0.0371516636392:0.341735955717008:'0.26218025344058743:0.2391269771185358:0.11980515008466874:0.0371516636392:0.341735955717008:"0.26218025344058743:0.2391269771185358:0.11980515008466874:0.0371516636392:0.341735955717008:\'0.26218025344058743:0.2391269771185358:0.11980515008466874:0.0371516636392:0.341735955717008\'"'</t>
-  </si>
-  <si>
-    <t>0.17297868951796821:0.0038734044236464053:0.15141123544969604:0.1239330787920094:0.5478035918166799:'0.17297868951796821:0.0038734044236464053:0.15141123544969604:0.1239330787920094:0.5478035918166799:"0.17297868951796821:0.0038734044236464053:0.15141123544969604:0.1239330787920094:0.5478035918166799:\'0.17297868951796821:0.0038734044236464053:0.15141123544969604:0.1239330787920094:0.5478035918166799\'"'</t>
-  </si>
-  <si>
-    <t>0.3071458935191035:0.13511293658740064:0.06436706646403009:0.25103551846993916:0.24233858495952668:'0.3071458935191035:0.13511293658740064:0.06436706646403009:0.25103551846993916:0.24233858495952668:"0.3071458935191035:0.13511293658740064:0.06436706646403009:0.25103551846993916:0.24233858495952668:\'0.3071458935191035:0.13511293658740064:0.06436706646403009:0.25103551846993916:0.24233858495952668\'"'</t>
-  </si>
-  <si>
-    <t>0.0008499840013651758:0.0010790274898496441:0.001230791211281703:0.00043322934840114803:0.9964069679491023:'0.0008499840013651758:0.0010790274898496441:0.001230791211281703:0.00043322934840114803:0.9964069679491023:"0.0008499840013651758:0.0010790274898496441:0.001230791211281703:0.00043322934840114803:0.9964069679491023:\'0.0008499840013651758:0.0010790274898496441:0.001230791211281703:0.00043322934840114803:0.9964069679491023\'"'</t>
-  </si>
-  <si>
-    <t>0.074537560053405:0.23377596013418603:0.21868577765632807:0.21491927561621915:0.2580814265398616:'0.074537560053405:0.23377596013418603:0.21868577765632807:0.21491927561621915:0.2580814265398616:"0.074537560053405:0.23377596013418603:0.21868577765632807:0.21491927561621915:0.2580814265398616:\'0.074537560053405:0.23377596013418603:0.21868577765632807:0.21491927561621915:0.2580814265398616\'"'</t>
-  </si>
-  <si>
-    <t>0.0038831449836855747:0.2570750647234156:0.34538605480971696:0.21926666159432445:0.17438907388885735:'0.0038831449836855747:0.2570750647234156:0.34538605480971696:0.21926666159432445:0.17438907388885735:"0.0038831449836855747:0.2570750647234156:0.34538605480971696:0.21926666159432445:0.17438907388885735:\'0.0038831449836855747:0.2570750647234156:0.34538605480971696:0.21926666159432445:0.17438907388885735\'"'</t>
-  </si>
-  <si>
-    <t>0.10000252830735035:0.05411212378682602:0.040184273334564105:0.040011537136720614:0.7656895374345389:'0.10000252830735035:0.05411212378682602:0.040184273334564105:0.040011537136720614:0.7656895374345389:"0.10000252830735035:0.05411212378682602:0.040184273334564105:0.040011537136720614:0.7656895374345389:\'0.10000252830735035:0.05411212378682602:0.040184273334564105:0.040011537136720614:0.7656895374345389\'"'</t>
-  </si>
-  <si>
-    <t>0.05009674706362561:0.08270077476439788:0.0405067293390163:0.08045255983596511:0.7462431889969952:'0.05009674706362561:0.08270077476439788:0.0405067293390163:0.08045255983596511:0.7462431889969952:"0.05009674706362561:0.08270077476439788:0.0405067293390163:0.08045255983596511:0.7462431889969952:\'0.05009674706362561:0.08270077476439788:0.0405067293390163:0.08045255983596511:0.7462431889969952\'"'</t>
-  </si>
-  <si>
-    <t>0.043478271812166396:0.04165595053028977:0.06006448699021291:0.038298636775646516:0.8165026538916844:'0.043478271812166396:0.04165595053028977:0.06006448699021291:0.038298636775646516:0.8165026538916844:"0.043478271812166396:0.04165595053028977:0.06006448699021291:0.038298636775646516:0.8165026538916844:\'0.043478271812166396:0.04165595053028977:0.06006448699021291:0.038298636775646516:0.8165026538916844\'"'</t>
-  </si>
-  <si>
-    <t>0.14037800101418405:0.3252409319849474:0.19884286680342372:0.2868468330849948:0.048691367112449924:'0.14037800101418405:0.3252409319849474:0.19884286680342372:0.2868468330849948:0.048691367112449924:"0.14037800101418405:0.3252409319849474:0.19884286680342372:0.2868468330849948:0.048691367112449924:\'0.14037800101418405:0.3252409319849474:0.19884286680342372:0.2868468330849948:0.048691367112449924\'"'</t>
-  </si>
-  <si>
-    <t>0.267275179454366:0.04723230298522335:0.24410864883377942:0.024494377196729145:0.41688949152990207:'0.267275179454366:0.04723230298522335:0.24410864883377942:0.024494377196729145:0.41688949152990207:"0.267275179454366:0.04723230298522335:0.24410864883377942:0.024494377196729145:0.41688949152990207:\'0.267275179454366:0.04723230298522335:0.24410864883377942:0.024494377196729145:0.41688949152990207\'"'</t>
-  </si>
-  <si>
-    <t>0.012580916913995415:0.013647930365035737:0.012313135409237473:0.011776021160717033:0.9496819961510143:'0.012580916913995415:0.013647930365035737:0.012313135409237473:0.011776021160717033:0.9496819961510143:"0.012580916913995415:0.013647930365035737:0.012313135409237473:0.011776021160717033:0.9496819961510143:\'0.012580916913995415:0.013647930365035737:0.012313135409237473:0.011776021160717033:0.9496819961510143\'"'</t>
-  </si>
-  <si>
-    <t>0.1797578576761459:0.08087059903348022:0.09418509128847868:0.5737293034264526:0.07145714857544264:'0.1797578576761459:0.08087059903348022:0.09418509128847868:0.5737293034264526:0.07145714857544264:"0.1797578576761459:0.08087059903348022:0.09418509128847868:0.5737293034264526:0.07145714857544264:\'0.1797578576761459:0.08087059903348022:0.09418509128847868:0.5737293034264526:0.07145714857544264\'"'</t>
-  </si>
-  <si>
-    <t>0.8784777661468466:0.006370503431624358:0.04859964178467366:0.028206730676399738:0.03834535796045566:'0.8784777661468466:0.006370503431624358:0.04859964178467366:0.028206730676399738:0.03834535796045566:\'0.8784777661468466:0.006370503431624358:0.04859964178467366:0.028206730676399738:0.03834535796045566:"0.8784777661468466:0.006370503431624358:0.04859964178467366:0.028206730676399738:0.03834535796045566:\\\'0.8784777661468466:0.006370503431624358:0.04859964178467366:0.028206730676399738:0.03834535796045566\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.5788884213912752:0.1148213613226778:0.07098608081635895:0.2342593506406826:0.0010447858290055308:'0.5788884213912752:0.1148213613226778:0.07098608081635895:0.2342593506406826:0.0010447858290055308:\'0.5788884213912752:0.1148213613226778:0.07098608081635895:0.2342593506406826:0.0010447858290055308:"0.5788884213912752:0.1148213613226778:0.07098608081635895:0.2342593506406826:0.0010447858290055308:\\\'0.5788884213912752:0.1148213613226778:0.07098608081635895:0.2342593506406826:0.0010447858290055308\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.1045832742016494:0.2739786511896807:0.04193551102332393:0.4496555852728088:0.1298469783125372:'0.1045832742016494:0.2739786511896807:0.04193551102332393:0.4496555852728088:0.1298469783125372:\'0.1045832742016494:0.2739786511896807:0.04193551102332393:0.4496555852728088:0.1298469783125372:"0.1045832742016494:0.2739786511896807:0.04193551102332393:0.4496555852728088:0.1298469783125372:\\\'0.1045832742016494:0.2739786511896807:0.04193551102332393:0.4496555852728088:0.1298469783125372\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.46969157849230714:0.03744275801747336:0.16899734942148248:0.09394011306381288:0.22992820100492414:'0.46969157849230714:0.03744275801747336:0.16899734942148248:0.09394011306381288:0.22992820100492414:\'0.46969157849230714:0.03744275801747336:0.16899734942148248:0.09394011306381288:0.22992820100492414:"0.46969157849230714:0.03744275801747336:0.16899734942148248:0.09394011306381288:0.22992820100492414:\\\'0.46969157849230714:0.03744275801747336:0.16899734942148248:0.09394011306381288:0.22992820100492414\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.3957114651979722:0.12655103364603323:0.21722155723607658:0.06003495743759002:0.20048098648232784:'0.3957114651979722:0.12655103364603323:0.21722155723607658:0.06003495743759002:0.20048098648232784:\'0.3957114651979722:0.12655103364603323:0.21722155723607658:0.06003495743759002:0.20048098648232784:"0.3957114651979722:0.12655103364603323:0.21722155723607658:0.06003495743759002:0.20048098648232784:\\\'0.3957114651979722:0.12655103364603323:0.21722155723607658:0.06003495743759002:0.20048098648232784\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.6379849661155549:0.12237712616089151:0.07293784141940536:0.039180538245610075:0.12751952805853817:'0.6379849661155549:0.12237712616089151:0.07293784141940536:0.039180538245610075:0.12751952805853817:\'0.6379849661155549:0.12237712616089151:0.07293784141940536:0.039180538245610075:0.12751952805853817:"0.6379849661155549:0.12237712616089151:0.07293784141940536:0.039180538245610075:0.12751952805853817:\\\'0.6379849661155549:0.12237712616089151:0.07293784141940536:0.039180538245610075:0.12751952805853817\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.6919501954151895:0.15649884726812238:0.08597952671094426:0.007373107703755164:0.05819832290198865:'0.6919501954151895:0.15649884726812238:0.08597952671094426:0.007373107703755164:0.05819832290198865:\'0.6919501954151895:0.15649884726812238:0.08597952671094426:0.007373107703755164:0.05819832290198865:"0.6919501954151895:0.15649884726812238:0.08597952671094426:0.007373107703755164:0.05819832290198865:\\\'0.6919501954151895:0.15649884726812238:0.08597952671094426:0.007373107703755164:0.05819832290198865\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.341735955717008:0.26218025344058743:0.2391269771185358:0.11980515008466874:0.0371516636392:'0.341735955717008:0.26218025344058743:0.2391269771185358:0.11980515008466874:0.0371516636392:\'0.341735955717008:0.26218025344058743:0.2391269771185358:0.11980515008466874:0.0371516636392:"0.341735955717008:0.26218025344058743:0.2391269771185358:0.11980515008466874:0.0371516636392:\\\'0.341735955717008:0.26218025344058743:0.2391269771185358:0.11980515008466874:0.0371516636392\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.5478035918166799:0.17297868951796821:0.0038734044236464053:0.15141123544969604:0.1239330787920094:'0.5478035918166799:0.17297868951796821:0.0038734044236464053:0.15141123544969604:0.1239330787920094:\'0.5478035918166799:0.17297868951796821:0.0038734044236464053:0.15141123544969604:0.1239330787920094:"0.5478035918166799:0.17297868951796821:0.0038734044236464053:0.15141123544969604:0.1239330787920094:\\\'0.5478035918166799:0.17297868951796821:0.0038734044236464053:0.15141123544969604:0.1239330787920094\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.24233858495952668:0.3071458935191035:0.13511293658740064:0.06436706646403009:0.25103551846993916:'0.24233858495952668:0.3071458935191035:0.13511293658740064:0.06436706646403009:0.25103551846993916:\'0.24233858495952668:0.3071458935191035:0.13511293658740064:0.06436706646403009:0.25103551846993916:"0.24233858495952668:0.3071458935191035:0.13511293658740064:0.06436706646403009:0.25103551846993916:\\\'0.24233858495952668:0.3071458935191035:0.13511293658740064:0.06436706646403009:0.25103551846993916\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.9964069679491023:0.0008499840013651758:0.0010790274898496441:0.001230791211281703:0.00043322934840114803:'0.9964069679491023:0.0008499840013651758:0.0010790274898496441:0.001230791211281703:0.00043322934840114803:\'0.9964069679491023:0.0008499840013651758:0.0010790274898496441:0.001230791211281703:0.00043322934840114803:"0.9964069679491023:0.0008499840013651758:0.0010790274898496441:0.001230791211281703:0.00043322934840114803:\\\'0.9964069679491023:0.0008499840013651758:0.0010790274898496441:0.001230791211281703:0.00043322934840114803\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.2580814265398616:0.074537560053405:0.23377596013418603:0.21868577765632807:0.21491927561621915:'0.2580814265398616:0.074537560053405:0.23377596013418603:0.21868577765632807:0.21491927561621915:\'0.2580814265398616:0.074537560053405:0.23377596013418603:0.21868577765632807:0.21491927561621915:"0.2580814265398616:0.074537560053405:0.23377596013418603:0.21868577765632807:0.21491927561621915:\\\'0.2580814265398616:0.074537560053405:0.23377596013418603:0.21868577765632807:0.21491927561621915\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.17438907388885735:0.0038831449836855747:0.2570750647234156:0.34538605480971696:0.21926666159432445:'0.17438907388885735:0.0038831449836855747:0.2570750647234156:0.34538605480971696:0.21926666159432445:\'0.17438907388885735:0.0038831449836855747:0.2570750647234156:0.34538605480971696:0.21926666159432445:"0.17438907388885735:0.0038831449836855747:0.2570750647234156:0.34538605480971696:0.21926666159432445:\\\'0.17438907388885735:0.0038831449836855747:0.2570750647234156:0.34538605480971696:0.21926666159432445\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.7656895374345389:0.10000252830735035:0.05411212378682602:0.040184273334564105:0.040011537136720614:'0.7656895374345389:0.10000252830735035:0.05411212378682602:0.040184273334564105:0.040011537136720614:\'0.7656895374345389:0.10000252830735035:0.05411212378682602:0.040184273334564105:0.040011537136720614:"0.7656895374345389:0.10000252830735035:0.05411212378682602:0.040184273334564105:0.040011537136720614:\\\'0.7656895374345389:0.10000252830735035:0.05411212378682602:0.040184273334564105:0.040011537136720614\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.7462431889969952:0.05009674706362561:0.08270077476439788:0.0405067293390163:0.08045255983596511:'0.7462431889969952:0.05009674706362561:0.08270077476439788:0.0405067293390163:0.08045255983596511:\'0.7462431889969952:0.05009674706362561:0.08270077476439788:0.0405067293390163:0.08045255983596511:"0.7462431889969952:0.05009674706362561:0.08270077476439788:0.0405067293390163:0.08045255983596511:\\\'0.7462431889969952:0.05009674706362561:0.08270077476439788:0.0405067293390163:0.08045255983596511\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.8165026538916844:0.043478271812166396:0.04165595053028977:0.06006448699021291:0.038298636775646516:'0.8165026538916844:0.043478271812166396:0.04165595053028977:0.06006448699021291:0.038298636775646516:\'0.8165026538916844:0.043478271812166396:0.04165595053028977:0.06006448699021291:0.038298636775646516:"0.8165026538916844:0.043478271812166396:0.04165595053028977:0.06006448699021291:0.038298636775646516:\\\'0.8165026538916844:0.043478271812166396:0.04165595053028977:0.06006448699021291:0.038298636775646516\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.048691367112449924:0.14037800101418405:0.3252409319849474:0.19884286680342372:0.2868468330849948:'0.048691367112449924:0.14037800101418405:0.3252409319849474:0.19884286680342372:0.2868468330849948:\'0.048691367112449924:0.14037800101418405:0.3252409319849474:0.19884286680342372:0.2868468330849948:"0.048691367112449924:0.14037800101418405:0.3252409319849474:0.19884286680342372:0.2868468330849948:\\\'0.048691367112449924:0.14037800101418405:0.3252409319849474:0.19884286680342372:0.2868468330849948\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.41688949152990207:0.267275179454366:0.04723230298522335:0.24410864883377942:0.024494377196729145:'0.41688949152990207:0.267275179454366:0.04723230298522335:0.24410864883377942:0.024494377196729145:\'0.41688949152990207:0.267275179454366:0.04723230298522335:0.24410864883377942:0.024494377196729145:"0.41688949152990207:0.267275179454366:0.04723230298522335:0.24410864883377942:0.024494377196729145:\\\'0.41688949152990207:0.267275179454366:0.04723230298522335:0.24410864883377942:0.024494377196729145\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.9496819961510143:0.012580916913995415:0.013647930365035737:0.012313135409237473:0.011776021160717033:'0.9496819961510143:0.012580916913995415:0.013647930365035737:0.012313135409237473:0.011776021160717033:\'0.9496819961510143:0.012580916913995415:0.013647930365035737:0.012313135409237473:0.011776021160717033:"0.9496819961510143:0.012580916913995415:0.013647930365035737:0.012313135409237473:0.011776021160717033:\\\'0.9496819961510143:0.012580916913995415:0.013647930365035737:0.012313135409237473:0.011776021160717033\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.07145714857544264:0.1797578576761459:0.08087059903348022:0.09418509128847868:0.5737293034264526:'0.07145714857544264:0.1797578576761459:0.08087059903348022:0.09418509128847868:0.5737293034264526:\'0.07145714857544264:0.1797578576761459:0.08087059903348022:0.09418509128847868:0.5737293034264526:"0.07145714857544264:0.1797578576761459:0.08087059903348022:0.09418509128847868:0.5737293034264526:\\\'0.07145714857544264:0.1797578576761459:0.08087059903348022:0.09418509128847868:0.5737293034264526\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.03834535796045566:0.8784777661468466:0.006370503431624358:0.04859964178467366:0.028206730676399738:'0.03834535796045566:0.8784777661468466:0.006370503431624358:0.04859964178467366:0.028206730676399738:\'0.03834535796045566:0.8784777661468466:0.006370503431624358:0.04859964178467366:0.028206730676399738:"0.03834535796045566:0.8784777661468466:0.006370503431624358:0.04859964178467366:0.028206730676399738:\\\'0.03834535796045566:0.8784777661468466:0.006370503431624358:0.04859964178467366:0.028206730676399738\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.0010447858290055308:0.5788884213912752:0.1148213613226778:0.07098608081635895:0.2342593506406826:'0.0010447858290055308:0.5788884213912752:0.1148213613226778:0.07098608081635895:0.2342593506406826:\'0.0010447858290055308:0.5788884213912752:0.1148213613226778:0.07098608081635895:0.2342593506406826:"0.0010447858290055308:0.5788884213912752:0.1148213613226778:0.07098608081635895:0.2342593506406826:\\\'0.0010447858290055308:0.5788884213912752:0.1148213613226778:0.07098608081635895:0.2342593506406826\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.1298469783125372:0.1045832742016494:0.2739786511896807:0.04193551102332393:0.4496555852728088:'0.1298469783125372:0.1045832742016494:0.2739786511896807:0.04193551102332393:0.4496555852728088:\'0.1298469783125372:0.1045832742016494:0.2739786511896807:0.04193551102332393:0.4496555852728088:"0.1298469783125372:0.1045832742016494:0.2739786511896807:0.04193551102332393:0.4496555852728088:\\\'0.1298469783125372:0.1045832742016494:0.2739786511896807:0.04193551102332393:0.4496555852728088\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.22992820100492414:0.46969157849230714:0.03744275801747336:0.16899734942148248:0.09394011306381288:'0.22992820100492414:0.46969157849230714:0.03744275801747336:0.16899734942148248:0.09394011306381288:\'0.22992820100492414:0.46969157849230714:0.03744275801747336:0.16899734942148248:0.09394011306381288:"0.22992820100492414:0.46969157849230714:0.03744275801747336:0.16899734942148248:0.09394011306381288:\\\'0.22992820100492414:0.46969157849230714:0.03744275801747336:0.16899734942148248:0.09394011306381288\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.20048098648232784:0.3957114651979722:0.12655103364603323:0.21722155723607658:0.06003495743759002:'0.20048098648232784:0.3957114651979722:0.12655103364603323:0.21722155723607658:0.06003495743759002:\'0.20048098648232784:0.3957114651979722:0.12655103364603323:0.21722155723607658:0.06003495743759002:"0.20048098648232784:0.3957114651979722:0.12655103364603323:0.21722155723607658:0.06003495743759002:\\\'0.20048098648232784:0.3957114651979722:0.12655103364603323:0.21722155723607658:0.06003495743759002\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.12751952805853817:0.6379849661155549:0.12237712616089151:0.07293784141940536:0.039180538245610075:'0.12751952805853817:0.6379849661155549:0.12237712616089151:0.07293784141940536:0.039180538245610075:\'0.12751952805853817:0.6379849661155549:0.12237712616089151:0.07293784141940536:0.039180538245610075:"0.12751952805853817:0.6379849661155549:0.12237712616089151:0.07293784141940536:0.039180538245610075:\\\'0.12751952805853817:0.6379849661155549:0.12237712616089151:0.07293784141940536:0.039180538245610075\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.05819832290198865:0.6919501954151895:0.15649884726812238:0.08597952671094426:0.007373107703755164:'0.05819832290198865:0.6919501954151895:0.15649884726812238:0.08597952671094426:0.007373107703755164:\'0.05819832290198865:0.6919501954151895:0.15649884726812238:0.08597952671094426:0.007373107703755164:"0.05819832290198865:0.6919501954151895:0.15649884726812238:0.08597952671094426:0.007373107703755164:\\\'0.05819832290198865:0.6919501954151895:0.15649884726812238:0.08597952671094426:0.007373107703755164\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.0371516636392:0.341735955717008:0.26218025344058743:0.2391269771185358:0.11980515008466874:'0.0371516636392:0.341735955717008:0.26218025344058743:0.2391269771185358:0.11980515008466874:\'0.0371516636392:0.341735955717008:0.26218025344058743:0.2391269771185358:0.11980515008466874:"0.0371516636392:0.341735955717008:0.26218025344058743:0.2391269771185358:0.11980515008466874:\\\'0.0371516636392:0.341735955717008:0.26218025344058743:0.2391269771185358:0.11980515008466874\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.1239330787920094:0.5478035918166799:0.17297868951796821:0.0038734044236464053:0.15141123544969604:'0.1239330787920094:0.5478035918166799:0.17297868951796821:0.0038734044236464053:0.15141123544969604:\'0.1239330787920094:0.5478035918166799:0.17297868951796821:0.0038734044236464053:0.15141123544969604:"0.1239330787920094:0.5478035918166799:0.17297868951796821:0.0038734044236464053:0.15141123544969604:\\\'0.1239330787920094:0.5478035918166799:0.17297868951796821:0.0038734044236464053:0.15141123544969604\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.25103551846993916:0.24233858495952668:0.3071458935191035:0.13511293658740064:0.06436706646403009:'0.25103551846993916:0.24233858495952668:0.3071458935191035:0.13511293658740064:0.06436706646403009:\'0.25103551846993916:0.24233858495952668:0.3071458935191035:0.13511293658740064:0.06436706646403009:"0.25103551846993916:0.24233858495952668:0.3071458935191035:0.13511293658740064:0.06436706646403009:\\\'0.25103551846993916:0.24233858495952668:0.3071458935191035:0.13511293658740064:0.06436706646403009\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.00043322934840114803:0.9964069679491023:0.0008499840013651758:0.0010790274898496441:0.001230791211281703:'0.00043322934840114803:0.9964069679491023:0.0008499840013651758:0.0010790274898496441:0.001230791211281703:\'0.00043322934840114803:0.9964069679491023:0.0008499840013651758:0.0010790274898496441:0.001230791211281703:"0.00043322934840114803:0.9964069679491023:0.0008499840013651758:0.0010790274898496441:0.001230791211281703:\\\'0.00043322934840114803:0.9964069679491023:0.0008499840013651758:0.0010790274898496441:0.001230791211281703\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.21491927561621915:0.2580814265398616:0.074537560053405:0.23377596013418603:0.21868577765632807:'0.21491927561621915:0.2580814265398616:0.074537560053405:0.23377596013418603:0.21868577765632807:\'0.21491927561621915:0.2580814265398616:0.074537560053405:0.23377596013418603:0.21868577765632807:"0.21491927561621915:0.2580814265398616:0.074537560053405:0.23377596013418603:0.21868577765632807:\\\'0.21491927561621915:0.2580814265398616:0.074537560053405:0.23377596013418603:0.21868577765632807\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.21926666159432445:0.17438907388885735:0.0038831449836855747:0.2570750647234156:0.34538605480971696:'0.21926666159432445:0.17438907388885735:0.0038831449836855747:0.2570750647234156:0.34538605480971696:\'0.21926666159432445:0.17438907388885735:0.0038831449836855747:0.2570750647234156:0.34538605480971696:"0.21926666159432445:0.17438907388885735:0.0038831449836855747:0.2570750647234156:0.34538605480971696:\\\'0.21926666159432445:0.17438907388885735:0.0038831449836855747:0.2570750647234156:0.34538605480971696\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.040011537136720614:0.7656895374345389:0.10000252830735035:0.05411212378682602:0.040184273334564105:'0.040011537136720614:0.7656895374345389:0.10000252830735035:0.05411212378682602:0.040184273334564105:\'0.040011537136720614:0.7656895374345389:0.10000252830735035:0.05411212378682602:0.040184273334564105:"0.040011537136720614:0.7656895374345389:0.10000252830735035:0.05411212378682602:0.040184273334564105:\\\'0.040011537136720614:0.7656895374345389:0.10000252830735035:0.05411212378682602:0.040184273334564105\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.08045255983596511:0.7462431889969952:0.05009674706362561:0.08270077476439788:0.0405067293390163:'0.08045255983596511:0.7462431889969952:0.05009674706362561:0.08270077476439788:0.0405067293390163:\'0.08045255983596511:0.7462431889969952:0.05009674706362561:0.08270077476439788:0.0405067293390163:"0.08045255983596511:0.7462431889969952:0.05009674706362561:0.08270077476439788:0.0405067293390163:\\\'0.08045255983596511:0.7462431889969952:0.05009674706362561:0.08270077476439788:0.0405067293390163\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.038298636775646516:0.8165026538916844:0.043478271812166396:0.04165595053028977:0.06006448699021291:'0.038298636775646516:0.8165026538916844:0.043478271812166396:0.04165595053028977:0.06006448699021291:\'0.038298636775646516:0.8165026538916844:0.043478271812166396:0.04165595053028977:0.06006448699021291:"0.038298636775646516:0.8165026538916844:0.043478271812166396:0.04165595053028977:0.06006448699021291:\\\'0.038298636775646516:0.8165026538916844:0.043478271812166396:0.04165595053028977:0.06006448699021291\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.2868468330849948:0.048691367112449924:0.14037800101418405:0.3252409319849474:0.19884286680342372:'0.2868468330849948:0.048691367112449924:0.14037800101418405:0.3252409319849474:0.19884286680342372:\'0.2868468330849948:0.048691367112449924:0.14037800101418405:0.3252409319849474:0.19884286680342372:"0.2868468330849948:0.048691367112449924:0.14037800101418405:0.3252409319849474:0.19884286680342372:\\\'0.2868468330849948:0.048691367112449924:0.14037800101418405:0.3252409319849474:0.19884286680342372\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.024494377196729145:0.41688949152990207:0.267275179454366:0.04723230298522335:0.24410864883377942:'0.024494377196729145:0.41688949152990207:0.267275179454366:0.04723230298522335:0.24410864883377942:\'0.024494377196729145:0.41688949152990207:0.267275179454366:0.04723230298522335:0.24410864883377942:"0.024494377196729145:0.41688949152990207:0.267275179454366:0.04723230298522335:0.24410864883377942:\\\'0.024494377196729145:0.41688949152990207:0.267275179454366:0.04723230298522335:0.24410864883377942\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.011776021160717033:0.9496819961510143:0.012580916913995415:0.013647930365035737:0.012313135409237473:'0.011776021160717033:0.9496819961510143:0.012580916913995415:0.013647930365035737:0.012313135409237473:\'0.011776021160717033:0.9496819961510143:0.012580916913995415:0.013647930365035737:0.012313135409237473:"0.011776021160717033:0.9496819961510143:0.012580916913995415:0.013647930365035737:0.012313135409237473:\\\'0.011776021160717033:0.9496819961510143:0.012580916913995415:0.013647930365035737:0.012313135409237473\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.5737293034264526:0.07145714857544264:0.1797578576761459:0.08087059903348022:0.09418509128847868:'0.5737293034264526:0.07145714857544264:0.1797578576761459:0.08087059903348022:0.09418509128847868:\'0.5737293034264526:0.07145714857544264:0.1797578576761459:0.08087059903348022:0.09418509128847868:"0.5737293034264526:0.07145714857544264:0.1797578576761459:0.08087059903348022:0.09418509128847868:\\\'0.5737293034264526:0.07145714857544264:0.1797578576761459:0.08087059903348022:0.09418509128847868\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.028206730676399738:0.03834535796045566:0.8784777661468466:0.006370503431624358:0.04859964178467366:'0.028206730676399738:0.03834535796045566:0.8784777661468466:0.006370503431624358:0.04859964178467366:\'0.028206730676399738:0.03834535796045566:0.8784777661468466:0.006370503431624358:0.04859964178467366:"0.028206730676399738:0.03834535796045566:0.8784777661468466:0.006370503431624358:0.04859964178467366:\\\'0.028206730676399738:0.03834535796045566:0.8784777661468466:0.006370503431624358:0.04859964178467366\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.2342593506406826:0.0010447858290055308:0.5788884213912752:0.1148213613226778:0.07098608081635895:'0.2342593506406826:0.0010447858290055308:0.5788884213912752:0.1148213613226778:0.07098608081635895:\'0.2342593506406826:0.0010447858290055308:0.5788884213912752:0.1148213613226778:0.07098608081635895:"0.2342593506406826:0.0010447858290055308:0.5788884213912752:0.1148213613226778:0.07098608081635895:\\\'0.2342593506406826:0.0010447858290055308:0.5788884213912752:0.1148213613226778:0.07098608081635895\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.4496555852728088:0.1298469783125372:0.1045832742016494:0.2739786511896807:0.04193551102332393:'0.4496555852728088:0.1298469783125372:0.1045832742016494:0.2739786511896807:0.04193551102332393:\'0.4496555852728088:0.1298469783125372:0.1045832742016494:0.2739786511896807:0.04193551102332393:"0.4496555852728088:0.1298469783125372:0.1045832742016494:0.2739786511896807:0.04193551102332393:\\\'0.4496555852728088:0.1298469783125372:0.1045832742016494:0.2739786511896807:0.04193551102332393\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.09394011306381288:0.22992820100492414:0.46969157849230714:0.03744275801747336:0.16899734942148248:'0.09394011306381288:0.22992820100492414:0.46969157849230714:0.03744275801747336:0.16899734942148248:\'0.09394011306381288:0.22992820100492414:0.46969157849230714:0.03744275801747336:0.16899734942148248:"0.09394011306381288:0.22992820100492414:0.46969157849230714:0.03744275801747336:0.16899734942148248:\\\'0.09394011306381288:0.22992820100492414:0.46969157849230714:0.03744275801747336:0.16899734942148248\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.06003495743759002:0.20048098648232784:0.3957114651979722:0.12655103364603323:0.21722155723607658:'0.06003495743759002:0.20048098648232784:0.3957114651979722:0.12655103364603323:0.21722155723607658:\'0.06003495743759002:0.20048098648232784:0.3957114651979722:0.12655103364603323:0.21722155723607658:"0.06003495743759002:0.20048098648232784:0.3957114651979722:0.12655103364603323:0.21722155723607658:\\\'0.06003495743759002:0.20048098648232784:0.3957114651979722:0.12655103364603323:0.21722155723607658\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.039180538245610075:0.12751952805853817:0.6379849661155549:0.12237712616089151:0.07293784141940536:'0.039180538245610075:0.12751952805853817:0.6379849661155549:0.12237712616089151:0.07293784141940536:\'0.039180538245610075:0.12751952805853817:0.6379849661155549:0.12237712616089151:0.07293784141940536:"0.039180538245610075:0.12751952805853817:0.6379849661155549:0.12237712616089151:0.07293784141940536:\\\'0.039180538245610075:0.12751952805853817:0.6379849661155549:0.12237712616089151:0.07293784141940536\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.007373107703755164:0.05819832290198865:0.6919501954151895:0.15649884726812238:0.08597952671094426:'0.007373107703755164:0.05819832290198865:0.6919501954151895:0.15649884726812238:0.08597952671094426:\'0.007373107703755164:0.05819832290198865:0.6919501954151895:0.15649884726812238:0.08597952671094426:"0.007373107703755164:0.05819832290198865:0.6919501954151895:0.15649884726812238:0.08597952671094426:\\\'0.007373107703755164:0.05819832290198865:0.6919501954151895:0.15649884726812238:0.08597952671094426\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.11980515008466874:0.0371516636392:0.341735955717008:0.26218025344058743:0.2391269771185358:'0.11980515008466874:0.0371516636392:0.341735955717008:0.26218025344058743:0.2391269771185358:\'0.11980515008466874:0.0371516636392:0.341735955717008:0.26218025344058743:0.2391269771185358:"0.11980515008466874:0.0371516636392:0.341735955717008:0.26218025344058743:0.2391269771185358:\\\'0.11980515008466874:0.0371516636392:0.341735955717008:0.26218025344058743:0.2391269771185358\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.15141123544969604:0.1239330787920094:0.5478035918166799:0.17297868951796821:0.0038734044236464053:'0.15141123544969604:0.1239330787920094:0.5478035918166799:0.17297868951796821:0.0038734044236464053:\'0.15141123544969604:0.1239330787920094:0.5478035918166799:0.17297868951796821:0.0038734044236464053:"0.15141123544969604:0.1239330787920094:0.5478035918166799:0.17297868951796821:0.0038734044236464053:\\\'0.15141123544969604:0.1239330787920094:0.5478035918166799:0.17297868951796821:0.0038734044236464053\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.06436706646403009:0.25103551846993916:0.24233858495952668:0.3071458935191035:0.13511293658740064:'0.06436706646403009:0.25103551846993916:0.24233858495952668:0.3071458935191035:0.13511293658740064:\'0.06436706646403009:0.25103551846993916:0.24233858495952668:0.3071458935191035:0.13511293658740064:"0.06436706646403009:0.25103551846993916:0.24233858495952668:0.3071458935191035:0.13511293658740064:\\\'0.06436706646403009:0.25103551846993916:0.24233858495952668:0.3071458935191035:0.13511293658740064\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.001230791211281703:0.00043322934840114803:0.9964069679491023:0.0008499840013651758:0.0010790274898496441:'0.001230791211281703:0.00043322934840114803:0.9964069679491023:0.0008499840013651758:0.0010790274898496441:\'0.001230791211281703:0.00043322934840114803:0.9964069679491023:0.0008499840013651758:0.0010790274898496441:"0.001230791211281703:0.00043322934840114803:0.9964069679491023:0.0008499840013651758:0.0010790274898496441:\\\'0.001230791211281703:0.00043322934840114803:0.9964069679491023:0.0008499840013651758:0.0010790274898496441\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.21868577765632807:0.21491927561621915:0.2580814265398616:0.074537560053405:0.23377596013418603:'0.21868577765632807:0.21491927561621915:0.2580814265398616:0.074537560053405:0.23377596013418603:\'0.21868577765632807:0.21491927561621915:0.2580814265398616:0.074537560053405:0.23377596013418603:"0.21868577765632807:0.21491927561621915:0.2580814265398616:0.074537560053405:0.23377596013418603:\\\'0.21868577765632807:0.21491927561621915:0.2580814265398616:0.074537560053405:0.23377596013418603\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.34538605480971696:0.21926666159432445:0.17438907388885735:0.0038831449836855747:0.2570750647234156:'0.34538605480971696:0.21926666159432445:0.17438907388885735:0.0038831449836855747:0.2570750647234156:\'0.34538605480971696:0.21926666159432445:0.17438907388885735:0.0038831449836855747:0.2570750647234156:"0.34538605480971696:0.21926666159432445:0.17438907388885735:0.0038831449836855747:0.2570750647234156:\\\'0.34538605480971696:0.21926666159432445:0.17438907388885735:0.0038831449836855747:0.2570750647234156\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.040184273334564105:0.040011537136720614:0.7656895374345389:0.10000252830735035:0.05411212378682602:'0.040184273334564105:0.040011537136720614:0.7656895374345389:0.10000252830735035:0.05411212378682602:\'0.040184273334564105:0.040011537136720614:0.7656895374345389:0.10000252830735035:0.05411212378682602:"0.040184273334564105:0.040011537136720614:0.7656895374345389:0.10000252830735035:0.05411212378682602:\\\'0.040184273334564105:0.040011537136720614:0.7656895374345389:0.10000252830735035:0.05411212378682602\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.0405067293390163:0.08045255983596511:0.7462431889969952:0.05009674706362561:0.08270077476439788:'0.0405067293390163:0.08045255983596511:0.7462431889969952:0.05009674706362561:0.08270077476439788:\'0.0405067293390163:0.08045255983596511:0.7462431889969952:0.05009674706362561:0.08270077476439788:"0.0405067293390163:0.08045255983596511:0.7462431889969952:0.05009674706362561:0.08270077476439788:\\\'0.0405067293390163:0.08045255983596511:0.7462431889969952:0.05009674706362561:0.08270077476439788\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.06006448699021291:0.038298636775646516:0.8165026538916844:0.043478271812166396:0.04165595053028977:'0.06006448699021291:0.038298636775646516:0.8165026538916844:0.043478271812166396:0.04165595053028977:\'0.06006448699021291:0.038298636775646516:0.8165026538916844:0.043478271812166396:0.04165595053028977:"0.06006448699021291:0.038298636775646516:0.8165026538916844:0.043478271812166396:0.04165595053028977:\\\'0.06006448699021291:0.038298636775646516:0.8165026538916844:0.043478271812166396:0.04165595053028977\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.19884286680342372:0.2868468330849948:0.048691367112449924:0.14037800101418405:0.3252409319849474:'0.19884286680342372:0.2868468330849948:0.048691367112449924:0.14037800101418405:0.3252409319849474:\'0.19884286680342372:0.2868468330849948:0.048691367112449924:0.14037800101418405:0.3252409319849474:"0.19884286680342372:0.2868468330849948:0.048691367112449924:0.14037800101418405:0.3252409319849474:\\\'0.19884286680342372:0.2868468330849948:0.048691367112449924:0.14037800101418405:0.3252409319849474\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.24410864883377942:0.024494377196729145:0.41688949152990207:0.267275179454366:0.04723230298522335:'0.24410864883377942:0.024494377196729145:0.41688949152990207:0.267275179454366:0.04723230298522335:\'0.24410864883377942:0.024494377196729145:0.41688949152990207:0.267275179454366:0.04723230298522335:"0.24410864883377942:0.024494377196729145:0.41688949152990207:0.267275179454366:0.04723230298522335:\\\'0.24410864883377942:0.024494377196729145:0.41688949152990207:0.267275179454366:0.04723230298522335\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.012313135409237473:0.011776021160717033:0.9496819961510143:0.012580916913995415:0.013647930365035737:'0.012313135409237473:0.011776021160717033:0.9496819961510143:0.012580916913995415:0.013647930365035737:\'0.012313135409237473:0.011776021160717033:0.9496819961510143:0.012580916913995415:0.013647930365035737:"0.012313135409237473:0.011776021160717033:0.9496819961510143:0.012580916913995415:0.013647930365035737:\\\'0.012313135409237473:0.011776021160717033:0.9496819961510143:0.012580916913995415:0.013647930365035737\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.09418509128847868:0.5737293034264526:0.07145714857544264:0.1797578576761459:0.08087059903348022:'0.09418509128847868:0.5737293034264526:0.07145714857544264:0.1797578576761459:0.08087059903348022:\'0.09418509128847868:0.5737293034264526:0.07145714857544264:0.1797578576761459:0.08087059903348022:"0.09418509128847868:0.5737293034264526:0.07145714857544264:0.1797578576761459:0.08087059903348022:\\\'0.09418509128847868:0.5737293034264526:0.07145714857544264:0.1797578576761459:0.08087059903348022\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.04859964178467366:0.028206730676399738:0.03834535796045566:0.8784777661468466:0.006370503431624358:'0.04859964178467366:0.028206730676399738:0.03834535796045566:0.8784777661468466:0.006370503431624358:\'0.04859964178467366:0.028206730676399738:0.03834535796045566:0.8784777661468466:0.006370503431624358:"0.04859964178467366:0.028206730676399738:0.03834535796045566:0.8784777661468466:0.006370503431624358:\\\'0.04859964178467366:0.028206730676399738:0.03834535796045566:0.8784777661468466:0.006370503431624358\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.07098608081635895:0.2342593506406826:0.0010447858290055308:0.5788884213912752:0.1148213613226778:'0.07098608081635895:0.2342593506406826:0.0010447858290055308:0.5788884213912752:0.1148213613226778:\'0.07098608081635895:0.2342593506406826:0.0010447858290055308:0.5788884213912752:0.1148213613226778:"0.07098608081635895:0.2342593506406826:0.0010447858290055308:0.5788884213912752:0.1148213613226778:\\\'0.07098608081635895:0.2342593506406826:0.0010447858290055308:0.5788884213912752:0.1148213613226778\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.04193551102332393:0.4496555852728088:0.1298469783125372:0.1045832742016494:0.2739786511896807:'0.04193551102332393:0.4496555852728088:0.1298469783125372:0.1045832742016494:0.2739786511896807:\'0.04193551102332393:0.4496555852728088:0.1298469783125372:0.1045832742016494:0.2739786511896807:"0.04193551102332393:0.4496555852728088:0.1298469783125372:0.1045832742016494:0.2739786511896807:\\\'0.04193551102332393:0.4496555852728088:0.1298469783125372:0.1045832742016494:0.2739786511896807\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.16899734942148248:0.09394011306381288:0.22992820100492414:0.46969157849230714:0.03744275801747336:'0.16899734942148248:0.09394011306381288:0.22992820100492414:0.46969157849230714:0.03744275801747336:\'0.16899734942148248:0.09394011306381288:0.22992820100492414:0.46969157849230714:0.03744275801747336:"0.16899734942148248:0.09394011306381288:0.22992820100492414:0.46969157849230714:0.03744275801747336:\\\'0.16899734942148248:0.09394011306381288:0.22992820100492414:0.46969157849230714:0.03744275801747336\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.21722155723607658:0.06003495743759002:0.20048098648232784:0.3957114651979722:0.12655103364603323:'0.21722155723607658:0.06003495743759002:0.20048098648232784:0.3957114651979722:0.12655103364603323:\'0.21722155723607658:0.06003495743759002:0.20048098648232784:0.3957114651979722:0.12655103364603323:"0.21722155723607658:0.06003495743759002:0.20048098648232784:0.3957114651979722:0.12655103364603323:\\\'0.21722155723607658:0.06003495743759002:0.20048098648232784:0.3957114651979722:0.12655103364603323\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.07293784141940536:0.039180538245610075:0.12751952805853817:0.6379849661155549:0.12237712616089151:'0.07293784141940536:0.039180538245610075:0.12751952805853817:0.6379849661155549:0.12237712616089151:\'0.07293784141940536:0.039180538245610075:0.12751952805853817:0.6379849661155549:0.12237712616089151:"0.07293784141940536:0.039180538245610075:0.12751952805853817:0.6379849661155549:0.12237712616089151:\\\'0.07293784141940536:0.039180538245610075:0.12751952805853817:0.6379849661155549:0.12237712616089151\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.08597952671094426:0.007373107703755164:0.05819832290198865:0.6919501954151895:0.15649884726812238:'0.08597952671094426:0.007373107703755164:0.05819832290198865:0.6919501954151895:0.15649884726812238:\'0.08597952671094426:0.007373107703755164:0.05819832290198865:0.6919501954151895:0.15649884726812238:"0.08597952671094426:0.007373107703755164:0.05819832290198865:0.6919501954151895:0.15649884726812238:\\\'0.08597952671094426:0.007373107703755164:0.05819832290198865:0.6919501954151895:0.15649884726812238\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.2391269771185358:0.11980515008466874:0.0371516636392:0.341735955717008:0.26218025344058743:'0.2391269771185358:0.11980515008466874:0.0371516636392:0.341735955717008:0.26218025344058743:\'0.2391269771185358:0.11980515008466874:0.0371516636392:0.341735955717008:0.26218025344058743:"0.2391269771185358:0.11980515008466874:0.0371516636392:0.341735955717008:0.26218025344058743:\\\'0.2391269771185358:0.11980515008466874:0.0371516636392:0.341735955717008:0.26218025344058743\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.0038734044236464053:0.15141123544969604:0.1239330787920094:0.5478035918166799:0.17297868951796821:'0.0038734044236464053:0.15141123544969604:0.1239330787920094:0.5478035918166799:0.17297868951796821:\'0.0038734044236464053:0.15141123544969604:0.1239330787920094:0.5478035918166799:0.17297868951796821:"0.0038734044236464053:0.15141123544969604:0.1239330787920094:0.5478035918166799:0.17297868951796821:\\\'0.0038734044236464053:0.15141123544969604:0.1239330787920094:0.5478035918166799:0.17297868951796821\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.13511293658740064:0.06436706646403009:0.25103551846993916:0.24233858495952668:0.3071458935191035:'0.13511293658740064:0.06436706646403009:0.25103551846993916:0.24233858495952668:0.3071458935191035:\'0.13511293658740064:0.06436706646403009:0.25103551846993916:0.24233858495952668:0.3071458935191035:"0.13511293658740064:0.06436706646403009:0.25103551846993916:0.24233858495952668:0.3071458935191035:\\\'0.13511293658740064:0.06436706646403009:0.25103551846993916:0.24233858495952668:0.3071458935191035\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.0010790274898496441:0.001230791211281703:0.00043322934840114803:0.9964069679491023:0.0008499840013651758:'0.0010790274898496441:0.001230791211281703:0.00043322934840114803:0.9964069679491023:0.0008499840013651758:\'0.0010790274898496441:0.001230791211281703:0.00043322934840114803:0.9964069679491023:0.0008499840013651758:"0.0010790274898496441:0.001230791211281703:0.00043322934840114803:0.9964069679491023:0.0008499840013651758:\\\'0.0010790274898496441:0.001230791211281703:0.00043322934840114803:0.9964069679491023:0.0008499840013651758\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.23377596013418603:0.21868577765632807:0.21491927561621915:0.2580814265398616:0.074537560053405:'0.23377596013418603:0.21868577765632807:0.21491927561621915:0.2580814265398616:0.074537560053405:\'0.23377596013418603:0.21868577765632807:0.21491927561621915:0.2580814265398616:0.074537560053405:"0.23377596013418603:0.21868577765632807:0.21491927561621915:0.2580814265398616:0.074537560053405:\\\'0.23377596013418603:0.21868577765632807:0.21491927561621915:0.2580814265398616:0.074537560053405\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.2570750647234156:0.34538605480971696:0.21926666159432445:0.17438907388885735:0.0038831449836855747:'0.2570750647234156:0.34538605480971696:0.21926666159432445:0.17438907388885735:0.0038831449836855747:\'0.2570750647234156:0.34538605480971696:0.21926666159432445:0.17438907388885735:0.0038831449836855747:"0.2570750647234156:0.34538605480971696:0.21926666159432445:0.17438907388885735:0.0038831449836855747:\\\'0.2570750647234156:0.34538605480971696:0.21926666159432445:0.17438907388885735:0.0038831449836855747\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.05411212378682602:0.040184273334564105:0.040011537136720614:0.7656895374345389:0.10000252830735035:'0.05411212378682602:0.040184273334564105:0.040011537136720614:0.7656895374345389:0.10000252830735035:\'0.05411212378682602:0.040184273334564105:0.040011537136720614:0.7656895374345389:0.10000252830735035:"0.05411212378682602:0.040184273334564105:0.040011537136720614:0.7656895374345389:0.10000252830735035:\\\'0.05411212378682602:0.040184273334564105:0.040011537136720614:0.7656895374345389:0.10000252830735035\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.08270077476439788:0.0405067293390163:0.08045255983596511:0.7462431889969952:0.05009674706362561:'0.08270077476439788:0.0405067293390163:0.08045255983596511:0.7462431889969952:0.05009674706362561:\'0.08270077476439788:0.0405067293390163:0.08045255983596511:0.7462431889969952:0.05009674706362561:"0.08270077476439788:0.0405067293390163:0.08045255983596511:0.7462431889969952:0.05009674706362561:\\\'0.08270077476439788:0.0405067293390163:0.08045255983596511:0.7462431889969952:0.05009674706362561\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.04165595053028977:0.06006448699021291:0.038298636775646516:0.8165026538916844:0.043478271812166396:'0.04165595053028977:0.06006448699021291:0.038298636775646516:0.8165026538916844:0.043478271812166396:\'0.04165595053028977:0.06006448699021291:0.038298636775646516:0.8165026538916844:0.043478271812166396:"0.04165595053028977:0.06006448699021291:0.038298636775646516:0.8165026538916844:0.043478271812166396:\\\'0.04165595053028977:0.06006448699021291:0.038298636775646516:0.8165026538916844:0.043478271812166396\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.3252409319849474:0.19884286680342372:0.2868468330849948:0.048691367112449924:0.14037800101418405:'0.3252409319849474:0.19884286680342372:0.2868468330849948:0.048691367112449924:0.14037800101418405:\'0.3252409319849474:0.19884286680342372:0.2868468330849948:0.048691367112449924:0.14037800101418405:"0.3252409319849474:0.19884286680342372:0.2868468330849948:0.048691367112449924:0.14037800101418405:\\\'0.3252409319849474:0.19884286680342372:0.2868468330849948:0.048691367112449924:0.14037800101418405\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.04723230298522335:0.24410864883377942:0.024494377196729145:0.41688949152990207:0.267275179454366:'0.04723230298522335:0.24410864883377942:0.024494377196729145:0.41688949152990207:0.267275179454366:\'0.04723230298522335:0.24410864883377942:0.024494377196729145:0.41688949152990207:0.267275179454366:"0.04723230298522335:0.24410864883377942:0.024494377196729145:0.41688949152990207:0.267275179454366:\\\'0.04723230298522335:0.24410864883377942:0.024494377196729145:0.41688949152990207:0.267275179454366\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.013647930365035737:0.012313135409237473:0.011776021160717033:0.9496819961510143:0.012580916913995415:'0.013647930365035737:0.012313135409237473:0.011776021160717033:0.9496819961510143:0.012580916913995415:\'0.013647930365035737:0.012313135409237473:0.011776021160717033:0.9496819961510143:0.012580916913995415:"0.013647930365035737:0.012313135409237473:0.011776021160717033:0.9496819961510143:0.012580916913995415:\\\'0.013647930365035737:0.012313135409237473:0.011776021160717033:0.9496819961510143:0.012580916913995415\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.08087059903348022:0.09418509128847868:0.5737293034264526:0.07145714857544264:0.1797578576761459:'0.08087059903348022:0.09418509128847868:0.5737293034264526:0.07145714857544264:0.1797578576761459:\'0.08087059903348022:0.09418509128847868:0.5737293034264526:0.07145714857544264:0.1797578576761459:"0.08087059903348022:0.09418509128847868:0.5737293034264526:0.07145714857544264:0.1797578576761459:\\\'0.08087059903348022:0.09418509128847868:0.5737293034264526:0.07145714857544264:0.1797578576761459\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.006370503431624358:0.04859964178467366:0.028206730676399738:0.03834535796045566:0.8784777661468466:'0.006370503431624358:0.04859964178467366:0.028206730676399738:0.03834535796045566:0.8784777661468466:\'0.006370503431624358:0.04859964178467366:0.028206730676399738:0.03834535796045566:0.8784777661468466:"0.006370503431624358:0.04859964178467366:0.028206730676399738:0.03834535796045566:0.8784777661468466:\\\'0.006370503431624358:0.04859964178467366:0.028206730676399738:0.03834535796045566:0.8784777661468466\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.1148213613226778:0.07098608081635895:0.2342593506406826:0.0010447858290055308:0.5788884213912752:'0.1148213613226778:0.07098608081635895:0.2342593506406826:0.0010447858290055308:0.5788884213912752:\'0.1148213613226778:0.07098608081635895:0.2342593506406826:0.0010447858290055308:0.5788884213912752:"0.1148213613226778:0.07098608081635895:0.2342593506406826:0.0010447858290055308:0.5788884213912752:\\\'0.1148213613226778:0.07098608081635895:0.2342593506406826:0.0010447858290055308:0.5788884213912752\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.2739786511896807:0.04193551102332393:0.4496555852728088:0.1298469783125372:0.1045832742016494:'0.2739786511896807:0.04193551102332393:0.4496555852728088:0.1298469783125372:0.1045832742016494:\'0.2739786511896807:0.04193551102332393:0.4496555852728088:0.1298469783125372:0.1045832742016494:"0.2739786511896807:0.04193551102332393:0.4496555852728088:0.1298469783125372:0.1045832742016494:\\\'0.2739786511896807:0.04193551102332393:0.4496555852728088:0.1298469783125372:0.1045832742016494\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.03744275801747336:0.16899734942148248:0.09394011306381288:0.22992820100492414:0.46969157849230714:'0.03744275801747336:0.16899734942148248:0.09394011306381288:0.22992820100492414:0.46969157849230714:\'0.03744275801747336:0.16899734942148248:0.09394011306381288:0.22992820100492414:0.46969157849230714:"0.03744275801747336:0.16899734942148248:0.09394011306381288:0.22992820100492414:0.46969157849230714:\\\'0.03744275801747336:0.16899734942148248:0.09394011306381288:0.22992820100492414:0.46969157849230714\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.12655103364603323:0.21722155723607658:0.06003495743759002:0.20048098648232784:0.3957114651979722:'0.12655103364603323:0.21722155723607658:0.06003495743759002:0.20048098648232784:0.3957114651979722:\'0.12655103364603323:0.21722155723607658:0.06003495743759002:0.20048098648232784:0.3957114651979722:"0.12655103364603323:0.21722155723607658:0.06003495743759002:0.20048098648232784:0.3957114651979722:\\\'0.12655103364603323:0.21722155723607658:0.06003495743759002:0.20048098648232784:0.3957114651979722\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.12237712616089151:0.07293784141940536:0.039180538245610075:0.12751952805853817:0.6379849661155549:'0.12237712616089151:0.07293784141940536:0.039180538245610075:0.12751952805853817:0.6379849661155549:\'0.12237712616089151:0.07293784141940536:0.039180538245610075:0.12751952805853817:0.6379849661155549:"0.12237712616089151:0.07293784141940536:0.039180538245610075:0.12751952805853817:0.6379849661155549:\\\'0.12237712616089151:0.07293784141940536:0.039180538245610075:0.12751952805853817:0.6379849661155549\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.15649884726812238:0.08597952671094426:0.007373107703755164:0.05819832290198865:0.6919501954151895:'0.15649884726812238:0.08597952671094426:0.007373107703755164:0.05819832290198865:0.6919501954151895:\'0.15649884726812238:0.08597952671094426:0.007373107703755164:0.05819832290198865:0.6919501954151895:"0.15649884726812238:0.08597952671094426:0.007373107703755164:0.05819832290198865:0.6919501954151895:\\\'0.15649884726812238:0.08597952671094426:0.007373107703755164:0.05819832290198865:0.6919501954151895\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.26218025344058743:0.2391269771185358:0.11980515008466874:0.0371516636392:0.341735955717008:'0.26218025344058743:0.2391269771185358:0.11980515008466874:0.0371516636392:0.341735955717008:\'0.26218025344058743:0.2391269771185358:0.11980515008466874:0.0371516636392:0.341735955717008:"0.26218025344058743:0.2391269771185358:0.11980515008466874:0.0371516636392:0.341735955717008:\\\'0.26218025344058743:0.2391269771185358:0.11980515008466874:0.0371516636392:0.341735955717008\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.17297868951796821:0.0038734044236464053:0.15141123544969604:0.1239330787920094:0.5478035918166799:'0.17297868951796821:0.0038734044236464053:0.15141123544969604:0.1239330787920094:0.5478035918166799:\'0.17297868951796821:0.0038734044236464053:0.15141123544969604:0.1239330787920094:0.5478035918166799:"0.17297868951796821:0.0038734044236464053:0.15141123544969604:0.1239330787920094:0.5478035918166799:\\\'0.17297868951796821:0.0038734044236464053:0.15141123544969604:0.1239330787920094:0.5478035918166799\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.3071458935191035:0.13511293658740064:0.06436706646403009:0.25103551846993916:0.24233858495952668:'0.3071458935191035:0.13511293658740064:0.06436706646403009:0.25103551846993916:0.24233858495952668:\'0.3071458935191035:0.13511293658740064:0.06436706646403009:0.25103551846993916:0.24233858495952668:"0.3071458935191035:0.13511293658740064:0.06436706646403009:0.25103551846993916:0.24233858495952668:\\\'0.3071458935191035:0.13511293658740064:0.06436706646403009:0.25103551846993916:0.24233858495952668\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.0008499840013651758:0.0010790274898496441:0.001230791211281703:0.00043322934840114803:0.9964069679491023:'0.0008499840013651758:0.0010790274898496441:0.001230791211281703:0.00043322934840114803:0.9964069679491023:\'0.0008499840013651758:0.0010790274898496441:0.001230791211281703:0.00043322934840114803:0.9964069679491023:"0.0008499840013651758:0.0010790274898496441:0.001230791211281703:0.00043322934840114803:0.9964069679491023:\\\'0.0008499840013651758:0.0010790274898496441:0.001230791211281703:0.00043322934840114803:0.9964069679491023\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.074537560053405:0.23377596013418603:0.21868577765632807:0.21491927561621915:0.2580814265398616:'0.074537560053405:0.23377596013418603:0.21868577765632807:0.21491927561621915:0.2580814265398616:\'0.074537560053405:0.23377596013418603:0.21868577765632807:0.21491927561621915:0.2580814265398616:"0.074537560053405:0.23377596013418603:0.21868577765632807:0.21491927561621915:0.2580814265398616:\\\'0.074537560053405:0.23377596013418603:0.21868577765632807:0.21491927561621915:0.2580814265398616\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.0038831449836855747:0.2570750647234156:0.34538605480971696:0.21926666159432445:0.17438907388885735:'0.0038831449836855747:0.2570750647234156:0.34538605480971696:0.21926666159432445:0.17438907388885735:\'0.0038831449836855747:0.2570750647234156:0.34538605480971696:0.21926666159432445:0.17438907388885735:"0.0038831449836855747:0.2570750647234156:0.34538605480971696:0.21926666159432445:0.17438907388885735:\\\'0.0038831449836855747:0.2570750647234156:0.34538605480971696:0.21926666159432445:0.17438907388885735\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.10000252830735035:0.05411212378682602:0.040184273334564105:0.040011537136720614:0.7656895374345389:'0.10000252830735035:0.05411212378682602:0.040184273334564105:0.040011537136720614:0.7656895374345389:\'0.10000252830735035:0.05411212378682602:0.040184273334564105:0.040011537136720614:0.7656895374345389:"0.10000252830735035:0.05411212378682602:0.040184273334564105:0.040011537136720614:0.7656895374345389:\\\'0.10000252830735035:0.05411212378682602:0.040184273334564105:0.040011537136720614:0.7656895374345389\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.05009674706362561:0.08270077476439788:0.0405067293390163:0.08045255983596511:0.7462431889969952:'0.05009674706362561:0.08270077476439788:0.0405067293390163:0.08045255983596511:0.7462431889969952:\'0.05009674706362561:0.08270077476439788:0.0405067293390163:0.08045255983596511:0.7462431889969952:"0.05009674706362561:0.08270077476439788:0.0405067293390163:0.08045255983596511:0.7462431889969952:\\\'0.05009674706362561:0.08270077476439788:0.0405067293390163:0.08045255983596511:0.7462431889969952\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.043478271812166396:0.04165595053028977:0.06006448699021291:0.038298636775646516:0.8165026538916844:'0.043478271812166396:0.04165595053028977:0.06006448699021291:0.038298636775646516:0.8165026538916844:\'0.043478271812166396:0.04165595053028977:0.06006448699021291:0.038298636775646516:0.8165026538916844:"0.043478271812166396:0.04165595053028977:0.06006448699021291:0.038298636775646516:0.8165026538916844:\\\'0.043478271812166396:0.04165595053028977:0.06006448699021291:0.038298636775646516:0.8165026538916844\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.14037800101418405:0.3252409319849474:0.19884286680342372:0.2868468330849948:0.048691367112449924:'0.14037800101418405:0.3252409319849474:0.19884286680342372:0.2868468330849948:0.048691367112449924:\'0.14037800101418405:0.3252409319849474:0.19884286680342372:0.2868468330849948:0.048691367112449924:"0.14037800101418405:0.3252409319849474:0.19884286680342372:0.2868468330849948:0.048691367112449924:\\\'0.14037800101418405:0.3252409319849474:0.19884286680342372:0.2868468330849948:0.048691367112449924\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.267275179454366:0.04723230298522335:0.24410864883377942:0.024494377196729145:0.41688949152990207:'0.267275179454366:0.04723230298522335:0.24410864883377942:0.024494377196729145:0.41688949152990207:\'0.267275179454366:0.04723230298522335:0.24410864883377942:0.024494377196729145:0.41688949152990207:"0.267275179454366:0.04723230298522335:0.24410864883377942:0.024494377196729145:0.41688949152990207:\\\'0.267275179454366:0.04723230298522335:0.24410864883377942:0.024494377196729145:0.41688949152990207\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.012580916913995415:0.013647930365035737:0.012313135409237473:0.011776021160717033:0.9496819961510143:'0.012580916913995415:0.013647930365035737:0.012313135409237473:0.011776021160717033:0.9496819961510143:\'0.012580916913995415:0.013647930365035737:0.012313135409237473:0.011776021160717033:0.9496819961510143:"0.012580916913995415:0.013647930365035737:0.012313135409237473:0.011776021160717033:0.9496819961510143:\\\'0.012580916913995415:0.013647930365035737:0.012313135409237473:0.011776021160717033:0.9496819961510143\\\'"\''</t>
-  </si>
-  <si>
-    <t>0.1797578576761459:0.08087059903348022:0.09418509128847868:0.5737293034264526:0.07145714857544264:'0.1797578576761459:0.08087059903348022:0.09418509128847868:0.5737293034264526:0.07145714857544264:\'0.1797578576761459:0.08087059903348022:0.09418509128847868:0.5737293034264526:0.07145714857544264:"0.1797578576761459:0.08087059903348022:0.09418509128847868:0.5737293034264526:0.07145714857544264:\\\'0.1797578576761459:0.08087059903348022:0.09418509128847868:0.5737293034264526:0.07145714857544264\\\'"\''</t>
   </si>
   <si>
     <t>ngB</t>
@@ -8316,304 +7116,304 @@
   <sheetData>
     <row r="1" spans="1:101">
       <c r="B1" s="1" t="s">
-        <v>104</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>106</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>107</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>108</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>109</v>
+        <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>110</v>
+        <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>111</v>
+        <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>112</v>
+        <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>113</v>
+        <v>9</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>114</v>
+        <v>10</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>115</v>
+        <v>11</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>116</v>
+        <v>12</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>117</v>
+        <v>13</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>118</v>
+        <v>14</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>119</v>
+        <v>15</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>120</v>
+        <v>16</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>121</v>
+        <v>17</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>122</v>
+        <v>18</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>123</v>
+        <v>19</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>124</v>
+        <v>20</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>125</v>
+        <v>21</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>126</v>
+        <v>22</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>127</v>
+        <v>23</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>128</v>
+        <v>24</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>129</v>
+        <v>25</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>130</v>
+        <v>26</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>131</v>
+        <v>27</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>132</v>
+        <v>28</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>133</v>
+        <v>29</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>134</v>
+        <v>30</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>135</v>
+        <v>31</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>136</v>
+        <v>32</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>137</v>
+        <v>33</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>138</v>
+        <v>34</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>139</v>
+        <v>35</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>140</v>
+        <v>36</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>141</v>
+        <v>37</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>142</v>
+        <v>38</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>143</v>
+        <v>39</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>144</v>
+        <v>40</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>145</v>
+        <v>41</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>146</v>
+        <v>42</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>147</v>
+        <v>43</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>148</v>
+        <v>44</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>149</v>
+        <v>45</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>150</v>
+        <v>46</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>151</v>
+        <v>47</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>152</v>
+        <v>48</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>153</v>
+        <v>49</v>
       </c>
       <c r="AZ1" s="1" t="s">
-        <v>154</v>
+        <v>50</v>
       </c>
       <c r="BA1" s="1" t="s">
-        <v>155</v>
+        <v>51</v>
       </c>
       <c r="BB1" s="1" t="s">
-        <v>156</v>
+        <v>52</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>157</v>
+        <v>53</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>158</v>
+        <v>54</v>
       </c>
       <c r="BE1" s="1" t="s">
-        <v>159</v>
+        <v>55</v>
       </c>
       <c r="BF1" s="1" t="s">
-        <v>160</v>
+        <v>56</v>
       </c>
       <c r="BG1" s="1" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="BH1" s="1" t="s">
-        <v>162</v>
+        <v>58</v>
       </c>
       <c r="BI1" s="1" t="s">
-        <v>163</v>
+        <v>59</v>
       </c>
       <c r="BJ1" s="1" t="s">
-        <v>164</v>
+        <v>60</v>
       </c>
       <c r="BK1" s="1" t="s">
-        <v>165</v>
+        <v>61</v>
       </c>
       <c r="BL1" s="1" t="s">
-        <v>166</v>
+        <v>62</v>
       </c>
       <c r="BM1" s="1" t="s">
-        <v>167</v>
+        <v>63</v>
       </c>
       <c r="BN1" s="1" t="s">
-        <v>168</v>
+        <v>64</v>
       </c>
       <c r="BO1" s="1" t="s">
-        <v>169</v>
+        <v>65</v>
       </c>
       <c r="BP1" s="1" t="s">
-        <v>170</v>
+        <v>66</v>
       </c>
       <c r="BQ1" s="1" t="s">
-        <v>171</v>
+        <v>67</v>
       </c>
       <c r="BR1" s="1" t="s">
-        <v>172</v>
+        <v>68</v>
       </c>
       <c r="BS1" s="1" t="s">
-        <v>173</v>
+        <v>69</v>
       </c>
       <c r="BT1" s="1" t="s">
-        <v>174</v>
+        <v>70</v>
       </c>
       <c r="BU1" s="1" t="s">
-        <v>175</v>
+        <v>71</v>
       </c>
       <c r="BV1" s="1" t="s">
-        <v>176</v>
+        <v>72</v>
       </c>
       <c r="BW1" s="1" t="s">
-        <v>177</v>
+        <v>73</v>
       </c>
       <c r="BX1" s="1" t="s">
-        <v>178</v>
+        <v>74</v>
       </c>
       <c r="BY1" s="1" t="s">
-        <v>179</v>
+        <v>75</v>
       </c>
       <c r="BZ1" s="1" t="s">
-        <v>180</v>
+        <v>76</v>
       </c>
       <c r="CA1" s="1" t="s">
-        <v>181</v>
+        <v>77</v>
       </c>
       <c r="CB1" s="1" t="s">
-        <v>182</v>
+        <v>78</v>
       </c>
       <c r="CC1" s="1" t="s">
-        <v>183</v>
+        <v>79</v>
       </c>
       <c r="CD1" s="1" t="s">
-        <v>184</v>
+        <v>80</v>
       </c>
       <c r="CE1" s="1" t="s">
-        <v>185</v>
+        <v>81</v>
       </c>
       <c r="CF1" s="1" t="s">
-        <v>186</v>
+        <v>82</v>
       </c>
       <c r="CG1" s="1" t="s">
-        <v>187</v>
+        <v>83</v>
       </c>
       <c r="CH1" s="1" t="s">
-        <v>188</v>
+        <v>84</v>
       </c>
       <c r="CI1" s="1" t="s">
-        <v>189</v>
+        <v>85</v>
       </c>
       <c r="CJ1" s="1" t="s">
-        <v>190</v>
+        <v>86</v>
       </c>
       <c r="CK1" s="1" t="s">
-        <v>191</v>
+        <v>87</v>
       </c>
       <c r="CL1" s="1" t="s">
-        <v>192</v>
+        <v>88</v>
       </c>
       <c r="CM1" s="1" t="s">
-        <v>193</v>
+        <v>89</v>
       </c>
       <c r="CN1" s="1" t="s">
-        <v>194</v>
+        <v>90</v>
       </c>
       <c r="CO1" s="1" t="s">
-        <v>195</v>
+        <v>91</v>
       </c>
       <c r="CP1" s="1" t="s">
-        <v>196</v>
+        <v>92</v>
       </c>
       <c r="CQ1" s="1" t="s">
-        <v>197</v>
+        <v>93</v>
       </c>
       <c r="CR1" s="1" t="s">
-        <v>198</v>
+        <v>94</v>
       </c>
       <c r="CS1" s="1" t="s">
-        <v>199</v>
+        <v>95</v>
       </c>
       <c r="CT1" s="1" t="s">
-        <v>200</v>
+        <v>96</v>
       </c>
       <c r="CU1" s="1" t="s">
-        <v>201</v>
+        <v>97</v>
       </c>
       <c r="CV1" s="1" t="s">
-        <v>202</v>
+        <v>98</v>
       </c>
       <c r="CW1" s="1" t="s">
-        <v>203</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:101">
@@ -8651,7 +7451,7 @@
         <v>102</v>
       </c>
       <c r="L2" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="M2" t="s">
         <v>102</v>
@@ -8675,7 +7475,7 @@
         <v>102</v>
       </c>
       <c r="T2" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="U2" t="s">
         <v>100</v>
@@ -8956,7 +7756,7 @@
         <v>102</v>
       </c>
       <c r="L3" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="M3" t="s">
         <v>100</v>
@@ -8980,7 +7780,7 @@
         <v>102</v>
       </c>
       <c r="T3" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="U3" t="s">
         <v>100</v>
@@ -9261,7 +8061,7 @@
         <v>102</v>
       </c>
       <c r="L4" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="M4" t="s">
         <v>102</v>
@@ -9285,7 +8085,7 @@
         <v>102</v>
       </c>
       <c r="T4" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="U4" t="s">
         <v>100</v>
@@ -9566,7 +8366,7 @@
         <v>102</v>
       </c>
       <c r="L5" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="M5" t="s">
         <v>100</v>
@@ -9590,7 +8390,7 @@
         <v>102</v>
       </c>
       <c r="T5" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="U5" t="s">
         <v>100</v>
@@ -9871,7 +8671,7 @@
         <v>102</v>
       </c>
       <c r="L6" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="M6" t="s">
         <v>102</v>
@@ -9895,7 +8695,7 @@
         <v>102</v>
       </c>
       <c r="T6" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="U6" t="s">
         <v>102</v>
@@ -10176,7 +8976,7 @@
         <v>102</v>
       </c>
       <c r="L7" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="M7" t="s">
         <v>102</v>
@@ -10200,7 +9000,7 @@
         <v>102</v>
       </c>
       <c r="T7" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="U7" t="s">
         <v>100</v>
@@ -10481,7 +9281,7 @@
         <v>102</v>
       </c>
       <c r="L8" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="M8" t="s">
         <v>100</v>
@@ -10505,7 +9305,7 @@
         <v>102</v>
       </c>
       <c r="T8" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="U8" t="s">
         <v>100</v>
@@ -10786,7 +9586,7 @@
         <v>102</v>
       </c>
       <c r="L9" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="M9" t="s">
         <v>100</v>
@@ -10810,7 +9610,7 @@
         <v>102</v>
       </c>
       <c r="T9" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="U9" t="s">
         <v>100</v>
@@ -11091,7 +9891,7 @@
         <v>102</v>
       </c>
       <c r="L10" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="M10" t="s">
         <v>101</v>
@@ -11115,7 +9915,7 @@
         <v>102</v>
       </c>
       <c r="T10" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="U10" t="s">
         <v>101</v>
@@ -11396,7 +10196,7 @@
         <v>102</v>
       </c>
       <c r="L11" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="M11" t="s">
         <v>101</v>
@@ -11420,7 +10220,7 @@
         <v>102</v>
       </c>
       <c r="T11" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="U11" t="s">
         <v>100</v>
@@ -11701,7 +10501,7 @@
         <v>102</v>
       </c>
       <c r="L12" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="M12" t="s">
         <v>100</v>
@@ -11725,7 +10525,7 @@
         <v>102</v>
       </c>
       <c r="T12" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="U12" t="s">
         <v>100</v>
@@ -12006,7 +10806,7 @@
         <v>102</v>
       </c>
       <c r="L13" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="M13" t="s">
         <v>100</v>
@@ -12030,7 +10830,7 @@
         <v>102</v>
       </c>
       <c r="T13" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="U13" t="s">
         <v>100</v>
@@ -12311,7 +11111,7 @@
         <v>102</v>
       </c>
       <c r="L14" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="M14" t="s">
         <v>102</v>
@@ -12335,7 +11135,7 @@
         <v>102</v>
       </c>
       <c r="T14" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="U14" t="s">
         <v>102</v>
@@ -12616,7 +11416,7 @@
         <v>102</v>
       </c>
       <c r="L15" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="M15" t="s">
         <v>102</v>
@@ -12640,7 +11440,7 @@
         <v>102</v>
       </c>
       <c r="T15" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="U15" t="s">
         <v>100</v>
@@ -12921,7 +11721,7 @@
         <v>102</v>
       </c>
       <c r="L16" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="M16" t="s">
         <v>100</v>
@@ -12945,7 +11745,7 @@
         <v>102</v>
       </c>
       <c r="T16" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="U16" t="s">
         <v>100</v>
@@ -13226,7 +12026,7 @@
         <v>102</v>
       </c>
       <c r="L17" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="M17" t="s">
         <v>102</v>
@@ -13250,7 +12050,7 @@
         <v>102</v>
       </c>
       <c r="T17" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="U17" t="s">
         <v>100</v>
@@ -13531,7 +12331,7 @@
         <v>102</v>
       </c>
       <c r="L18" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="M18" t="s">
         <v>101</v>
@@ -13555,7 +12355,7 @@
         <v>102</v>
       </c>
       <c r="T18" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="U18" t="s">
         <v>101</v>
@@ -13836,7 +12636,7 @@
         <v>102</v>
       </c>
       <c r="L19" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="M19" t="s">
         <v>102</v>
@@ -13860,7 +12660,7 @@
         <v>102</v>
       </c>
       <c r="T19" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="U19" t="s">
         <v>100</v>
@@ -14141,7 +12941,7 @@
         <v>102</v>
       </c>
       <c r="L20" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="M20" t="s">
         <v>101</v>
@@ -14165,7 +12965,7 @@
         <v>102</v>
       </c>
       <c r="T20" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="U20" t="s">
         <v>101</v>
@@ -14446,7 +13246,7 @@
         <v>102</v>
       </c>
       <c r="L21" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="M21" t="s">
         <v>102</v>
@@ -14470,7 +13270,7 @@
         <v>102</v>
       </c>
       <c r="T21" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="U21" t="s">
         <v>100</v>
@@ -14731,304 +13531,304 @@
   <sheetData>
     <row r="1" spans="1:101">
       <c r="B1" s="1" t="s">
-        <v>205</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>206</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>207</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>208</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>209</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>210</v>
+        <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>211</v>
+        <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>212</v>
+        <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>213</v>
+        <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>214</v>
+        <v>9</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>215</v>
+        <v>10</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>216</v>
+        <v>11</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>217</v>
+        <v>12</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>218</v>
+        <v>13</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>219</v>
+        <v>14</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>220</v>
+        <v>15</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>221</v>
+        <v>16</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>222</v>
+        <v>17</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>223</v>
+        <v>18</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>224</v>
+        <v>19</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>225</v>
+        <v>20</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>226</v>
+        <v>21</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>227</v>
+        <v>22</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>228</v>
+        <v>23</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>229</v>
+        <v>24</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>230</v>
+        <v>25</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>231</v>
+        <v>26</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>232</v>
+        <v>27</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>233</v>
+        <v>28</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>234</v>
+        <v>29</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>235</v>
+        <v>30</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>236</v>
+        <v>31</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>237</v>
+        <v>32</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>238</v>
+        <v>33</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>239</v>
+        <v>34</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>240</v>
+        <v>35</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>241</v>
+        <v>36</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>242</v>
+        <v>37</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>243</v>
+        <v>38</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>244</v>
+        <v>39</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>245</v>
+        <v>40</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>246</v>
+        <v>41</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>247</v>
+        <v>42</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>248</v>
+        <v>43</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>249</v>
+        <v>44</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>250</v>
+        <v>45</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>251</v>
+        <v>46</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>252</v>
+        <v>47</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>253</v>
+        <v>48</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>254</v>
+        <v>49</v>
       </c>
       <c r="AZ1" s="1" t="s">
-        <v>255</v>
+        <v>50</v>
       </c>
       <c r="BA1" s="1" t="s">
-        <v>256</v>
+        <v>51</v>
       </c>
       <c r="BB1" s="1" t="s">
-        <v>257</v>
+        <v>52</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>258</v>
+        <v>53</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>259</v>
+        <v>54</v>
       </c>
       <c r="BE1" s="1" t="s">
-        <v>260</v>
+        <v>55</v>
       </c>
       <c r="BF1" s="1" t="s">
-        <v>261</v>
+        <v>56</v>
       </c>
       <c r="BG1" s="1" t="s">
-        <v>262</v>
+        <v>57</v>
       </c>
       <c r="BH1" s="1" t="s">
-        <v>263</v>
+        <v>58</v>
       </c>
       <c r="BI1" s="1" t="s">
-        <v>264</v>
+        <v>59</v>
       </c>
       <c r="BJ1" s="1" t="s">
-        <v>265</v>
+        <v>60</v>
       </c>
       <c r="BK1" s="1" t="s">
-        <v>266</v>
+        <v>61</v>
       </c>
       <c r="BL1" s="1" t="s">
-        <v>267</v>
+        <v>62</v>
       </c>
       <c r="BM1" s="1" t="s">
-        <v>268</v>
+        <v>63</v>
       </c>
       <c r="BN1" s="1" t="s">
-        <v>269</v>
+        <v>64</v>
       </c>
       <c r="BO1" s="1" t="s">
-        <v>270</v>
+        <v>65</v>
       </c>
       <c r="BP1" s="1" t="s">
-        <v>271</v>
+        <v>66</v>
       </c>
       <c r="BQ1" s="1" t="s">
-        <v>272</v>
+        <v>67</v>
       </c>
       <c r="BR1" s="1" t="s">
-        <v>273</v>
+        <v>68</v>
       </c>
       <c r="BS1" s="1" t="s">
-        <v>274</v>
+        <v>69</v>
       </c>
       <c r="BT1" s="1" t="s">
-        <v>275</v>
+        <v>70</v>
       </c>
       <c r="BU1" s="1" t="s">
-        <v>276</v>
+        <v>71</v>
       </c>
       <c r="BV1" s="1" t="s">
-        <v>277</v>
+        <v>72</v>
       </c>
       <c r="BW1" s="1" t="s">
-        <v>278</v>
+        <v>73</v>
       </c>
       <c r="BX1" s="1" t="s">
-        <v>279</v>
+        <v>74</v>
       </c>
       <c r="BY1" s="1" t="s">
-        <v>280</v>
+        <v>75</v>
       </c>
       <c r="BZ1" s="1" t="s">
-        <v>281</v>
+        <v>76</v>
       </c>
       <c r="CA1" s="1" t="s">
-        <v>282</v>
+        <v>77</v>
       </c>
       <c r="CB1" s="1" t="s">
-        <v>283</v>
+        <v>78</v>
       </c>
       <c r="CC1" s="1" t="s">
-        <v>284</v>
+        <v>79</v>
       </c>
       <c r="CD1" s="1" t="s">
-        <v>285</v>
+        <v>80</v>
       </c>
       <c r="CE1" s="1" t="s">
-        <v>286</v>
+        <v>81</v>
       </c>
       <c r="CF1" s="1" t="s">
-        <v>287</v>
+        <v>82</v>
       </c>
       <c r="CG1" s="1" t="s">
-        <v>288</v>
+        <v>83</v>
       </c>
       <c r="CH1" s="1" t="s">
-        <v>289</v>
+        <v>84</v>
       </c>
       <c r="CI1" s="1" t="s">
-        <v>290</v>
+        <v>85</v>
       </c>
       <c r="CJ1" s="1" t="s">
-        <v>291</v>
+        <v>86</v>
       </c>
       <c r="CK1" s="1" t="s">
-        <v>292</v>
+        <v>87</v>
       </c>
       <c r="CL1" s="1" t="s">
-        <v>293</v>
+        <v>88</v>
       </c>
       <c r="CM1" s="1" t="s">
-        <v>294</v>
+        <v>89</v>
       </c>
       <c r="CN1" s="1" t="s">
-        <v>295</v>
+        <v>90</v>
       </c>
       <c r="CO1" s="1" t="s">
-        <v>296</v>
+        <v>91</v>
       </c>
       <c r="CP1" s="1" t="s">
-        <v>297</v>
+        <v>92</v>
       </c>
       <c r="CQ1" s="1" t="s">
-        <v>298</v>
+        <v>93</v>
       </c>
       <c r="CR1" s="1" t="s">
-        <v>299</v>
+        <v>94</v>
       </c>
       <c r="CS1" s="1" t="s">
-        <v>300</v>
+        <v>95</v>
       </c>
       <c r="CT1" s="1" t="s">
-        <v>301</v>
+        <v>96</v>
       </c>
       <c r="CU1" s="1" t="s">
-        <v>302</v>
+        <v>97</v>
       </c>
       <c r="CV1" s="1" t="s">
-        <v>303</v>
+        <v>98</v>
       </c>
       <c r="CW1" s="1" t="s">
-        <v>304</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:101">
@@ -21146,304 +19946,304 @@
   <sheetData>
     <row r="1" spans="1:101">
       <c r="B1" s="1" t="s">
-        <v>305</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>306</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>307</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>308</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>309</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>310</v>
+        <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>311</v>
+        <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>312</v>
+        <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>313</v>
+        <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>314</v>
+        <v>9</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>315</v>
+        <v>10</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>316</v>
+        <v>11</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>317</v>
+        <v>12</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>318</v>
+        <v>13</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>319</v>
+        <v>14</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>320</v>
+        <v>15</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>321</v>
+        <v>16</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>322</v>
+        <v>17</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>323</v>
+        <v>18</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>324</v>
+        <v>19</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>325</v>
+        <v>20</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>326</v>
+        <v>21</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>327</v>
+        <v>22</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>328</v>
+        <v>23</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>329</v>
+        <v>24</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>330</v>
+        <v>25</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>331</v>
+        <v>26</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>332</v>
+        <v>27</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>333</v>
+        <v>28</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>334</v>
+        <v>29</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>335</v>
+        <v>30</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>336</v>
+        <v>31</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>337</v>
+        <v>32</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>338</v>
+        <v>33</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>339</v>
+        <v>34</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>340</v>
+        <v>35</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>341</v>
+        <v>36</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>342</v>
+        <v>37</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>343</v>
+        <v>38</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>344</v>
+        <v>39</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>345</v>
+        <v>40</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>346</v>
+        <v>41</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>347</v>
+        <v>42</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>348</v>
+        <v>43</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>349</v>
+        <v>44</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>350</v>
+        <v>45</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>351</v>
+        <v>46</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>352</v>
+        <v>47</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>353</v>
+        <v>48</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>354</v>
+        <v>49</v>
       </c>
       <c r="AZ1" s="1" t="s">
-        <v>355</v>
+        <v>50</v>
       </c>
       <c r="BA1" s="1" t="s">
-        <v>356</v>
+        <v>51</v>
       </c>
       <c r="BB1" s="1" t="s">
-        <v>357</v>
+        <v>52</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>358</v>
+        <v>53</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>359</v>
+        <v>54</v>
       </c>
       <c r="BE1" s="1" t="s">
-        <v>360</v>
+        <v>55</v>
       </c>
       <c r="BF1" s="1" t="s">
-        <v>361</v>
+        <v>56</v>
       </c>
       <c r="BG1" s="1" t="s">
-        <v>362</v>
+        <v>57</v>
       </c>
       <c r="BH1" s="1" t="s">
-        <v>363</v>
+        <v>58</v>
       </c>
       <c r="BI1" s="1" t="s">
-        <v>364</v>
+        <v>59</v>
       </c>
       <c r="BJ1" s="1" t="s">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="BK1" s="1" t="s">
-        <v>366</v>
+        <v>61</v>
       </c>
       <c r="BL1" s="1" t="s">
-        <v>367</v>
+        <v>62</v>
       </c>
       <c r="BM1" s="1" t="s">
-        <v>368</v>
+        <v>63</v>
       </c>
       <c r="BN1" s="1" t="s">
-        <v>369</v>
+        <v>64</v>
       </c>
       <c r="BO1" s="1" t="s">
-        <v>370</v>
+        <v>65</v>
       </c>
       <c r="BP1" s="1" t="s">
-        <v>371</v>
+        <v>66</v>
       </c>
       <c r="BQ1" s="1" t="s">
-        <v>372</v>
+        <v>67</v>
       </c>
       <c r="BR1" s="1" t="s">
-        <v>373</v>
+        <v>68</v>
       </c>
       <c r="BS1" s="1" t="s">
-        <v>374</v>
+        <v>69</v>
       </c>
       <c r="BT1" s="1" t="s">
-        <v>375</v>
+        <v>70</v>
       </c>
       <c r="BU1" s="1" t="s">
-        <v>376</v>
+        <v>71</v>
       </c>
       <c r="BV1" s="1" t="s">
-        <v>377</v>
+        <v>72</v>
       </c>
       <c r="BW1" s="1" t="s">
-        <v>378</v>
+        <v>73</v>
       </c>
       <c r="BX1" s="1" t="s">
-        <v>379</v>
+        <v>74</v>
       </c>
       <c r="BY1" s="1" t="s">
-        <v>380</v>
+        <v>75</v>
       </c>
       <c r="BZ1" s="1" t="s">
-        <v>381</v>
+        <v>76</v>
       </c>
       <c r="CA1" s="1" t="s">
-        <v>382</v>
+        <v>77</v>
       </c>
       <c r="CB1" s="1" t="s">
-        <v>383</v>
+        <v>78</v>
       </c>
       <c r="CC1" s="1" t="s">
-        <v>384</v>
+        <v>79</v>
       </c>
       <c r="CD1" s="1" t="s">
-        <v>385</v>
+        <v>80</v>
       </c>
       <c r="CE1" s="1" t="s">
-        <v>386</v>
+        <v>81</v>
       </c>
       <c r="CF1" s="1" t="s">
-        <v>387</v>
+        <v>82</v>
       </c>
       <c r="CG1" s="1" t="s">
-        <v>388</v>
+        <v>83</v>
       </c>
       <c r="CH1" s="1" t="s">
-        <v>389</v>
+        <v>84</v>
       </c>
       <c r="CI1" s="1" t="s">
-        <v>390</v>
+        <v>85</v>
       </c>
       <c r="CJ1" s="1" t="s">
-        <v>391</v>
+        <v>86</v>
       </c>
       <c r="CK1" s="1" t="s">
-        <v>392</v>
+        <v>87</v>
       </c>
       <c r="CL1" s="1" t="s">
-        <v>393</v>
+        <v>88</v>
       </c>
       <c r="CM1" s="1" t="s">
-        <v>394</v>
+        <v>89</v>
       </c>
       <c r="CN1" s="1" t="s">
-        <v>395</v>
+        <v>90</v>
       </c>
       <c r="CO1" s="1" t="s">
-        <v>396</v>
+        <v>91</v>
       </c>
       <c r="CP1" s="1" t="s">
-        <v>397</v>
+        <v>92</v>
       </c>
       <c r="CQ1" s="1" t="s">
-        <v>398</v>
+        <v>93</v>
       </c>
       <c r="CR1" s="1" t="s">
-        <v>399</v>
+        <v>94</v>
       </c>
       <c r="CS1" s="1" t="s">
-        <v>400</v>
+        <v>95</v>
       </c>
       <c r="CT1" s="1" t="s">
-        <v>401</v>
+        <v>96</v>
       </c>
       <c r="CU1" s="1" t="s">
-        <v>402</v>
+        <v>97</v>
       </c>
       <c r="CV1" s="1" t="s">
-        <v>403</v>
+        <v>98</v>
       </c>
       <c r="CW1" s="1" t="s">
-        <v>404</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:101">
@@ -27561,304 +26361,304 @@
   <sheetData>
     <row r="1" spans="1:101">
       <c r="B1" s="1" t="s">
-        <v>405</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>406</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>407</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>408</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>409</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>410</v>
+        <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>411</v>
+        <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>412</v>
+        <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>413</v>
+        <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>414</v>
+        <v>9</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>415</v>
+        <v>10</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>416</v>
+        <v>11</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>417</v>
+        <v>12</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>418</v>
+        <v>13</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>419</v>
+        <v>14</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>420</v>
+        <v>15</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>421</v>
+        <v>16</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>422</v>
+        <v>17</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>423</v>
+        <v>18</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>424</v>
+        <v>19</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>425</v>
+        <v>20</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>426</v>
+        <v>21</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>427</v>
+        <v>22</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>428</v>
+        <v>23</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>429</v>
+        <v>24</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>430</v>
+        <v>25</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>431</v>
+        <v>26</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>432</v>
+        <v>27</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>433</v>
+        <v>28</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>434</v>
+        <v>29</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>435</v>
+        <v>30</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>436</v>
+        <v>31</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>437</v>
+        <v>32</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>438</v>
+        <v>33</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>439</v>
+        <v>34</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>440</v>
+        <v>35</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>441</v>
+        <v>36</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>442</v>
+        <v>37</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>443</v>
+        <v>38</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>444</v>
+        <v>39</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>445</v>
+        <v>40</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>446</v>
+        <v>41</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>447</v>
+        <v>42</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>448</v>
+        <v>43</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>449</v>
+        <v>44</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>450</v>
+        <v>45</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>451</v>
+        <v>46</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>452</v>
+        <v>47</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>453</v>
+        <v>48</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>454</v>
+        <v>49</v>
       </c>
       <c r="AZ1" s="1" t="s">
-        <v>455</v>
+        <v>50</v>
       </c>
       <c r="BA1" s="1" t="s">
-        <v>456</v>
+        <v>51</v>
       </c>
       <c r="BB1" s="1" t="s">
-        <v>457</v>
+        <v>52</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>458</v>
+        <v>53</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>459</v>
+        <v>54</v>
       </c>
       <c r="BE1" s="1" t="s">
-        <v>460</v>
+        <v>55</v>
       </c>
       <c r="BF1" s="1" t="s">
-        <v>461</v>
+        <v>56</v>
       </c>
       <c r="BG1" s="1" t="s">
-        <v>462</v>
+        <v>57</v>
       </c>
       <c r="BH1" s="1" t="s">
-        <v>463</v>
+        <v>58</v>
       </c>
       <c r="BI1" s="1" t="s">
-        <v>464</v>
+        <v>59</v>
       </c>
       <c r="BJ1" s="1" t="s">
-        <v>465</v>
+        <v>60</v>
       </c>
       <c r="BK1" s="1" t="s">
-        <v>466</v>
+        <v>61</v>
       </c>
       <c r="BL1" s="1" t="s">
-        <v>467</v>
+        <v>62</v>
       </c>
       <c r="BM1" s="1" t="s">
-        <v>468</v>
+        <v>63</v>
       </c>
       <c r="BN1" s="1" t="s">
-        <v>469</v>
+        <v>64</v>
       </c>
       <c r="BO1" s="1" t="s">
-        <v>470</v>
+        <v>65</v>
       </c>
       <c r="BP1" s="1" t="s">
-        <v>471</v>
+        <v>66</v>
       </c>
       <c r="BQ1" s="1" t="s">
-        <v>472</v>
+        <v>67</v>
       </c>
       <c r="BR1" s="1" t="s">
-        <v>473</v>
+        <v>68</v>
       </c>
       <c r="BS1" s="1" t="s">
-        <v>474</v>
+        <v>69</v>
       </c>
       <c r="BT1" s="1" t="s">
-        <v>475</v>
+        <v>70</v>
       </c>
       <c r="BU1" s="1" t="s">
-        <v>476</v>
+        <v>71</v>
       </c>
       <c r="BV1" s="1" t="s">
-        <v>477</v>
+        <v>72</v>
       </c>
       <c r="BW1" s="1" t="s">
-        <v>478</v>
+        <v>73</v>
       </c>
       <c r="BX1" s="1" t="s">
-        <v>479</v>
+        <v>74</v>
       </c>
       <c r="BY1" s="1" t="s">
-        <v>480</v>
+        <v>75</v>
       </c>
       <c r="BZ1" s="1" t="s">
-        <v>481</v>
+        <v>76</v>
       </c>
       <c r="CA1" s="1" t="s">
-        <v>482</v>
+        <v>77</v>
       </c>
       <c r="CB1" s="1" t="s">
-        <v>483</v>
+        <v>78</v>
       </c>
       <c r="CC1" s="1" t="s">
-        <v>484</v>
+        <v>79</v>
       </c>
       <c r="CD1" s="1" t="s">
-        <v>485</v>
+        <v>80</v>
       </c>
       <c r="CE1" s="1" t="s">
-        <v>486</v>
+        <v>81</v>
       </c>
       <c r="CF1" s="1" t="s">
-        <v>487</v>
+        <v>82</v>
       </c>
       <c r="CG1" s="1" t="s">
-        <v>488</v>
+        <v>83</v>
       </c>
       <c r="CH1" s="1" t="s">
-        <v>489</v>
+        <v>84</v>
       </c>
       <c r="CI1" s="1" t="s">
-        <v>490</v>
+        <v>85</v>
       </c>
       <c r="CJ1" s="1" t="s">
-        <v>491</v>
+        <v>86</v>
       </c>
       <c r="CK1" s="1" t="s">
-        <v>492</v>
+        <v>87</v>
       </c>
       <c r="CL1" s="1" t="s">
-        <v>493</v>
+        <v>88</v>
       </c>
       <c r="CM1" s="1" t="s">
-        <v>494</v>
+        <v>89</v>
       </c>
       <c r="CN1" s="1" t="s">
-        <v>495</v>
+        <v>90</v>
       </c>
       <c r="CO1" s="1" t="s">
-        <v>496</v>
+        <v>91</v>
       </c>
       <c r="CP1" s="1" t="s">
-        <v>497</v>
+        <v>92</v>
       </c>
       <c r="CQ1" s="1" t="s">
-        <v>498</v>
+        <v>93</v>
       </c>
       <c r="CR1" s="1" t="s">
-        <v>499</v>
+        <v>94</v>
       </c>
       <c r="CS1" s="1" t="s">
-        <v>500</v>
+        <v>95</v>
       </c>
       <c r="CT1" s="1" t="s">
-        <v>501</v>
+        <v>96</v>
       </c>
       <c r="CU1" s="1" t="s">
-        <v>502</v>
+        <v>97</v>
       </c>
       <c r="CV1" s="1" t="s">
-        <v>503</v>
+        <v>98</v>
       </c>
       <c r="CW1" s="1" t="s">
-        <v>504</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:101">
@@ -27926,7 +26726,7 @@
         <v>100</v>
       </c>
       <c r="V2" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="W2" t="s">
         <v>101</v>
@@ -27956,7 +26756,7 @@
         <v>101</v>
       </c>
       <c r="AF2" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AG2" t="s">
         <v>102</v>
@@ -27980,7 +26780,7 @@
         <v>101</v>
       </c>
       <c r="AN2" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AO2" t="s">
         <v>101</v>
@@ -28231,7 +27031,7 @@
         <v>100</v>
       </c>
       <c r="V3" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="W3" t="s">
         <v>101</v>
@@ -28261,7 +27061,7 @@
         <v>101</v>
       </c>
       <c r="AF3" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AG3" t="s">
         <v>100</v>
@@ -28276,7 +27076,7 @@
         <v>101</v>
       </c>
       <c r="AK3" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AL3" t="s">
         <v>100</v>
@@ -28285,7 +27085,7 @@
         <v>101</v>
       </c>
       <c r="AN3" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AO3" t="s">
         <v>101</v>
@@ -28536,7 +27336,7 @@
         <v>100</v>
       </c>
       <c r="V4" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="W4" t="s">
         <v>101</v>
@@ -28566,7 +27366,7 @@
         <v>102</v>
       </c>
       <c r="AF4" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AG4" t="s">
         <v>102</v>
@@ -28581,7 +27381,7 @@
         <v>101</v>
       </c>
       <c r="AK4" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AL4" t="s">
         <v>102</v>
@@ -28590,7 +27390,7 @@
         <v>101</v>
       </c>
       <c r="AN4" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AO4" t="s">
         <v>100</v>
@@ -28871,7 +27671,7 @@
         <v>100</v>
       </c>
       <c r="AF5" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AG5" t="s">
         <v>100</v>
@@ -28895,7 +27695,7 @@
         <v>101</v>
       </c>
       <c r="AN5" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AO5" t="s">
         <v>100</v>
@@ -29146,7 +27946,7 @@
         <v>101</v>
       </c>
       <c r="V6" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="W6" t="s">
         <v>101</v>
@@ -29176,7 +27976,7 @@
         <v>101</v>
       </c>
       <c r="AF6" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AG6" t="s">
         <v>100</v>
@@ -29200,7 +28000,7 @@
         <v>101</v>
       </c>
       <c r="AN6" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AO6" t="s">
         <v>101</v>
@@ -29481,7 +28281,7 @@
         <v>102</v>
       </c>
       <c r="AF7" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AG7" t="s">
         <v>102</v>
@@ -29505,7 +28305,7 @@
         <v>101</v>
       </c>
       <c r="AN7" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AO7" t="s">
         <v>100</v>
@@ -29756,7 +28556,7 @@
         <v>100</v>
       </c>
       <c r="V8" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="W8" t="s">
         <v>101</v>
@@ -29786,7 +28586,7 @@
         <v>100</v>
       </c>
       <c r="AF8" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AG8" t="s">
         <v>100</v>
@@ -29801,7 +28601,7 @@
         <v>101</v>
       </c>
       <c r="AK8" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AL8" t="s">
         <v>102</v>
@@ -29810,7 +28610,7 @@
         <v>101</v>
       </c>
       <c r="AN8" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AO8" t="s">
         <v>100</v>
@@ -30061,7 +28861,7 @@
         <v>100</v>
       </c>
       <c r="V9" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="W9" t="s">
         <v>101</v>
@@ -30091,7 +28891,7 @@
         <v>102</v>
       </c>
       <c r="AF9" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AG9" t="s">
         <v>100</v>
@@ -30106,7 +28906,7 @@
         <v>101</v>
       </c>
       <c r="AK9" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AL9" t="s">
         <v>102</v>
@@ -30115,7 +28915,7 @@
         <v>101</v>
       </c>
       <c r="AN9" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AO9" t="s">
         <v>101</v>
@@ -30396,7 +29196,7 @@
         <v>102</v>
       </c>
       <c r="AF10" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AG10" t="s">
         <v>100</v>
@@ -30420,7 +29220,7 @@
         <v>101</v>
       </c>
       <c r="AN10" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AO10" t="s">
         <v>100</v>
@@ -30671,7 +29471,7 @@
         <v>100</v>
       </c>
       <c r="V11" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="W11" t="s">
         <v>101</v>
@@ -30701,7 +29501,7 @@
         <v>102</v>
       </c>
       <c r="AF11" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AG11" t="s">
         <v>102</v>
@@ -30716,7 +29516,7 @@
         <v>101</v>
       </c>
       <c r="AK11" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AL11" t="s">
         <v>102</v>
@@ -30725,7 +29525,7 @@
         <v>101</v>
       </c>
       <c r="AN11" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AO11" t="s">
         <v>100</v>
@@ -31311,7 +30111,7 @@
         <v>100</v>
       </c>
       <c r="AF13" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AG13" t="s">
         <v>102</v>
@@ -31335,7 +30135,7 @@
         <v>101</v>
       </c>
       <c r="AN13" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AO13" t="s">
         <v>100</v>
@@ -31586,7 +30386,7 @@
         <v>100</v>
       </c>
       <c r="V14" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="W14" t="s">
         <v>101</v>
@@ -31616,7 +30416,7 @@
         <v>102</v>
       </c>
       <c r="AF14" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AG14" t="s">
         <v>100</v>
@@ -31631,7 +30431,7 @@
         <v>101</v>
       </c>
       <c r="AK14" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AL14" t="s">
         <v>102</v>
@@ -31640,7 +30440,7 @@
         <v>100</v>
       </c>
       <c r="AN14" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AO14" t="s">
         <v>100</v>
@@ -31891,7 +30691,7 @@
         <v>100</v>
       </c>
       <c r="V15" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="W15" t="s">
         <v>101</v>
@@ -31921,7 +30721,7 @@
         <v>102</v>
       </c>
       <c r="AF15" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AG15" t="s">
         <v>102</v>
@@ -31936,7 +30736,7 @@
         <v>101</v>
       </c>
       <c r="AK15" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AL15" t="s">
         <v>102</v>
@@ -31945,7 +30745,7 @@
         <v>102</v>
       </c>
       <c r="AN15" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AO15" t="s">
         <v>102</v>
@@ -32196,7 +30996,7 @@
         <v>100</v>
       </c>
       <c r="V16" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="W16" t="s">
         <v>101</v>
@@ -32226,7 +31026,7 @@
         <v>100</v>
       </c>
       <c r="AF16" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AG16" t="s">
         <v>100</v>
@@ -32241,7 +31041,7 @@
         <v>101</v>
       </c>
       <c r="AK16" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AL16" t="s">
         <v>100</v>
@@ -32250,7 +31050,7 @@
         <v>101</v>
       </c>
       <c r="AN16" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AO16" t="s">
         <v>100</v>
@@ -32501,7 +31301,7 @@
         <v>101</v>
       </c>
       <c r="V17" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="W17" t="s">
         <v>101</v>
@@ -32531,7 +31331,7 @@
         <v>101</v>
       </c>
       <c r="AF17" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AG17" t="s">
         <v>101</v>
@@ -32546,7 +31346,7 @@
         <v>101</v>
       </c>
       <c r="AK17" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AL17" t="s">
         <v>101</v>
@@ -32555,7 +31355,7 @@
         <v>101</v>
       </c>
       <c r="AN17" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AO17" t="s">
         <v>101</v>
@@ -32836,7 +31636,7 @@
         <v>101</v>
       </c>
       <c r="AF18" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AG18" t="s">
         <v>100</v>
@@ -32860,7 +31660,7 @@
         <v>101</v>
       </c>
       <c r="AN18" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AO18" t="s">
         <v>101</v>
@@ -33111,7 +31911,7 @@
         <v>101</v>
       </c>
       <c r="V19" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="W19" t="s">
         <v>101</v>
@@ -33141,7 +31941,7 @@
         <v>101</v>
       </c>
       <c r="AF19" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AG19" t="s">
         <v>100</v>
@@ -33156,7 +31956,7 @@
         <v>101</v>
       </c>
       <c r="AK19" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AL19" t="s">
         <v>100</v>
@@ -33165,7 +31965,7 @@
         <v>101</v>
       </c>
       <c r="AN19" t="s">
-        <v>505</v>
+        <v>105</v>
       </c>
       <c r="AO19" t="s">
         <v>101</v>

</xml_diff>